<commit_message>
Add new solution for LeetCode problem 3443: Maximum Manhattan Distance After K Changes, update workspace configuration, and modify last opened files list.
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>#</t>
   </si>
@@ -75,6 +75,12 @@
   </si>
   <si>
     <t>Partition Array Such That Maximum Difference Is K</t>
+  </si>
+  <si>
+    <t>Maximum Manhattan Distance After K Changes</t>
+  </si>
+  <si>
+    <t>math, string, counting</t>
   </si>
 </sst>
 </file>
@@ -1228,13 +1234,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="156" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="3"/>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="4"/>
   <cols>
     <col min="1" max="1" width="9.23076923076923" style="1"/>
     <col min="2" max="2" width="23.4326923076923" style="2" customWidth="1"/>
@@ -1363,6 +1369,35 @@
         <v>45827</v>
       </c>
     </row>
+    <row r="5" ht="51" spans="1:9">
+      <c r="A5" s="1">
+        <v>3443</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1">
+        <v>25</v>
+      </c>
+      <c r="H5" s="3">
+        <v>45828</v>
+      </c>
+      <c r="I5" s="3">
+        <v>45828</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:I4">
     <sortCondition ref="I2"/>

</xml_diff>

<commit_message>
Update workspace configuration to include new LeetCode problem 3085: Minimum Deletions to Make String K-Special, and modify last opened files list.
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="29100" windowHeight="14540"/>
+    <workbookView windowWidth="26860" windowHeight="14520"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>#</t>
   </si>
@@ -81,6 +81,12 @@
   </si>
   <si>
     <t>math, string, counting</t>
+  </si>
+  <si>
+    <t>Minimum Deletions to Make String K-Special</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#hash-table #string #greedy #sorting #counting </t>
   </si>
 </sst>
 </file>
@@ -1234,13 +1240,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="156" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="4"/>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="5"/>
   <cols>
     <col min="1" max="1" width="9.23076923076923" style="1"/>
     <col min="2" max="2" width="23.4326923076923" style="2" customWidth="1"/>
@@ -1398,6 +1404,35 @@
         <v>45828</v>
       </c>
     </row>
+    <row r="6" ht="51" spans="1:9">
+      <c r="A6" s="1">
+        <v>3085</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1">
+        <v>25</v>
+      </c>
+      <c r="H6" s="3">
+        <v>45829</v>
+      </c>
+      <c r="I6" s="3">
+        <v>45829</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:I4">
     <sortCondition ref="I2"/>

</xml_diff>

<commit_message>
Add hotkeys configuration for editor and update workspace to reflect new markdown file for LeetCode problem 2081: Sum of k-Mirror Numbers, including recent changes to last opened files.
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="26860" windowHeight="14520"/>
+    <workbookView windowWidth="26860" windowHeight="14540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>#</t>
   </si>
@@ -87,6 +87,15 @@
   </si>
   <si>
     <t xml:space="preserve">#hash-table #string #greedy #sorting #counting </t>
+  </si>
+  <si>
+    <t>Sum of k-Mirror Numbers</t>
+  </si>
+  <si>
+    <t>#math #enumeration</t>
+  </si>
+  <si>
+    <t>hard</t>
   </si>
 </sst>
 </file>
@@ -1240,13 +1249,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="156" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="5"/>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="6"/>
   <cols>
     <col min="1" max="1" width="9.23076923076923" style="1"/>
     <col min="2" max="2" width="23.4326923076923" style="2" customWidth="1"/>
@@ -1433,6 +1442,35 @@
         <v>45829</v>
       </c>
     </row>
+    <row r="7" ht="34" spans="1:9">
+      <c r="A7" s="1">
+        <v>2081</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1">
+        <v>40</v>
+      </c>
+      <c r="H7" s="3">
+        <v>45831</v>
+      </c>
+      <c r="I7" s="3">
+        <v>45831</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:I4">
     <sortCondition ref="I2"/>

</xml_diff>

<commit_message>
Refactor binary search implementation in 704.binary-search.py: rename variables for clarity and add new markdown file for problem description and examples.
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t>#</t>
   </si>
@@ -92,10 +92,16 @@
     <t>Sum of k-Mirror Numbers</t>
   </si>
   <si>
-    <t>#math #enumeration</t>
+    <t>#math #enumeration #binary-search</t>
   </si>
   <si>
     <t>hard</t>
+  </si>
+  <si>
+    <t>Binary Search</t>
+  </si>
+  <si>
+    <t>#binary-search</t>
   </si>
 </sst>
 </file>
@@ -1249,13 +1255,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="156" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="156" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="6"/>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="7"/>
   <cols>
     <col min="1" max="1" width="9.23076923076923" style="1"/>
     <col min="2" max="2" width="23.4326923076923" style="2" customWidth="1"/>
@@ -1263,7 +1269,7 @@
     <col min="4" max="4" width="9.23076923076923" style="1"/>
     <col min="5" max="5" width="11.0288461538462" style="1" customWidth="1"/>
     <col min="6" max="7" width="9.23076923076923" style="1"/>
-    <col min="8" max="8" width="10.9230769230769" style="1"/>
+    <col min="8" max="8" width="12.0769230769231" style="1"/>
     <col min="9" max="9" width="14.0576923076923" style="1" customWidth="1"/>
     <col min="10" max="16384" width="9.23076923076923" style="1"/>
   </cols>
@@ -1442,7 +1448,7 @@
         <v>45829</v>
       </c>
     </row>
-    <row r="7" ht="34" spans="1:9">
+    <row r="7" ht="51" spans="1:9">
       <c r="A7" s="1">
         <v>2081</v>
       </c>
@@ -1468,6 +1474,35 @@
         <v>45831</v>
       </c>
       <c r="I7" s="3">
+        <v>45831</v>
+      </c>
+    </row>
+    <row r="8" ht="17" spans="1:9">
+      <c r="A8" s="1">
+        <v>704</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="1">
+        <v>5</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1">
+        <v>10</v>
+      </c>
+      <c r="H8" s="3">
+        <v>44339</v>
+      </c>
+      <c r="I8" s="3">
         <v>45831</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update workspace configuration to include new markdown file for LeetCode problem 34: Find First and Last Position of Element in Sorted Array, and adjust last opened files list accordingly.
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>#</t>
   </si>
@@ -101,7 +101,13 @@
     <t>Binary Search</t>
   </si>
   <si>
-    <t>#binary-search</t>
+    <t>#binary-search #必背</t>
+  </si>
+  <si>
+    <t>Find First and Last Position of Element in Sorted Array</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> #array  #binary-search #核心 </t>
   </si>
 </sst>
 </file>
@@ -1255,13 +1261,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="156" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="7"/>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
   <cols>
     <col min="1" max="1" width="9.23076923076923" style="1"/>
     <col min="2" max="2" width="23.4326923076923" style="2" customWidth="1"/>
@@ -1477,7 +1483,7 @@
         <v>45831</v>
       </c>
     </row>
-    <row r="8" ht="17" spans="1:9">
+    <row r="8" ht="34" spans="1:9">
       <c r="A8" s="1">
         <v>704</v>
       </c>
@@ -1503,6 +1509,35 @@
         <v>44339</v>
       </c>
       <c r="I8" s="3">
+        <v>45831</v>
+      </c>
+    </row>
+    <row r="9" ht="51" spans="1:9">
+      <c r="A9" s="1">
+        <v>34</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="1">
+        <v>5</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1">
+        <v>34</v>
+      </c>
+      <c r="H9" s="3">
+        <v>44339</v>
+      </c>
+      <c r="I9" s="3">
         <v>45831</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add markdown file for LeetCode problem 153: Find Minimum in Rotated Sorted Array, including problem description, examples, and solution with complexity analysis. Update workspace configuration to include this new file and adjust last opened files list accordingly.
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="26860" windowHeight="14540"/>
+    <workbookView windowWidth="29100" windowHeight="14520"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
   <si>
     <t>#</t>
   </si>
@@ -108,6 +108,18 @@
   </si>
   <si>
     <t xml:space="preserve"> #array  #binary-search #核心 </t>
+  </si>
+  <si>
+    <t>Find All K-Distant Indices in an Array</t>
+  </si>
+  <si>
+    <t>#array #two-pointers</t>
+  </si>
+  <si>
+    <t>Find Minimum in Rotated Sorted Array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#array  #binary-search #重点 </t>
   </si>
 </sst>
 </file>
@@ -1261,10 +1273,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="156" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="156" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -1541,6 +1553,64 @@
         <v>45831</v>
       </c>
     </row>
+    <row r="10" ht="34" spans="1:9">
+      <c r="A10" s="1">
+        <v>2200</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1</v>
+      </c>
+      <c r="G10" s="1">
+        <v>33</v>
+      </c>
+      <c r="H10" s="3">
+        <v>45832</v>
+      </c>
+      <c r="I10" s="3">
+        <v>45832</v>
+      </c>
+    </row>
+    <row r="11" ht="34" spans="1:9">
+      <c r="A11" s="1">
+        <v>153</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="1">
+        <v>6</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1">
+        <v>10</v>
+      </c>
+      <c r="H11" s="3">
+        <v>45832</v>
+      </c>
+      <c r="I11" s="3">
+        <v>45832</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:I4">
     <sortCondition ref="I2"/>

</xml_diff>

<commit_message>
Update workspace configuration to include new markdown file for LeetCode problem 278: First Bad Version, adjusting file paths, titles, and last opened files list accordingly. Swap positions of problems 153 and 154 in the workspace layout.
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="29100" windowHeight="14520"/>
+    <workbookView windowWidth="29100" windowHeight="14540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
   <si>
     <t>#</t>
   </si>
@@ -120,6 +120,15 @@
   </si>
   <si>
     <t xml:space="preserve">#array  #binary-search #重点 </t>
+  </si>
+  <si>
+    <t>Find Minimum in Rotated Sorted Array II</t>
+  </si>
+  <si>
+    <t>First Bad Version</t>
+  </si>
+  <si>
+    <t>#binary-search #重点</t>
   </si>
 </sst>
 </file>
@@ -1273,10 +1282,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="156" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="156" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -1611,6 +1620,64 @@
         <v>45832</v>
       </c>
     </row>
+    <row r="12" ht="34" spans="1:9">
+      <c r="A12" s="1">
+        <v>154</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1">
+        <v>3</v>
+      </c>
+      <c r="G12" s="1">
+        <v>21</v>
+      </c>
+      <c r="H12" s="3">
+        <v>45832</v>
+      </c>
+      <c r="I12" s="3">
+        <v>45832</v>
+      </c>
+    </row>
+    <row r="13" ht="34" spans="1:9">
+      <c r="A13" s="1">
+        <v>278</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="1">
+        <v>6</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
+      <c r="G13" s="1">
+        <v>3</v>
+      </c>
+      <c r="H13" s="3">
+        <v>45832</v>
+      </c>
+      <c r="I13" s="3">
+        <v>45832</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:I4">
     <sortCondition ref="I2"/>

</xml_diff>

<commit_message>
Add markdown file for LeetCode problem 2040: Kth Smallest Product of Two Sorted Arrays, including problem description, examples, and two approaches with complexity analysis. Update workspace configuration to include this new file and adjust last opened files list accordingly.
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
   <si>
     <t>#</t>
   </si>
@@ -129,6 +129,12 @@
   </si>
   <si>
     <t>#binary-search #重点</t>
+  </si>
+  <si>
+    <t>Kth Smallest Product of Two Sorted Arrays</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#array #binary-search </t>
   </si>
 </sst>
 </file>
@@ -1282,10 +1288,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="156" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -1678,6 +1684,35 @@
         <v>45832</v>
       </c>
     </row>
+    <row r="14" ht="34" spans="1:9">
+      <c r="A14" s="1">
+        <v>2040</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1</v>
+      </c>
+      <c r="G14" s="1">
+        <v>60</v>
+      </c>
+      <c r="H14" s="3">
+        <v>45833</v>
+      </c>
+      <c r="I14" s="3">
+        <v>45833</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:I4">
     <sortCondition ref="I2"/>

</xml_diff>

<commit_message>
Update workspace configuration to reflect changes in markdown files for LeetCode problems 2040 and 2311, including file path adjustments, title updates, and last opened files list modifications. Add new markdown file for problem 2311: Longest Binary Subsequence Less Than or Equal to K, detailing problem description, examples, and a greedy approach with complexity analysis.
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="29100" windowHeight="14540"/>
+    <workbookView windowWidth="26860" windowHeight="14540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="38">
   <si>
     <t>#</t>
   </si>
@@ -135,6 +135,12 @@
   </si>
   <si>
     <t xml:space="preserve">#array #binary-search </t>
+  </si>
+  <si>
+    <t>Longest Binary Subsequence Less Than or Equal to K</t>
+  </si>
+  <si>
+    <t>#string #dp #greedy #memoization</t>
   </si>
 </sst>
 </file>
@@ -1288,10 +1294,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="156" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -1713,6 +1719,35 @@
         <v>45833</v>
       </c>
     </row>
+    <row r="15" ht="51" spans="1:9">
+      <c r="A15" s="1">
+        <v>2311</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="1">
+        <v>1</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1">
+        <v>13</v>
+      </c>
+      <c r="H15" s="3">
+        <v>45834</v>
+      </c>
+      <c r="I15" s="3">
+        <v>45834</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:I4">
     <sortCondition ref="I2"/>

</xml_diff>

<commit_message>
Add markdown file for LeetCode problem 2014: Longest Subsequence Repeated k Times, including problem description, examples, and a brute-force enumeration approach with complexity analysis. Update workspace configuration to reflect changes in file paths and titles.
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="40">
   <si>
     <t>#</t>
   </si>
@@ -141,6 +141,12 @@
   </si>
   <si>
     <t>#string #dp #greedy #memoization</t>
+  </si>
+  <si>
+    <t>Longest Subsequence Repeated k Times</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#string #backtracking #greedy #enumeration </t>
   </si>
 </sst>
 </file>
@@ -1294,10 +1300,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="156" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="156" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -1748,6 +1754,35 @@
         <v>45834</v>
       </c>
     </row>
+    <row r="16" ht="68" spans="1:9">
+      <c r="A16" s="1">
+        <v>2014</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0</v>
+      </c>
+      <c r="F16" s="1">
+        <v>1</v>
+      </c>
+      <c r="G16" s="1">
+        <v>56</v>
+      </c>
+      <c r="H16" s="3">
+        <v>45835</v>
+      </c>
+      <c r="I16" s="3">
+        <v>45835</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:I4">
     <sortCondition ref="I2"/>

</xml_diff>

<commit_message>
Update workspace configuration to reflect changes in file paths and titles for markdown files related to LeetCode problems, including renaming and reorganizing notes for better clarity. Add new content to the markdown file for problem 658: Find K Closest Elements, enhancing the problem description and examples.
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="26860" windowHeight="14540"/>
+    <workbookView windowWidth="29100" windowHeight="14540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
   <si>
     <t>#</t>
   </si>
@@ -129,6 +129,12 @@
   </si>
   <si>
     <t>#binary-search #重点</t>
+  </si>
+  <si>
+    <t>Find K Closest Elements</t>
+  </si>
+  <si>
+    <t>#array #binary-search #重点</t>
   </si>
   <si>
     <t>Kth Smallest Product of Two Sorted Arrays</t>
@@ -1300,10 +1306,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="156" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="156" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -1698,7 +1704,7 @@
     </row>
     <row r="14" ht="34" spans="1:9">
       <c r="A14" s="1">
-        <v>2040</v>
+        <v>658</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>34</v>
@@ -1707,27 +1713,27 @@
         <v>35</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="E14" s="1">
         <v>0</v>
       </c>
       <c r="F14" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G14" s="1">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="H14" s="3">
-        <v>45833</v>
+        <v>45832</v>
       </c>
       <c r="I14" s="3">
-        <v>45833</v>
+        <v>45832</v>
       </c>
     </row>
-    <row r="15" ht="51" spans="1:9">
+    <row r="15" ht="34" spans="1:9">
       <c r="A15" s="1">
-        <v>2311</v>
+        <v>2040</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>36</v>
@@ -1736,27 +1742,27 @@
         <v>37</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="E15" s="1">
+        <v>0</v>
+      </c>
+      <c r="F15" s="1">
         <v>1</v>
       </c>
-      <c r="F15" s="1">
-        <v>0</v>
-      </c>
       <c r="G15" s="1">
-        <v>13</v>
+        <v>60</v>
       </c>
       <c r="H15" s="3">
-        <v>45834</v>
+        <v>45833</v>
       </c>
       <c r="I15" s="3">
-        <v>45834</v>
+        <v>45833</v>
       </c>
     </row>
-    <row r="16" ht="68" spans="1:9">
+    <row r="16" ht="51" spans="1:9">
       <c r="A16" s="1">
-        <v>2014</v>
+        <v>2311</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>38</v>
@@ -1765,22 +1771,59 @@
         <v>39</v>
       </c>
       <c r="D16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="1">
+        <v>1</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1">
+        <v>13</v>
+      </c>
+      <c r="H16" s="3">
+        <v>45834</v>
+      </c>
+      <c r="I16" s="3">
+        <v>45834</v>
+      </c>
+    </row>
+    <row r="17" ht="68" spans="1:9">
+      <c r="A17" s="1">
+        <v>2014</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E17" s="1">
         <v>0</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F17" s="1">
         <v>1</v>
       </c>
-      <c r="G16" s="1">
+      <c r="G17" s="1">
         <v>56</v>
       </c>
-      <c r="H16" s="3">
+      <c r="H17" s="3">
         <v>45835</v>
       </c>
-      <c r="I16" s="3">
+      <c r="I17" s="3">
         <v>45835</v>
+      </c>
+    </row>
+    <row r="18" ht="17" spans="1:2">
+      <c r="A18" s="1">
+        <v>658</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update workspace configuration and markdown files for LeetCode problems 33 and 34: Rename and reorganize notes, reflecting changes in file paths and titles. Add new content to problem 34, including a detailed solution for finding the first and last positions of a target in a sorted array.
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="44">
   <si>
     <t>#</t>
   </si>
@@ -153,6 +153,12 @@
   </si>
   <si>
     <t xml:space="preserve">#string #backtracking #greedy #enumeration </t>
+  </si>
+  <si>
+    <t>Search in Rotated Sorted Array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#array #binary-search #必背 </t>
   </si>
 </sst>
 </file>
@@ -1308,8 +1314,8 @@
   <sheetPr/>
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="156" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="156" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -1571,7 +1577,7 @@
         <v>14</v>
       </c>
       <c r="E9" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F9" s="1">
         <v>1</v>
@@ -1583,7 +1589,7 @@
         <v>44339</v>
       </c>
       <c r="I9" s="3">
-        <v>45831</v>
+        <v>45835</v>
       </c>
     </row>
     <row r="10" ht="34" spans="1:9">
@@ -1818,12 +1824,33 @@
         <v>45835</v>
       </c>
     </row>
-    <row r="18" ht="17" spans="1:2">
+    <row r="18" ht="34" spans="1:9">
       <c r="A18" s="1">
-        <v>658</v>
+        <v>33</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>34</v>
+        <v>42</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="1">
+        <v>3</v>
+      </c>
+      <c r="F18" s="1">
+        <v>1</v>
+      </c>
+      <c r="G18" s="1">
+        <v>25</v>
+      </c>
+      <c r="H18" s="3">
+        <v>45835</v>
+      </c>
+      <c r="I18" s="3">
+        <v>45835</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update workspace configuration and add new markdown file for LeetCode problem 81: Search in Rotated Sorted Array II, reflecting changes in file paths and titles. Adjust last opened files list and current tab settings accordingly.
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="46">
   <si>
     <t>#</t>
   </si>
@@ -159,6 +159,12 @@
   </si>
   <si>
     <t xml:space="preserve">#array #binary-search #必背 </t>
+  </si>
+  <si>
+    <t>Search in Rotated Sorted Array II</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#array  #binary-search #必背 </t>
   </si>
 </sst>
 </file>
@@ -1312,10 +1318,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="156" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="156" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -1853,6 +1859,35 @@
         <v>45835</v>
       </c>
     </row>
+    <row r="19" ht="34" spans="1:9">
+      <c r="A19" s="1">
+        <v>81</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="1">
+        <v>2</v>
+      </c>
+      <c r="F19" s="1">
+        <v>2</v>
+      </c>
+      <c r="G19" s="1">
+        <v>22</v>
+      </c>
+      <c r="H19" s="3">
+        <v>45835</v>
+      </c>
+      <c r="I19" s="3">
+        <v>45835</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:I4">
     <sortCondition ref="I2"/>

</xml_diff>

<commit_message>
Update workspace configuration and add new markdown file for LeetCode problem 2099: Find Subsequence of Length K With the Largest Sum, reflecting changes in file paths, titles, and last opened files list. Adjust current tab settings accordingly.
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="48">
   <si>
     <t>#</t>
   </si>
@@ -165,6 +165,12 @@
   </si>
   <si>
     <t xml:space="preserve">#array  #binary-search #必背 </t>
+  </si>
+  <si>
+    <t>Find Subsequence of Length K With the Largest Sum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#array #hash-table #sorting #heap </t>
   </si>
 </sst>
 </file>
@@ -1318,10 +1324,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="156" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="156" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -1888,6 +1894,35 @@
         <v>45835</v>
       </c>
     </row>
+    <row r="20" ht="51" spans="1:9">
+      <c r="A20" s="1">
+        <v>2099</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="1">
+        <v>1</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0</v>
+      </c>
+      <c r="G20" s="1">
+        <v>13</v>
+      </c>
+      <c r="H20" s="3">
+        <v>45836</v>
+      </c>
+      <c r="I20" s="3">
+        <v>45836</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:I4">
     <sortCondition ref="I2"/>

</xml_diff>

<commit_message>
Add new markdown file for LeetCode problem 594: Longest Harmonious Subsequence, including problem description, examples, and two solution approaches with complexity analysis. Update workspace configuration to reflect changes in file paths and titles.
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="50">
   <si>
     <t>#</t>
   </si>
@@ -171,6 +171,12 @@
   </si>
   <si>
     <t xml:space="preserve">#array #hash-table #sorting #heap </t>
+  </si>
+  <si>
+    <t>Longest Harmonious Subsequence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#array #hash-table #sliding-window #sorting  #counting </t>
   </si>
 </sst>
 </file>
@@ -1324,10 +1330,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="156" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="156" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -1923,6 +1929,39 @@
         <v>45836</v>
       </c>
     </row>
+    <row r="21" spans="8:9">
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+    </row>
+    <row r="22" ht="68" spans="1:9">
+      <c r="A22" s="1">
+        <v>594</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1</v>
+      </c>
+      <c r="F22" s="1">
+        <v>0</v>
+      </c>
+      <c r="G22" s="1">
+        <v>10</v>
+      </c>
+      <c r="H22" s="3">
+        <v>45838</v>
+      </c>
+      <c r="I22" s="3">
+        <v>45838</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:I4">
     <sortCondition ref="I2"/>

</xml_diff>

<commit_message>
Update workspace configuration and add new markdown files for LeetCode problems 4, 594, and 1498: Include problem descriptions, examples, and solutions with complexity analysis. Adjust file paths, titles, and last opened files list accordingly.
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="54">
   <si>
     <t>#</t>
   </si>
@@ -173,10 +173,22 @@
     <t xml:space="preserve">#array #hash-table #sorting #heap </t>
   </si>
   <si>
+    <t>Number of Subsequences That Satisfy the Given Sum Condition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#array #two-pointers #binary-search #sorting </t>
+  </si>
+  <si>
     <t>Longest Harmonious Subsequence</t>
   </si>
   <si>
     <t xml:space="preserve">#array #hash-table #sliding-window #sorting  #counting </t>
+  </si>
+  <si>
+    <t>Median of Two Sorted Arrays</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#array #binary-search #divide-and-conquer #核心 </t>
   </si>
 </sst>
 </file>
@@ -1330,10 +1342,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="156" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="156" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -1929,19 +1941,44 @@
         <v>45836</v>
       </c>
     </row>
-    <row r="21" spans="8:9">
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
+    <row r="21" ht="51" spans="1:9">
+      <c r="A21" s="1">
+        <v>1498</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0</v>
+      </c>
+      <c r="F21" s="1">
+        <v>1</v>
+      </c>
+      <c r="G21" s="1">
+        <v>18</v>
+      </c>
+      <c r="H21" s="3">
+        <v>45837</v>
+      </c>
+      <c r="I21" s="3">
+        <v>45837</v>
+      </c>
     </row>
     <row r="22" ht="68" spans="1:9">
       <c r="A22" s="1">
         <v>594</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>11</v>
@@ -1959,6 +1996,35 @@
         <v>45838</v>
       </c>
       <c r="I22" s="3">
+        <v>45838</v>
+      </c>
+    </row>
+    <row r="23" ht="51" spans="1:9">
+      <c r="A23" s="1">
+        <v>4</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" s="1">
+        <v>1</v>
+      </c>
+      <c r="F23" s="1">
+        <v>4</v>
+      </c>
+      <c r="G23" s="1">
+        <v>18</v>
+      </c>
+      <c r="H23" s="3">
+        <v>45838</v>
+      </c>
+      <c r="I23" s="3">
         <v>45838</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update workspace configuration and add new markdown files for LeetCode problems 74 and 162: Include problem descriptions, examples, and solutions with complexity analysis. Adjust file paths, titles, and last opened files list accordingly.
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="58">
   <si>
     <t>#</t>
   </si>
@@ -189,6 +189,18 @@
   </si>
   <si>
     <t xml:space="preserve">#array #binary-search #divide-and-conquer #核心 </t>
+  </si>
+  <si>
+    <t>Search a 2D Matrix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#array  #binary-search #matrix #核心 </t>
+  </si>
+  <si>
+    <t>Find Peak Element</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#array #binary-search #核心 </t>
   </si>
 </sst>
 </file>
@@ -1342,10 +1354,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="156" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="156" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -2028,6 +2040,64 @@
         <v>45838</v>
       </c>
     </row>
+    <row r="24" ht="51" spans="1:9">
+      <c r="A24" s="1">
+        <v>74</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" s="1">
+        <v>4</v>
+      </c>
+      <c r="F24" s="1">
+        <v>1</v>
+      </c>
+      <c r="G24" s="1">
+        <v>10</v>
+      </c>
+      <c r="H24" s="3">
+        <v>45838</v>
+      </c>
+      <c r="I24" s="3">
+        <v>45838</v>
+      </c>
+    </row>
+    <row r="25" ht="34" spans="1:9">
+      <c r="A25" s="1">
+        <v>162</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="1">
+        <v>3</v>
+      </c>
+      <c r="F25" s="1">
+        <v>0</v>
+      </c>
+      <c r="G25" s="1">
+        <v>18</v>
+      </c>
+      <c r="H25" s="3">
+        <v>45838</v>
+      </c>
+      <c r="I25" s="3">
+        <v>45838</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:I4">
     <sortCondition ref="I2"/>

</xml_diff>

<commit_message>
Add new markdown file for LeetCode problem 852: Peak Index in a Mountain Array, including problem description, examples, and solution with complexity analysis. Update workspace configuration to reflect changes in file paths and titles.
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="60">
   <si>
     <t>#</t>
   </si>
@@ -201,6 +201,12 @@
   </si>
   <si>
     <t xml:space="preserve">#array #binary-search #核心 </t>
+  </si>
+  <si>
+    <t>Peak Index in a Mountain Array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#array #binary-search #重点 </t>
   </si>
 </sst>
 </file>
@@ -1354,10 +1360,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="156" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -2098,6 +2104,35 @@
         <v>45838</v>
       </c>
     </row>
+    <row r="26" ht="34" spans="1:9">
+      <c r="A26" s="1">
+        <v>852</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E26" s="1">
+        <v>3</v>
+      </c>
+      <c r="F26" s="1">
+        <v>0</v>
+      </c>
+      <c r="G26" s="1">
+        <v>3</v>
+      </c>
+      <c r="H26" s="3">
+        <v>45838</v>
+      </c>
+      <c r="I26" s="3">
+        <v>45838</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:I4">
     <sortCondition ref="I2"/>

</xml_diff>

<commit_message>
Update workspace configuration and add new markdown files for LeetCode problems 852 and 875: Include problem descriptions, examples, and solutions with complexity analysis. Adjust file paths and last opened files list accordingly.
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="62">
   <si>
     <t>#</t>
   </si>
@@ -207,6 +207,12 @@
   </si>
   <si>
     <t xml:space="preserve">#array #binary-search #重点 </t>
+  </si>
+  <si>
+    <t>Koko Eating Bananas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#two-pointers #array #binary-search #必背 </t>
   </si>
 </sst>
 </file>
@@ -1360,10 +1366,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="156" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -2133,6 +2139,35 @@
         <v>45838</v>
       </c>
     </row>
+    <row r="27" ht="51" spans="1:9">
+      <c r="A27" s="1">
+        <v>875</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E27" s="1">
+        <v>3</v>
+      </c>
+      <c r="F27" s="1">
+        <v>0</v>
+      </c>
+      <c r="G27" s="1">
+        <v>10</v>
+      </c>
+      <c r="H27" s="3">
+        <v>45838</v>
+      </c>
+      <c r="I27" s="3">
+        <v>45838</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:I4">
     <sortCondition ref="I2"/>

</xml_diff>

<commit_message>
Update workspace configuration and add new markdown file for LeetCode problem 1283: Find the Smallest Divisor Given a Threshold, including problem description, examples, and solution with complexity analysis. Adjust file paths and titles accordingly, and link to related problem 875: Koko Eating Bananas.
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="63">
   <si>
     <t>#</t>
   </si>
@@ -212,7 +212,10 @@
     <t>Koko Eating Bananas</t>
   </si>
   <si>
-    <t xml:space="preserve">#two-pointers #array #binary-search #必背 </t>
+    <t xml:space="preserve">#two-pointers #array #binary-search #核心 </t>
+  </si>
+  <si>
+    <t>Find the Smallest Divisor Given a Threshold</t>
   </si>
 </sst>
 </file>
@@ -1366,10 +1369,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="156" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="156" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -2168,6 +2171,35 @@
         <v>45838</v>
       </c>
     </row>
+    <row r="28" ht="51" spans="1:9">
+      <c r="A28" s="1">
+        <v>1283</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" s="1">
+        <v>3</v>
+      </c>
+      <c r="F28" s="1">
+        <v>0</v>
+      </c>
+      <c r="G28" s="1">
+        <v>10</v>
+      </c>
+      <c r="H28" s="3">
+        <v>45838</v>
+      </c>
+      <c r="I28" s="3">
+        <v>45838</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:I4">
     <sortCondition ref="I2"/>

</xml_diff>

<commit_message>
Update workspace configuration and add new markdown file for LeetCode problem 69: Sqrt(x). Include problem description, examples, and solution with complexity analysis. Adjust file paths and titles accordingly, and update last opened files list.
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="65">
   <si>
     <t>#</t>
   </si>
@@ -216,6 +216,12 @@
   </si>
   <si>
     <t>Find the Smallest Divisor Given a Threshold</t>
+  </si>
+  <si>
+    <t>Sqrt(x)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#math #binary-search #重点 </t>
   </si>
 </sst>
 </file>
@@ -1369,10 +1375,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="156" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -2200,6 +2206,35 @@
         <v>45838</v>
       </c>
     </row>
+    <row r="29" ht="34" spans="1:9">
+      <c r="A29" s="1">
+        <v>69</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" s="1">
+        <v>4</v>
+      </c>
+      <c r="F29" s="1">
+        <v>0</v>
+      </c>
+      <c r="G29" s="1">
+        <v>4</v>
+      </c>
+      <c r="H29" s="3">
+        <v>45838</v>
+      </c>
+      <c r="I29" s="3">
+        <v>45838</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:I4">
     <sortCondition ref="I2"/>

</xml_diff>

<commit_message>
Update workspace configuration and markdown files: Change titles and file paths for multiple notes, add new markdown for LeetCode problem 3330, and implement solution for counting possible original strings based on consecutive characters.
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="29100" windowHeight="14540"/>
+    <workbookView windowWidth="29100" windowHeight="14520"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="73">
   <si>
     <t>#</t>
   </si>
@@ -222,6 +222,30 @@
   </si>
   <si>
     <t xml:space="preserve">#math #binary-search #重点 </t>
+  </si>
+  <si>
+    <t>Maximum 69 Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#math #greedy </t>
+  </si>
+  <si>
+    <t>Sort an Array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#array #divide-and-conquer #sorting #heap </t>
+  </si>
+  <si>
+    <t>Find the Original Typed String I</t>
+  </si>
+  <si>
+    <t>#string</t>
+  </si>
+  <si>
+    <t>Largest BST Subtree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#dynamic-programming #tree #dfs #bst #binary-tree </t>
   </si>
 </sst>
 </file>
@@ -1375,10 +1399,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="156" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="156" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -2235,6 +2259,122 @@
         <v>45838</v>
       </c>
     </row>
+    <row r="30" ht="17" spans="1:9">
+      <c r="A30" s="1">
+        <v>1323</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" s="1">
+        <v>1</v>
+      </c>
+      <c r="F30" s="1">
+        <v>0</v>
+      </c>
+      <c r="G30" s="1">
+        <v>9</v>
+      </c>
+      <c r="H30" s="3">
+        <v>45838</v>
+      </c>
+      <c r="I30" s="3">
+        <v>45838</v>
+      </c>
+    </row>
+    <row r="31" ht="51" spans="1:9">
+      <c r="A31" s="1">
+        <v>912</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E31" s="1">
+        <v>2</v>
+      </c>
+      <c r="F31" s="1">
+        <v>2</v>
+      </c>
+      <c r="G31" s="1">
+        <v>18</v>
+      </c>
+      <c r="H31" s="3">
+        <v>45838</v>
+      </c>
+      <c r="I31" s="3">
+        <v>45838</v>
+      </c>
+    </row>
+    <row r="32" ht="34" spans="1:9">
+      <c r="A32" s="1">
+        <v>3330</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" s="1">
+        <v>1</v>
+      </c>
+      <c r="F32" s="1">
+        <v>0</v>
+      </c>
+      <c r="G32" s="1">
+        <v>16</v>
+      </c>
+      <c r="H32" s="3">
+        <v>45839</v>
+      </c>
+      <c r="I32" s="3">
+        <v>45839</v>
+      </c>
+    </row>
+    <row r="33" ht="68" spans="1:9">
+      <c r="A33" s="1">
+        <v>333</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E33" s="1">
+        <v>0</v>
+      </c>
+      <c r="F33" s="1">
+        <v>1</v>
+      </c>
+      <c r="G33" s="1">
+        <v>53</v>
+      </c>
+      <c r="H33" s="3">
+        <v>45839</v>
+      </c>
+      <c r="I33" s="3">
+        <v>45839</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:I4">
     <sortCondition ref="I2"/>

</xml_diff>

<commit_message>
Update workspace configuration and add new markdown for LeetCode problem 3333: Replace references to problem 26 with 3333 in the workspace, and include detailed problem description, examples, and a Python solution for counting possible original strings based on consecutive characters.
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="29100" windowHeight="14520"/>
+    <workbookView windowWidth="29100" windowHeight="14540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="83">
   <si>
     <t>#</t>
   </si>
@@ -246,6 +246,36 @@
   </si>
   <si>
     <t xml:space="preserve">#dynamic-programming #tree #dfs #bst #binary-tree </t>
+  </si>
+  <si>
+    <t>Smallest Rectangle Enclosing Black Pixels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#array #binary-search #bfs #dfs #matrix #重点 </t>
+  </si>
+  <si>
+    <t>Search in a Sorted Array of Unknown Size</t>
+  </si>
+  <si>
+    <t>Sort Colors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#array  #two-pointers #sorting #必背 </t>
+  </si>
+  <si>
+    <t>Remove Duplicates from Sorted Array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#array #two-pointers #核心 </t>
+  </si>
+  <si>
+    <t>Find the Original Typed String II</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#string #dynamic-programming  #prefix-sum </t>
+  </si>
+  <si>
+    <t>？？dp 难！</t>
   </si>
 </sst>
 </file>
@@ -1399,10 +1429,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="156" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="156" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -1415,7 +1445,8 @@
     <col min="6" max="7" width="9.23076923076923" style="1"/>
     <col min="8" max="8" width="12.0769230769231" style="1"/>
     <col min="9" max="9" width="14.0576923076923" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.23076923076923" style="1"/>
+    <col min="10" max="10" width="23.2115384615385" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.23076923076923" style="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="34" customHeight="1" spans="1:9">
@@ -2375,11 +2406,160 @@
         <v>45839</v>
       </c>
     </row>
+    <row r="34" ht="51" spans="1:9">
+      <c r="A34" s="1">
+        <v>302</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E34" s="1">
+        <v>1</v>
+      </c>
+      <c r="F34" s="1">
+        <v>3</v>
+      </c>
+      <c r="G34" s="1">
+        <v>38</v>
+      </c>
+      <c r="H34" s="3">
+        <v>45839</v>
+      </c>
+      <c r="I34" s="3">
+        <v>45839</v>
+      </c>
+    </row>
+    <row r="35" ht="34" spans="1:9">
+      <c r="A35" s="1">
+        <v>702</v>
+      </c>
+      <c r="B35" t="s">
+        <v>75</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E35" s="1">
+        <v>2</v>
+      </c>
+      <c r="F35" s="1">
+        <v>1</v>
+      </c>
+      <c r="G35" s="1">
+        <v>3</v>
+      </c>
+      <c r="H35" s="3">
+        <v>45839</v>
+      </c>
+      <c r="I35" s="3">
+        <v>45839</v>
+      </c>
+    </row>
+    <row r="36" ht="51" spans="1:9">
+      <c r="A36" s="1">
+        <v>75</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E36" s="1">
+        <v>3</v>
+      </c>
+      <c r="F36" s="1">
+        <v>0</v>
+      </c>
+      <c r="G36" s="1">
+        <v>6</v>
+      </c>
+      <c r="H36" s="3">
+        <v>45839</v>
+      </c>
+      <c r="I36" s="3">
+        <v>45839</v>
+      </c>
+    </row>
+    <row r="37" ht="34" spans="1:9">
+      <c r="A37" s="1">
+        <v>26</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37" s="1">
+        <v>3</v>
+      </c>
+      <c r="F37" s="1">
+        <v>0</v>
+      </c>
+      <c r="G37" s="1">
+        <v>5</v>
+      </c>
+      <c r="H37" s="3">
+        <v>45839</v>
+      </c>
+      <c r="I37" s="3">
+        <v>45839</v>
+      </c>
+    </row>
+    <row r="38" ht="51" spans="1:10">
+      <c r="A38" s="1">
+        <v>3333</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E38" s="1">
+        <v>0</v>
+      </c>
+      <c r="F38" s="1">
+        <v>1</v>
+      </c>
+      <c r="G38" s="1">
+        <v>40</v>
+      </c>
+      <c r="H38" s="3">
+        <v>45840</v>
+      </c>
+      <c r="I38" s="3">
+        <v>45840</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:I4">
     <sortCondition ref="I2"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add new markdown file for LeetCode problem 283: Include problem description, examples, and a Python solution for moving zeroes, along with complexity analysis. Update workspace configuration to reflect changes.
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -7,7 +7,7 @@
     <workbookView windowWidth="29100" windowHeight="14540"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="86">
   <si>
     <t>#</t>
   </si>
@@ -276,6 +276,15 @@
   </si>
   <si>
     <t>？？dp 难！</t>
+  </si>
+  <si>
+    <t>Remove Duplicates from Sorted Array II</t>
+  </si>
+  <si>
+    <t>Merge Sorted Array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#array #two-pointers #sorting #核心 </t>
   </si>
 </sst>
 </file>
@@ -891,17 +900,20 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1429,10 +1441,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J38"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="156" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="162" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -1449,7 +1461,7 @@
     <col min="11" max="16384" width="9.23076923076923" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="34" customHeight="1" spans="1:9">
+    <row r="1" s="1" customFormat="1" ht="34" customHeight="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1478,7 +1490,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" ht="17" spans="1:9">
+    <row r="2" s="1" customFormat="1" ht="17" spans="1:9">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1500,14 +1512,14 @@
       <c r="G2" s="1">
         <v>5</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="4">
         <v>44197</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2" s="4">
         <v>45826</v>
       </c>
     </row>
-    <row r="3" ht="53" customHeight="1" spans="1:9">
+    <row r="3" s="1" customFormat="1" ht="53" customHeight="1" spans="1:9">
       <c r="A3" s="1">
         <v>2966</v>
       </c>
@@ -1529,14 +1541,14 @@
       <c r="G3" s="1">
         <v>10</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="4">
         <v>45826</v>
       </c>
-      <c r="I3" s="3">
+      <c r="I3" s="4">
         <v>45826</v>
       </c>
     </row>
-    <row r="4" ht="51" spans="1:9">
+    <row r="4" s="1" customFormat="1" ht="51" spans="1:9">
       <c r="A4" s="1">
         <v>2294</v>
       </c>
@@ -1558,14 +1570,14 @@
       <c r="G4" s="1">
         <v>10</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="4">
         <v>45827</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="4">
         <v>45827</v>
       </c>
     </row>
-    <row r="5" ht="51" spans="1:9">
+    <row r="5" s="1" customFormat="1" ht="51" spans="1:9">
       <c r="A5" s="1">
         <v>3443</v>
       </c>
@@ -1587,14 +1599,14 @@
       <c r="G5" s="1">
         <v>25</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="4">
         <v>45828</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="4">
         <v>45828</v>
       </c>
     </row>
-    <row r="6" ht="51" spans="1:9">
+    <row r="6" s="1" customFormat="1" ht="51" spans="1:9">
       <c r="A6" s="1">
         <v>3085</v>
       </c>
@@ -1616,14 +1628,14 @@
       <c r="G6" s="1">
         <v>25</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="4">
         <v>45829</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="4">
         <v>45829</v>
       </c>
     </row>
-    <row r="7" ht="51" spans="1:9">
+    <row r="7" s="1" customFormat="1" ht="51" spans="1:9">
       <c r="A7" s="1">
         <v>2081</v>
       </c>
@@ -1645,14 +1657,14 @@
       <c r="G7" s="1">
         <v>40</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="4">
         <v>45831</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="4">
         <v>45831</v>
       </c>
     </row>
-    <row r="8" ht="34" spans="1:9">
+    <row r="8" s="1" customFormat="1" ht="34" spans="1:9">
       <c r="A8" s="1">
         <v>704</v>
       </c>
@@ -1674,14 +1686,14 @@
       <c r="G8" s="1">
         <v>10</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="4">
         <v>44339</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I8" s="4">
         <v>45831</v>
       </c>
     </row>
-    <row r="9" ht="51" spans="1:9">
+    <row r="9" s="1" customFormat="1" ht="51" spans="1:9">
       <c r="A9" s="1">
         <v>34</v>
       </c>
@@ -1703,14 +1715,14 @@
       <c r="G9" s="1">
         <v>34</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="4">
         <v>44339</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9" s="4">
         <v>45835</v>
       </c>
     </row>
-    <row r="10" ht="34" spans="1:9">
+    <row r="10" s="1" customFormat="1" ht="34" spans="1:9">
       <c r="A10" s="1">
         <v>2200</v>
       </c>
@@ -1732,14 +1744,14 @@
       <c r="G10" s="1">
         <v>33</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="4">
         <v>45832</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I10" s="4">
         <v>45832</v>
       </c>
     </row>
-    <row r="11" ht="34" spans="1:9">
+    <row r="11" s="1" customFormat="1" ht="34" spans="1:9">
       <c r="A11" s="1">
         <v>153</v>
       </c>
@@ -1761,14 +1773,14 @@
       <c r="G11" s="1">
         <v>10</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="4">
         <v>45832</v>
       </c>
-      <c r="I11" s="3">
+      <c r="I11" s="4">
         <v>45832</v>
       </c>
     </row>
-    <row r="12" ht="34" spans="1:9">
+    <row r="12" s="1" customFormat="1" ht="34" spans="1:9">
       <c r="A12" s="1">
         <v>154</v>
       </c>
@@ -1790,14 +1802,14 @@
       <c r="G12" s="1">
         <v>21</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="4">
         <v>45832</v>
       </c>
-      <c r="I12" s="3">
+      <c r="I12" s="4">
         <v>45832</v>
       </c>
     </row>
-    <row r="13" ht="34" spans="1:9">
+    <row r="13" s="1" customFormat="1" ht="34" spans="1:9">
       <c r="A13" s="1">
         <v>278</v>
       </c>
@@ -1819,14 +1831,14 @@
       <c r="G13" s="1">
         <v>3</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H13" s="4">
         <v>45832</v>
       </c>
-      <c r="I13" s="3">
+      <c r="I13" s="4">
         <v>45832</v>
       </c>
     </row>
-    <row r="14" ht="34" spans="1:9">
+    <row r="14" s="1" customFormat="1" ht="34" spans="1:9">
       <c r="A14" s="1">
         <v>658</v>
       </c>
@@ -1848,14 +1860,14 @@
       <c r="G14" s="1">
         <v>20</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H14" s="4">
         <v>45832</v>
       </c>
-      <c r="I14" s="3">
+      <c r="I14" s="4">
         <v>45832</v>
       </c>
     </row>
-    <row r="15" ht="34" spans="1:9">
+    <row r="15" s="1" customFormat="1" ht="34" spans="1:9">
       <c r="A15" s="1">
         <v>2040</v>
       </c>
@@ -1877,14 +1889,14 @@
       <c r="G15" s="1">
         <v>60</v>
       </c>
-      <c r="H15" s="3">
+      <c r="H15" s="4">
         <v>45833</v>
       </c>
-      <c r="I15" s="3">
+      <c r="I15" s="4">
         <v>45833</v>
       </c>
     </row>
-    <row r="16" ht="51" spans="1:9">
+    <row r="16" s="1" customFormat="1" ht="51" spans="1:9">
       <c r="A16" s="1">
         <v>2311</v>
       </c>
@@ -1906,14 +1918,14 @@
       <c r="G16" s="1">
         <v>13</v>
       </c>
-      <c r="H16" s="3">
+      <c r="H16" s="4">
         <v>45834</v>
       </c>
-      <c r="I16" s="3">
+      <c r="I16" s="4">
         <v>45834</v>
       </c>
     </row>
-    <row r="17" ht="68" spans="1:9">
+    <row r="17" s="1" customFormat="1" ht="68" spans="1:9">
       <c r="A17" s="1">
         <v>2014</v>
       </c>
@@ -1935,14 +1947,14 @@
       <c r="G17" s="1">
         <v>56</v>
       </c>
-      <c r="H17" s="3">
+      <c r="H17" s="4">
         <v>45835</v>
       </c>
-      <c r="I17" s="3">
+      <c r="I17" s="4">
         <v>45835</v>
       </c>
     </row>
-    <row r="18" ht="34" spans="1:9">
+    <row r="18" s="1" customFormat="1" ht="34" spans="1:9">
       <c r="A18" s="1">
         <v>33</v>
       </c>
@@ -1964,14 +1976,14 @@
       <c r="G18" s="1">
         <v>25</v>
       </c>
-      <c r="H18" s="3">
+      <c r="H18" s="4">
         <v>45835</v>
       </c>
-      <c r="I18" s="3">
+      <c r="I18" s="4">
         <v>45835</v>
       </c>
     </row>
-    <row r="19" ht="34" spans="1:9">
+    <row r="19" s="1" customFormat="1" ht="34" spans="1:9">
       <c r="A19" s="1">
         <v>81</v>
       </c>
@@ -1993,14 +2005,14 @@
       <c r="G19" s="1">
         <v>22</v>
       </c>
-      <c r="H19" s="3">
+      <c r="H19" s="4">
         <v>45835</v>
       </c>
-      <c r="I19" s="3">
+      <c r="I19" s="4">
         <v>45835</v>
       </c>
     </row>
-    <row r="20" ht="51" spans="1:9">
+    <row r="20" s="1" customFormat="1" ht="51" spans="1:9">
       <c r="A20" s="1">
         <v>2099</v>
       </c>
@@ -2022,14 +2034,14 @@
       <c r="G20" s="1">
         <v>13</v>
       </c>
-      <c r="H20" s="3">
+      <c r="H20" s="4">
         <v>45836</v>
       </c>
-      <c r="I20" s="3">
+      <c r="I20" s="4">
         <v>45836</v>
       </c>
     </row>
-    <row r="21" ht="51" spans="1:9">
+    <row r="21" s="1" customFormat="1" ht="51" spans="1:9">
       <c r="A21" s="1">
         <v>1498</v>
       </c>
@@ -2051,14 +2063,14 @@
       <c r="G21" s="1">
         <v>18</v>
       </c>
-      <c r="H21" s="3">
+      <c r="H21" s="4">
         <v>45837</v>
       </c>
-      <c r="I21" s="3">
+      <c r="I21" s="4">
         <v>45837</v>
       </c>
     </row>
-    <row r="22" ht="68" spans="1:9">
+    <row r="22" s="1" customFormat="1" ht="68" spans="1:9">
       <c r="A22" s="1">
         <v>594</v>
       </c>
@@ -2080,14 +2092,14 @@
       <c r="G22" s="1">
         <v>10</v>
       </c>
-      <c r="H22" s="3">
+      <c r="H22" s="4">
         <v>45838</v>
       </c>
-      <c r="I22" s="3">
+      <c r="I22" s="4">
         <v>45838</v>
       </c>
     </row>
-    <row r="23" ht="51" spans="1:9">
+    <row r="23" s="1" customFormat="1" ht="51" spans="1:9">
       <c r="A23" s="1">
         <v>4</v>
       </c>
@@ -2109,14 +2121,14 @@
       <c r="G23" s="1">
         <v>18</v>
       </c>
-      <c r="H23" s="3">
+      <c r="H23" s="4">
         <v>45838</v>
       </c>
-      <c r="I23" s="3">
+      <c r="I23" s="4">
         <v>45838</v>
       </c>
     </row>
-    <row r="24" ht="51" spans="1:9">
+    <row r="24" s="1" customFormat="1" ht="51" spans="1:9">
       <c r="A24" s="1">
         <v>74</v>
       </c>
@@ -2138,14 +2150,14 @@
       <c r="G24" s="1">
         <v>10</v>
       </c>
-      <c r="H24" s="3">
+      <c r="H24" s="4">
         <v>45838</v>
       </c>
-      <c r="I24" s="3">
+      <c r="I24" s="4">
         <v>45838</v>
       </c>
     </row>
-    <row r="25" ht="34" spans="1:9">
+    <row r="25" s="1" customFormat="1" ht="34" spans="1:9">
       <c r="A25" s="1">
         <v>162</v>
       </c>
@@ -2167,14 +2179,14 @@
       <c r="G25" s="1">
         <v>18</v>
       </c>
-      <c r="H25" s="3">
+      <c r="H25" s="4">
         <v>45838</v>
       </c>
-      <c r="I25" s="3">
+      <c r="I25" s="4">
         <v>45838</v>
       </c>
     </row>
-    <row r="26" ht="34" spans="1:9">
+    <row r="26" s="1" customFormat="1" ht="34" spans="1:9">
       <c r="A26" s="1">
         <v>852</v>
       </c>
@@ -2196,14 +2208,14 @@
       <c r="G26" s="1">
         <v>3</v>
       </c>
-      <c r="H26" s="3">
+      <c r="H26" s="4">
         <v>45838</v>
       </c>
-      <c r="I26" s="3">
+      <c r="I26" s="4">
         <v>45838</v>
       </c>
     </row>
-    <row r="27" ht="51" spans="1:9">
+    <row r="27" s="1" customFormat="1" ht="51" spans="1:9">
       <c r="A27" s="1">
         <v>875</v>
       </c>
@@ -2225,14 +2237,14 @@
       <c r="G27" s="1">
         <v>10</v>
       </c>
-      <c r="H27" s="3">
+      <c r="H27" s="4">
         <v>45838</v>
       </c>
-      <c r="I27" s="3">
+      <c r="I27" s="4">
         <v>45838</v>
       </c>
     </row>
-    <row r="28" ht="51" spans="1:9">
+    <row r="28" s="1" customFormat="1" ht="51" spans="1:9">
       <c r="A28" s="1">
         <v>1283</v>
       </c>
@@ -2254,14 +2266,14 @@
       <c r="G28" s="1">
         <v>10</v>
       </c>
-      <c r="H28" s="3">
+      <c r="H28" s="4">
         <v>45838</v>
       </c>
-      <c r="I28" s="3">
+      <c r="I28" s="4">
         <v>45838</v>
       </c>
     </row>
-    <row r="29" ht="34" spans="1:9">
+    <row r="29" s="1" customFormat="1" ht="34" spans="1:9">
       <c r="A29" s="1">
         <v>69</v>
       </c>
@@ -2283,14 +2295,14 @@
       <c r="G29" s="1">
         <v>4</v>
       </c>
-      <c r="H29" s="3">
+      <c r="H29" s="4">
         <v>45838</v>
       </c>
-      <c r="I29" s="3">
+      <c r="I29" s="4">
         <v>45838</v>
       </c>
     </row>
-    <row r="30" ht="17" spans="1:9">
+    <row r="30" s="1" customFormat="1" ht="17" spans="1:9">
       <c r="A30" s="1">
         <v>1323</v>
       </c>
@@ -2312,14 +2324,14 @@
       <c r="G30" s="1">
         <v>9</v>
       </c>
-      <c r="H30" s="3">
+      <c r="H30" s="4">
         <v>45838</v>
       </c>
-      <c r="I30" s="3">
+      <c r="I30" s="4">
         <v>45838</v>
       </c>
     </row>
-    <row r="31" ht="51" spans="1:9">
+    <row r="31" s="1" customFormat="1" ht="51" spans="1:9">
       <c r="A31" s="1">
         <v>912</v>
       </c>
@@ -2341,14 +2353,14 @@
       <c r="G31" s="1">
         <v>18</v>
       </c>
-      <c r="H31" s="3">
+      <c r="H31" s="4">
         <v>45838</v>
       </c>
-      <c r="I31" s="3">
+      <c r="I31" s="4">
         <v>45838</v>
       </c>
     </row>
-    <row r="32" ht="34" spans="1:9">
+    <row r="32" s="1" customFormat="1" ht="34" spans="1:9">
       <c r="A32" s="1">
         <v>3330</v>
       </c>
@@ -2370,14 +2382,14 @@
       <c r="G32" s="1">
         <v>16</v>
       </c>
-      <c r="H32" s="3">
+      <c r="H32" s="4">
         <v>45839</v>
       </c>
-      <c r="I32" s="3">
+      <c r="I32" s="4">
         <v>45839</v>
       </c>
     </row>
-    <row r="33" ht="68" spans="1:9">
+    <row r="33" s="1" customFormat="1" ht="68" spans="1:9">
       <c r="A33" s="1">
         <v>333</v>
       </c>
@@ -2399,14 +2411,14 @@
       <c r="G33" s="1">
         <v>53</v>
       </c>
-      <c r="H33" s="3">
+      <c r="H33" s="4">
         <v>45839</v>
       </c>
-      <c r="I33" s="3">
+      <c r="I33" s="4">
         <v>45839</v>
       </c>
     </row>
-    <row r="34" ht="51" spans="1:9">
+    <row r="34" s="1" customFormat="1" ht="51" spans="1:9">
       <c r="A34" s="1">
         <v>302</v>
       </c>
@@ -2428,18 +2440,18 @@
       <c r="G34" s="1">
         <v>38</v>
       </c>
-      <c r="H34" s="3">
+      <c r="H34" s="4">
         <v>45839</v>
       </c>
-      <c r="I34" s="3">
+      <c r="I34" s="4">
         <v>45839</v>
       </c>
     </row>
-    <row r="35" ht="34" spans="1:9">
+    <row r="35" s="1" customFormat="1" ht="34" spans="1:9">
       <c r="A35" s="1">
         <v>702</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="3" t="s">
         <v>75</v>
       </c>
       <c r="C35" s="2" t="s">
@@ -2457,14 +2469,14 @@
       <c r="G35" s="1">
         <v>3</v>
       </c>
-      <c r="H35" s="3">
+      <c r="H35" s="4">
         <v>45839</v>
       </c>
-      <c r="I35" s="3">
+      <c r="I35" s="4">
         <v>45839</v>
       </c>
     </row>
-    <row r="36" ht="51" spans="1:9">
+    <row r="36" s="1" customFormat="1" ht="51" spans="1:9">
       <c r="A36" s="1">
         <v>75</v>
       </c>
@@ -2486,14 +2498,14 @@
       <c r="G36" s="1">
         <v>6</v>
       </c>
-      <c r="H36" s="3">
+      <c r="H36" s="4">
         <v>45839</v>
       </c>
-      <c r="I36" s="3">
+      <c r="I36" s="4">
         <v>45839</v>
       </c>
     </row>
-    <row r="37" ht="34" spans="1:9">
+    <row r="37" s="1" customFormat="1" ht="34" spans="1:9">
       <c r="A37" s="1">
         <v>26</v>
       </c>
@@ -2515,14 +2527,14 @@
       <c r="G37" s="1">
         <v>5</v>
       </c>
-      <c r="H37" s="3">
+      <c r="H37" s="4">
         <v>45839</v>
       </c>
-      <c r="I37" s="3">
+      <c r="I37" s="4">
         <v>45839</v>
       </c>
     </row>
-    <row r="38" ht="51" spans="1:10">
+    <row r="38" s="1" customFormat="1" ht="51" spans="1:10">
       <c r="A38" s="1">
         <v>3333</v>
       </c>
@@ -2544,22 +2556,76 @@
       <c r="G38" s="1">
         <v>40</v>
       </c>
-      <c r="H38" s="3">
+      <c r="H38" s="4">
         <v>45840</v>
       </c>
-      <c r="I38" s="3">
+      <c r="I38" s="4">
         <v>45840</v>
       </c>
       <c r="J38" s="1" t="s">
         <v>82</v>
       </c>
     </row>
+    <row r="39" s="1" customFormat="1" ht="34" spans="1:9">
+      <c r="A39" s="1">
+        <v>80</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E39" s="1">
+        <v>3</v>
+      </c>
+      <c r="F39" s="1">
+        <v>0</v>
+      </c>
+      <c r="G39" s="1">
+        <v>22</v>
+      </c>
+      <c r="H39" s="4">
+        <v>45840</v>
+      </c>
+      <c r="I39" s="4">
+        <v>45840</v>
+      </c>
+    </row>
+    <row r="40" ht="51" spans="1:9">
+      <c r="A40" s="1">
+        <v>88</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E40" s="1">
+        <v>3</v>
+      </c>
+      <c r="F40" s="1">
+        <v>0</v>
+      </c>
+      <c r="G40" s="1">
+        <v>15</v>
+      </c>
+      <c r="H40" s="4">
+        <v>45840</v>
+      </c>
+      <c r="I40" s="4">
+        <v>45840</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A2:I4">
-    <sortCondition ref="I2"/>
-  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update workspace configuration and markdown files: Add new markdown for problem 349: Intersection of Two Arrays, update links and titles for related problems, and add new markdown for problem 3304: Find the K-th Character in String Game.
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="29100" windowHeight="14540"/>
+    <workbookView windowHeight="16760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="95">
   <si>
     <t>#</t>
   </si>
@@ -65,6 +65,9 @@
     <t>easy</t>
   </si>
   <si>
+    <t>?</t>
+  </si>
+  <si>
     <t>Divide Array Into Arrays With Max Difference</t>
   </si>
   <si>
@@ -285,6 +288,30 @@
   </si>
   <si>
     <t xml:space="preserve">#array #two-pointers #sorting #核心 </t>
+  </si>
+  <si>
+    <t>Move Zeroes</t>
+  </si>
+  <si>
+    <t>Kth Largest Element in an Array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#heap #divide-and-conquer  #quickselect #array #核心 </t>
+  </si>
+  <si>
+    <t>Top K Frequent Elements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#array #divide-and-conquer #quickselect #核心 </t>
+  </si>
+  <si>
+    <t>？</t>
+  </si>
+  <si>
+    <t>Find the K-th Character in String Game</t>
+  </si>
+  <si>
+    <t>#math #bit-minipulation #recursive #simulation</t>
   </si>
 </sst>
 </file>
@@ -1441,10 +1468,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="162" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="I40" sqref="I40"/>
+    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="162" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="I44" sqref="I44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -1490,7 +1517,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" s="1" customFormat="1" ht="17" spans="1:9">
+    <row r="2" s="1" customFormat="1" ht="17" spans="1:10">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1518,19 +1545,22 @@
       <c r="I2" s="4">
         <v>45826</v>
       </c>
-    </row>
-    <row r="3" s="1" customFormat="1" ht="53" customHeight="1" spans="1:9">
+      <c r="J2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" s="1" customFormat="1" ht="53" customHeight="1" spans="1:10">
       <c r="A3" s="1">
         <v>2966</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E3" s="1">
         <v>1</v>
@@ -1547,19 +1577,22 @@
       <c r="I3" s="4">
         <v>45826</v>
       </c>
-    </row>
-    <row r="4" s="1" customFormat="1" ht="51" spans="1:9">
+      <c r="J3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" s="1" customFormat="1" ht="51" spans="1:10">
       <c r="A4" s="1">
         <v>2294</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="E4" s="1">
         <v>1</v>
@@ -1576,19 +1609,22 @@
       <c r="I4" s="4">
         <v>45827</v>
       </c>
-    </row>
-    <row r="5" s="1" customFormat="1" ht="51" spans="1:9">
+      <c r="J4" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" s="1" customFormat="1" ht="51" spans="1:10">
       <c r="A5" s="1">
         <v>3443</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E5" s="1">
         <v>0</v>
@@ -1605,19 +1641,22 @@
       <c r="I5" s="4">
         <v>45828</v>
       </c>
-    </row>
-    <row r="6" s="1" customFormat="1" ht="51" spans="1:9">
+      <c r="J5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" s="1" customFormat="1" ht="51" spans="1:10">
       <c r="A6" s="1">
         <v>3085</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E6" s="1">
         <v>0</v>
@@ -1634,19 +1673,22 @@
       <c r="I6" s="4">
         <v>45829</v>
       </c>
-    </row>
-    <row r="7" s="1" customFormat="1" ht="51" spans="1:9">
+      <c r="J6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" s="1" customFormat="1" ht="51" spans="1:10">
       <c r="A7" s="1">
         <v>2081</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E7" s="1">
         <v>0</v>
@@ -1663,16 +1705,19 @@
       <c r="I7" s="4">
         <v>45831</v>
       </c>
-    </row>
-    <row r="8" s="1" customFormat="1" ht="34" spans="1:9">
+      <c r="J7" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" s="1" customFormat="1" ht="34" spans="1:10">
       <c r="A8" s="1">
         <v>704</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -1692,19 +1737,22 @@
       <c r="I8" s="4">
         <v>45831</v>
       </c>
-    </row>
-    <row r="9" s="1" customFormat="1" ht="51" spans="1:9">
+      <c r="J8" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" s="1" customFormat="1" ht="51" spans="1:10">
       <c r="A9" s="1">
         <v>34</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E9" s="1">
         <v>6</v>
@@ -1721,16 +1769,19 @@
       <c r="I9" s="4">
         <v>45835</v>
       </c>
-    </row>
-    <row r="10" s="1" customFormat="1" ht="34" spans="1:9">
+      <c r="J9" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" s="1" customFormat="1" ht="34" spans="1:10">
       <c r="A10" s="1">
         <v>2200</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>11</v>
@@ -1749,6 +1800,9 @@
       </c>
       <c r="I10" s="4">
         <v>45832</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="11" s="1" customFormat="1" ht="34" spans="1:9">
@@ -1756,13 +1810,13 @@
         <v>153</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E11" s="1">
         <v>6</v>
@@ -1780,18 +1834,18 @@
         <v>45832</v>
       </c>
     </row>
-    <row r="12" s="1" customFormat="1" ht="34" spans="1:9">
+    <row r="12" s="1" customFormat="1" ht="34" spans="1:10">
       <c r="A12" s="1">
         <v>154</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="D12" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E12" s="1">
         <v>1</v>
@@ -1807,6 +1861,9 @@
       </c>
       <c r="I12" s="4">
         <v>45832</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="13" s="1" customFormat="1" ht="34" spans="1:9">
@@ -1814,10 +1871,10 @@
         <v>278</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>11</v>
@@ -1838,18 +1895,18 @@
         <v>45832</v>
       </c>
     </row>
-    <row r="14" s="1" customFormat="1" ht="34" spans="1:9">
+    <row r="14" s="1" customFormat="1" ht="34" spans="1:10">
       <c r="A14" s="1">
         <v>658</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E14" s="1">
         <v>0</v>
@@ -1866,19 +1923,22 @@
       <c r="I14" s="4">
         <v>45832</v>
       </c>
-    </row>
-    <row r="15" s="1" customFormat="1" ht="34" spans="1:9">
+      <c r="J14" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" s="1" customFormat="1" ht="34" spans="1:10">
       <c r="A15" s="1">
         <v>2040</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E15" s="1">
         <v>0</v>
@@ -1894,6 +1954,9 @@
       </c>
       <c r="I15" s="4">
         <v>45833</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="16" s="1" customFormat="1" ht="51" spans="1:9">
@@ -1901,13 +1964,13 @@
         <v>2311</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E16" s="1">
         <v>1</v>
@@ -1925,18 +1988,18 @@
         <v>45834</v>
       </c>
     </row>
-    <row r="17" s="1" customFormat="1" ht="68" spans="1:9">
+    <row r="17" s="1" customFormat="1" ht="68" spans="1:10">
       <c r="A17" s="1">
         <v>2014</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E17" s="1">
         <v>0</v>
@@ -1953,19 +2016,22 @@
       <c r="I17" s="4">
         <v>45835</v>
       </c>
-    </row>
-    <row r="18" s="1" customFormat="1" ht="34" spans="1:9">
+      <c r="J17" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" s="1" customFormat="1" ht="34" spans="1:10">
       <c r="A18" s="1">
         <v>33</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E18" s="1">
         <v>3</v>
@@ -1981,6 +2047,9 @@
       </c>
       <c r="I18" s="4">
         <v>45835</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="19" s="1" customFormat="1" ht="34" spans="1:9">
@@ -1988,13 +2057,13 @@
         <v>81</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E19" s="1">
         <v>2</v>
@@ -2017,10 +2086,10 @@
         <v>2099</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>11</v>
@@ -2041,18 +2110,18 @@
         <v>45836</v>
       </c>
     </row>
-    <row r="21" s="1" customFormat="1" ht="51" spans="1:9">
+    <row r="21" s="1" customFormat="1" ht="51" spans="1:10">
       <c r="A21" s="1">
         <v>1498</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E21" s="1">
         <v>0</v>
@@ -2068,6 +2137,9 @@
       </c>
       <c r="I21" s="4">
         <v>45837</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="22" s="1" customFormat="1" ht="68" spans="1:9">
@@ -2075,10 +2147,10 @@
         <v>594</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>11</v>
@@ -2099,18 +2171,18 @@
         <v>45838</v>
       </c>
     </row>
-    <row r="23" s="1" customFormat="1" ht="51" spans="1:9">
+    <row r="23" s="1" customFormat="1" ht="51" spans="1:10">
       <c r="A23" s="1">
         <v>4</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E23" s="1">
         <v>1</v>
@@ -2127,19 +2199,22 @@
       <c r="I23" s="4">
         <v>45838</v>
       </c>
-    </row>
-    <row r="24" s="1" customFormat="1" ht="51" spans="1:9">
+      <c r="J23" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" s="1" customFormat="1" ht="51" spans="1:10">
       <c r="A24" s="1">
         <v>74</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E24" s="1">
         <v>4</v>
@@ -2155,6 +2230,9 @@
       </c>
       <c r="I24" s="4">
         <v>45838</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="25" s="1" customFormat="1" ht="34" spans="1:9">
@@ -2162,13 +2240,13 @@
         <v>162</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E25" s="1">
         <v>3</v>
@@ -2191,13 +2269,13 @@
         <v>852</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E26" s="1">
         <v>3</v>
@@ -2220,13 +2298,13 @@
         <v>875</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E27" s="1">
         <v>3</v>
@@ -2249,13 +2327,13 @@
         <v>1283</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="D28" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E28" s="1">
         <v>3</v>
@@ -2278,10 +2356,10 @@
         <v>69</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>11</v>
@@ -2307,10 +2385,10 @@
         <v>1323</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>11</v>
@@ -2331,18 +2409,18 @@
         <v>45838</v>
       </c>
     </row>
-    <row r="31" s="1" customFormat="1" ht="51" spans="1:9">
+    <row r="31" s="1" customFormat="1" ht="51" spans="1:10">
       <c r="A31" s="1">
         <v>912</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E31" s="1">
         <v>2</v>
@@ -2358,6 +2436,9 @@
       </c>
       <c r="I31" s="4">
         <v>45838</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="32" s="1" customFormat="1" ht="34" spans="1:9">
@@ -2365,10 +2446,10 @@
         <v>3330</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>11</v>
@@ -2389,18 +2470,18 @@
         <v>45839</v>
       </c>
     </row>
-    <row r="33" s="1" customFormat="1" ht="68" spans="1:9">
+    <row r="33" s="1" customFormat="1" ht="68" spans="1:10">
       <c r="A33" s="1">
         <v>333</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E33" s="1">
         <v>0</v>
@@ -2417,19 +2498,22 @@
       <c r="I33" s="4">
         <v>45839</v>
       </c>
-    </row>
-    <row r="34" s="1" customFormat="1" ht="51" spans="1:9">
+      <c r="J33" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" s="1" customFormat="1" ht="51" spans="1:10">
       <c r="A34" s="1">
         <v>302</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E34" s="1">
         <v>1</v>
@@ -2446,19 +2530,22 @@
       <c r="I34" s="4">
         <v>45839</v>
       </c>
-    </row>
-    <row r="35" s="1" customFormat="1" ht="34" spans="1:9">
+      <c r="J34" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" s="1" customFormat="1" ht="34" spans="1:10">
       <c r="A35" s="1">
         <v>702</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E35" s="1">
         <v>2</v>
@@ -2474,6 +2561,9 @@
       </c>
       <c r="I35" s="4">
         <v>45839</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="36" s="1" customFormat="1" ht="51" spans="1:9">
@@ -2481,13 +2571,13 @@
         <v>75</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E36" s="1">
         <v>3</v>
@@ -2510,10 +2600,10 @@
         <v>26</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>11</v>
@@ -2539,13 +2629,13 @@
         <v>3333</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E38" s="1">
         <v>0</v>
@@ -2563,7 +2653,7 @@
         <v>45840</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="39" s="1" customFormat="1" ht="34" spans="1:9">
@@ -2571,13 +2661,13 @@
         <v>80</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E39" s="1">
         <v>3</v>
@@ -2600,10 +2690,10 @@
         <v>88</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>11</v>
@@ -2622,6 +2712,128 @@
       </c>
       <c r="I40" s="4">
         <v>45840</v>
+      </c>
+    </row>
+    <row r="41" ht="34" spans="1:9">
+      <c r="A41" s="1">
+        <v>283</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E41" s="1">
+        <v>3</v>
+      </c>
+      <c r="F41" s="1">
+        <v>0</v>
+      </c>
+      <c r="G41" s="1">
+        <v>7</v>
+      </c>
+      <c r="H41" s="4">
+        <v>45840</v>
+      </c>
+      <c r="I41" s="4">
+        <v>45840</v>
+      </c>
+    </row>
+    <row r="42" ht="68" spans="1:10">
+      <c r="A42" s="1">
+        <v>215</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E42" s="1">
+        <v>2</v>
+      </c>
+      <c r="F42" s="1">
+        <v>1</v>
+      </c>
+      <c r="G42" s="1">
+        <v>16</v>
+      </c>
+      <c r="H42" s="4">
+        <v>45840</v>
+      </c>
+      <c r="I42" s="4">
+        <v>45840</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="43" ht="51" spans="1:10">
+      <c r="A43" s="1">
+        <v>347</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E43" s="1">
+        <v>1</v>
+      </c>
+      <c r="F43" s="1">
+        <v>3</v>
+      </c>
+      <c r="G43" s="1">
+        <v>10</v>
+      </c>
+      <c r="H43" s="4">
+        <v>45840</v>
+      </c>
+      <c r="I43" s="4">
+        <v>45840</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="44" ht="68" spans="1:9">
+      <c r="A44" s="1">
+        <v>3304</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E44" s="1">
+        <v>0</v>
+      </c>
+      <c r="F44" s="1">
+        <v>1</v>
+      </c>
+      <c r="G44" s="1">
+        <v>20</v>
+      </c>
+      <c r="H44" s="4">
+        <v>45841</v>
+      </c>
+      <c r="I44" s="4">
+        <v>45841</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove markdown file for LeetCode problem 349: Intersection of Two Arrays, update workspace configuration to reflect changes, and add new markdown files for problems 42: Trapping Rain Water, 350: Intersection of Two Arrays II, and 845: Longest Mountain in Array.
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="100">
   <si>
     <t>#</t>
   </si>
@@ -312,6 +312,21 @@
   </si>
   <si>
     <t>#math #bit-minipulation #recursive #simulation</t>
+  </si>
+  <si>
+    <t>Intersection of Two Arrays</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#hash-table #array #two-pointers #核心 </t>
+  </si>
+  <si>
+    <t>Intersection of Two Arrays II</t>
+  </si>
+  <si>
+    <t>Longest Mountain in Array</t>
+  </si>
+  <si>
+    <t>Trapping Rain Water</t>
   </si>
 </sst>
 </file>
@@ -1468,10 +1483,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J44"/>
+  <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="162" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="I44" sqref="I44"/>
+    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="162" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -2807,7 +2822,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="44" ht="68" spans="1:9">
+    <row r="44" ht="68" spans="1:10">
       <c r="A44" s="1">
         <v>3304</v>
       </c>
@@ -2834,6 +2849,128 @@
       </c>
       <c r="I44" s="4">
         <v>45841</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45" ht="51" spans="1:9">
+      <c r="A45" s="1">
+        <v>349</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E45" s="1">
+        <v>4</v>
+      </c>
+      <c r="F45" s="1">
+        <v>0</v>
+      </c>
+      <c r="G45" s="1">
+        <v>5</v>
+      </c>
+      <c r="H45" s="4">
+        <v>45841</v>
+      </c>
+      <c r="I45" s="4">
+        <v>45841</v>
+      </c>
+    </row>
+    <row r="46" ht="51" spans="1:9">
+      <c r="A46" s="1">
+        <v>350</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E46" s="1">
+        <v>4</v>
+      </c>
+      <c r="F46" s="1">
+        <v>0</v>
+      </c>
+      <c r="G46" s="1">
+        <v>5</v>
+      </c>
+      <c r="H46" s="4">
+        <v>45841</v>
+      </c>
+      <c r="I46" s="4">
+        <v>45841</v>
+      </c>
+    </row>
+    <row r="47" ht="34" spans="1:9">
+      <c r="A47" s="1">
+        <v>845</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E47" s="1">
+        <v>2</v>
+      </c>
+      <c r="F47" s="1">
+        <v>2</v>
+      </c>
+      <c r="G47" s="1">
+        <v>20</v>
+      </c>
+      <c r="H47" s="4">
+        <v>45841</v>
+      </c>
+      <c r="I47" s="4">
+        <v>45841</v>
+      </c>
+    </row>
+    <row r="48" ht="34" spans="1:10">
+      <c r="A48" s="1">
+        <v>42</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E48" s="1">
+        <v>1</v>
+      </c>
+      <c r="F48" s="1">
+        <v>3</v>
+      </c>
+      <c r="G48" s="1">
+        <v>20</v>
+      </c>
+      <c r="H48" s="4">
+        <v>45841</v>
+      </c>
+      <c r="I48" s="4">
+        <v>45841</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update workspace configuration: Replace references to problem 6 with problem 43 in the workspace file, add new markdown files for problems 43: Multiply Strings, 969: Pancake Sorting, and 3307: Find the K-th Character in String Game II, and update markdown for problem 42: Trapping Rain Water with complexity analysis.
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="106">
   <si>
     <t>#</t>
   </si>
@@ -327,6 +327,24 @@
   </si>
   <si>
     <t>Trapping Rain Water</t>
+  </si>
+  <si>
+    <t>Multiply Strings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#math #string #simulation #核心 </t>
+  </si>
+  <si>
+    <t>Pancake Sorting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#array #two-pointers #greedy #sorting #重点 </t>
+  </si>
+  <si>
+    <t>Find the K-th Character in String Game II</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#math #bit-minipulation </t>
   </si>
 </sst>
 </file>
@@ -1483,10 +1501,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J48"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="162" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="I48" sqref="I48"/>
+      <selection activeCell="J50" sqref="J50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -2973,6 +2991,99 @@
         <v>12</v>
       </c>
     </row>
+    <row r="49" ht="34" spans="1:10">
+      <c r="A49" s="1">
+        <v>43</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E49" s="1">
+        <v>2</v>
+      </c>
+      <c r="F49" s="1">
+        <v>2</v>
+      </c>
+      <c r="G49" s="1">
+        <v>30</v>
+      </c>
+      <c r="H49" s="4">
+        <v>45841</v>
+      </c>
+      <c r="I49" s="4">
+        <v>45841</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="50" ht="51" spans="1:10">
+      <c r="A50" s="1">
+        <v>969</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E50" s="1">
+        <v>2</v>
+      </c>
+      <c r="F50" s="1">
+        <v>2</v>
+      </c>
+      <c r="G50" s="1">
+        <v>25</v>
+      </c>
+      <c r="H50" s="4">
+        <v>45841</v>
+      </c>
+      <c r="I50" s="4">
+        <v>45841</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="51" ht="34" spans="1:9">
+      <c r="A51" s="1">
+        <v>3307</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E51" s="1">
+        <v>1</v>
+      </c>
+      <c r="F51" s="1">
+        <v>0</v>
+      </c>
+      <c r="G51" s="1">
+        <v>24</v>
+      </c>
+      <c r="H51" s="4">
+        <v>45842</v>
+      </c>
+      <c r="I51" s="4">
+        <v>45842</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Update workspace configuration: Replace references to problem 21 with problem 141 and add new markdown files for problems 141: Linked List Cycle and 86: Partition List, including their respective solutions and complexity analyses.
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="112">
   <si>
     <t>#</t>
   </si>
@@ -345,6 +345,24 @@
   </si>
   <si>
     <t xml:space="preserve">#math #bit-minipulation </t>
+  </si>
+  <si>
+    <t>Merge Two Sorted Lists</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#linked-list #必背 </t>
+  </si>
+  <si>
+    <t>New 21 Game</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#dynamic-programming #sliding-window </t>
+  </si>
+  <si>
+    <t>Partition List</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#linked-list #two-pointers #核心 </t>
   </si>
 </sst>
 </file>
@@ -1501,10 +1519,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J51"/>
+  <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="162" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="J50" sqref="J50"/>
+    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="162" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="I54" sqref="I54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -3084,6 +3102,102 @@
         <v>45842</v>
       </c>
     </row>
+    <row r="52" ht="17" spans="1:10">
+      <c r="A52" s="1">
+        <v>21</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E52" s="1">
+        <v>3</v>
+      </c>
+      <c r="F52" s="1">
+        <v>2</v>
+      </c>
+      <c r="G52" s="1">
+        <v>20</v>
+      </c>
+      <c r="H52" s="4">
+        <v>45842</v>
+      </c>
+      <c r="I52" s="4">
+        <v>45842</v>
+      </c>
+      <c r="J52" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="53" ht="51" spans="1:10">
+      <c r="A53" s="1">
+        <v>837</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E53" s="1">
+        <v>0</v>
+      </c>
+      <c r="F53" s="1">
+        <v>1</v>
+      </c>
+      <c r="G53" s="1">
+        <v>50</v>
+      </c>
+      <c r="H53" s="4">
+        <v>45842</v>
+      </c>
+      <c r="I53" s="4">
+        <v>45842</v>
+      </c>
+      <c r="J53" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="54" ht="34" spans="1:10">
+      <c r="A54" s="1">
+        <v>86</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E54" s="1">
+        <v>2</v>
+      </c>
+      <c r="F54" s="1">
+        <v>2</v>
+      </c>
+      <c r="G54" s="1">
+        <v>61</v>
+      </c>
+      <c r="H54" s="4">
+        <v>45842</v>
+      </c>
+      <c r="I54" s="4">
+        <v>45842</v>
+      </c>
+      <c r="J54" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Remove markdown file for LeetCode problem 160: Intersection of Two Linked Lists and update workspace configuration to reflect changes. Add new markdown files for problems 328: Odd Even Linked List, 1394: Find Lucky Integer in an Array, and 1865: Finding Pairs With a Certain Sum, including problem descriptions, examples, and complexity analyses.
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="16760"/>
+    <workbookView windowHeight="16740"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="123">
   <si>
     <t>#</t>
   </si>
@@ -363,6 +363,39 @@
   </si>
   <si>
     <t xml:space="preserve">#linked-list #two-pointers #核心 </t>
+  </si>
+  <si>
+    <t>Linked List Cycle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#linked-list #two-pointers #必背 </t>
+  </si>
+  <si>
+    <t>Intersection of Two Linked Lists</t>
+  </si>
+  <si>
+    <t>Palindrome Linked List</t>
+  </si>
+  <si>
+    <t>Find Lucky Integer in an Array</t>
+  </si>
+  <si>
+    <t>Finding Pairs With a Certain Sum</t>
+  </si>
+  <si>
+    <t>#array #hash-table #design</t>
+  </si>
+  <si>
+    <t>Maximum Number of Events That Can Be Attended</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#array #greedy #sorting #heap </t>
+  </si>
+  <si>
+    <t>Odd Even Linked List</t>
+  </si>
+  <si>
+    <t>#linked-list</t>
   </si>
 </sst>
 </file>
@@ -1519,10 +1552,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J54"/>
+  <dimension ref="A1:J61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="162" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="I54" sqref="I54"/>
+    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="162" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="J61" sqref="J61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -3198,6 +3231,215 @@
         <v>12</v>
       </c>
     </row>
+    <row r="55" ht="34" spans="1:10">
+      <c r="A55" s="1">
+        <v>141</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E55" s="1">
+        <v>2</v>
+      </c>
+      <c r="F55" s="1">
+        <v>3</v>
+      </c>
+      <c r="G55" s="1">
+        <v>20</v>
+      </c>
+      <c r="H55" s="4">
+        <v>45842</v>
+      </c>
+      <c r="I55" s="4">
+        <v>45842</v>
+      </c>
+      <c r="J55" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="56" ht="34" spans="1:9">
+      <c r="A56" s="1">
+        <v>160</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E56" s="1">
+        <v>3</v>
+      </c>
+      <c r="F56" s="1">
+        <v>2</v>
+      </c>
+      <c r="G56" s="1">
+        <v>10</v>
+      </c>
+      <c r="H56" s="4">
+        <v>45842</v>
+      </c>
+      <c r="I56" s="4">
+        <v>45842</v>
+      </c>
+    </row>
+    <row r="57" ht="34" spans="1:10">
+      <c r="A57" s="1">
+        <v>234</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E57" s="1">
+        <v>3</v>
+      </c>
+      <c r="F57" s="1">
+        <v>2</v>
+      </c>
+      <c r="G57" s="1">
+        <v>20</v>
+      </c>
+      <c r="H57" s="4">
+        <v>45842</v>
+      </c>
+      <c r="I57" s="4">
+        <v>45842</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="58" ht="34" spans="1:9">
+      <c r="A58" s="1">
+        <v>1394</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E58" s="1">
+        <v>1</v>
+      </c>
+      <c r="F58" s="1">
+        <v>0</v>
+      </c>
+      <c r="G58" s="1">
+        <v>5</v>
+      </c>
+      <c r="H58" s="4">
+        <v>45843</v>
+      </c>
+      <c r="I58" s="4">
+        <v>45843</v>
+      </c>
+    </row>
+    <row r="59" ht="34" spans="1:9">
+      <c r="A59" s="1">
+        <v>1865</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E59" s="1">
+        <v>1</v>
+      </c>
+      <c r="F59" s="1">
+        <v>0</v>
+      </c>
+      <c r="G59" s="1">
+        <v>24</v>
+      </c>
+      <c r="H59" s="4">
+        <v>45844</v>
+      </c>
+      <c r="I59" s="4">
+        <v>45844</v>
+      </c>
+    </row>
+    <row r="60" ht="51" spans="1:9">
+      <c r="A60" s="1">
+        <v>1353</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E60" s="1">
+        <v>0</v>
+      </c>
+      <c r="F60" s="1">
+        <v>1</v>
+      </c>
+      <c r="G60" s="1">
+        <v>28</v>
+      </c>
+      <c r="H60" s="4">
+        <v>45845</v>
+      </c>
+      <c r="I60" s="4">
+        <v>45845</v>
+      </c>
+    </row>
+    <row r="61" ht="17" spans="1:10">
+      <c r="A61" s="1">
+        <v>328</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E61" s="1">
+        <v>1</v>
+      </c>
+      <c r="F61" s="1">
+        <v>0</v>
+      </c>
+      <c r="G61" s="1">
+        <v>20</v>
+      </c>
+      <c r="H61" s="4">
+        <v>45845</v>
+      </c>
+      <c r="I61" s="4">
+        <v>45845</v>
+      </c>
+      <c r="J61" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Add markdown file for LeetCode problem 287: Find the Duplicate Number, including problem description, examples, and constraints. Update workspace configuration to include the new file and adjust references for problem 142: Linked List Cycle II.
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="16740"/>
+    <workbookView windowWidth="26860" windowHeight="14540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="125">
   <si>
     <t>#</t>
   </si>
@@ -396,6 +396,12 @@
   </si>
   <si>
     <t>#linked-list</t>
+  </si>
+  <si>
+    <t>Find the Duplicate Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#array #two-pointers #重点 </t>
   </si>
 </sst>
 </file>
@@ -1552,10 +1558,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J61"/>
+  <dimension ref="A1:J62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="162" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="J61" sqref="J61"/>
+      <selection activeCell="J62" sqref="J62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -3440,6 +3446,35 @@
         <v>12</v>
       </c>
     </row>
+    <row r="62" ht="34" spans="1:9">
+      <c r="A62" s="1">
+        <v>287</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E62" s="1">
+        <v>0</v>
+      </c>
+      <c r="F62" s="1">
+        <v>3</v>
+      </c>
+      <c r="G62" s="1">
+        <v>20</v>
+      </c>
+      <c r="H62" s="4">
+        <v>45846</v>
+      </c>
+      <c r="I62" s="4">
+        <v>45846</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Add markdown files for LeetCode problems 56: Merge Intervals and 876: Middle of the Linked List, including problem descriptions, examples, and constraints. Update workspace configuration to include the new files and adjust references accordingly.
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="128">
   <si>
     <t>#</t>
   </si>
@@ -402,6 +402,15 @@
   </si>
   <si>
     <t xml:space="preserve">#array #two-pointers #重点 </t>
+  </si>
+  <si>
+    <t>Middle of the Linked List</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#linked-list #two-pointers #重点 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">#array #sorting #核心 </t>
   </si>
 </sst>
 </file>
@@ -1558,10 +1567,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J62"/>
+  <dimension ref="A1:J64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="162" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="J62" sqref="J62"/>
+    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="162" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -3475,6 +3484,40 @@
         <v>45846</v>
       </c>
     </row>
+    <row r="63" ht="34" spans="1:9">
+      <c r="A63" s="1">
+        <v>876</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E63" s="1">
+        <v>0</v>
+      </c>
+      <c r="F63" s="1">
+        <v>3</v>
+      </c>
+      <c r="G63" s="1">
+        <v>1</v>
+      </c>
+      <c r="H63" s="4">
+        <v>45846</v>
+      </c>
+      <c r="I63" s="4">
+        <v>45846</v>
+      </c>
+    </row>
+    <row r="64" ht="34" spans="3:3">
+      <c r="C64" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Add markdown file for LeetCode problem 3439: Reschedule Meetings for Maximum Free Time I, including problem description, examples, and constraints. Update workspace configuration to include the new file and adjust references accordingly.
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="26860" windowHeight="14540"/>
+    <workbookView windowWidth="26860" windowHeight="14520"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="131">
   <si>
     <t>#</t>
   </si>
@@ -410,7 +410,16 @@
     <t xml:space="preserve">#linked-list #two-pointers #重点 </t>
   </si>
   <si>
+    <t>Merge Intervals</t>
+  </si>
+  <si>
     <t xml:space="preserve">#array #sorting #核心 </t>
+  </si>
+  <si>
+    <t>Reschedule Meetings for Maximum Free Time I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#array #greedy #sliding-window </t>
   </si>
 </sst>
 </file>
@@ -1567,10 +1576,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J64"/>
+  <dimension ref="A1:J65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="162" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="162" topLeftCell="C60" workbookViewId="0">
+      <selection activeCell="J65" sqref="J65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -3513,9 +3522,65 @@
         <v>45846</v>
       </c>
     </row>
-    <row r="64" ht="34" spans="3:3">
+    <row r="64" ht="34" spans="1:9">
+      <c r="A64" s="1">
+        <v>56</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>127</v>
+      </c>
       <c r="C64" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E64" s="1">
+        <v>4</v>
+      </c>
+      <c r="F64" s="1">
+        <v>0</v>
+      </c>
+      <c r="G64" s="1">
+        <v>5</v>
+      </c>
+      <c r="H64" s="4">
+        <v>45846</v>
+      </c>
+      <c r="I64" s="4">
+        <v>45846</v>
+      </c>
+    </row>
+    <row r="65" ht="34" spans="1:10">
+      <c r="A65" s="1">
+        <v>3439</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E65" s="1">
+        <v>0</v>
+      </c>
+      <c r="F65" s="1">
+        <v>1</v>
+      </c>
+      <c r="G65" s="1">
+        <v>45</v>
+      </c>
+      <c r="H65" s="4">
+        <v>45847</v>
+      </c>
+      <c r="I65" s="4">
+        <v>45847</v>
+      </c>
+      <c r="J65" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add markdown file for LeetCode problem 57: Insert Interval, including problem description, examples, and constraints. Update workspace configuration to include the new file and adjust references accordingly.
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="26860" windowHeight="14520"/>
+    <workbookView windowWidth="29100" windowHeight="14520"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="133">
   <si>
     <t>#</t>
   </si>
@@ -420,6 +420,12 @@
   </si>
   <si>
     <t xml:space="preserve">#array #greedy #sliding-window </t>
+  </si>
+  <si>
+    <t>Insert Interval</t>
+  </si>
+  <si>
+    <t>#array</t>
   </si>
 </sst>
 </file>
@@ -1576,10 +1582,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J65"/>
+  <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="162" topLeftCell="C60" workbookViewId="0">
-      <selection activeCell="J65" sqref="J65"/>
+    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="162" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="H66" sqref="H66:I66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -3583,6 +3589,35 @@
         <v>12</v>
       </c>
     </row>
+    <row r="66" ht="17" spans="1:9">
+      <c r="A66" s="1">
+        <v>57</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E66" s="1">
+        <v>0</v>
+      </c>
+      <c r="F66" s="1">
+        <v>3</v>
+      </c>
+      <c r="G66" s="1">
+        <v>50</v>
+      </c>
+      <c r="H66" s="4">
+        <v>45847</v>
+      </c>
+      <c r="I66" s="4">
+        <v>45847</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Update markdown for LeetCode problem 57: Insert Interval to include additional tags. Add new markdown file for LeetCode problem 252: Meeting Rooms with problem description, examples, and constraints. Update workspace configuration to include the new file and adjust references accordingly.
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="134">
   <si>
     <t>#</t>
   </si>
@@ -425,7 +425,10 @@
     <t>Insert Interval</t>
   </si>
   <si>
-    <t>#array</t>
+    <t>#array #核心</t>
+  </si>
+  <si>
+    <t>Meeting Rooms</t>
   </si>
 </sst>
 </file>
@@ -1582,10 +1585,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J66"/>
+  <dimension ref="A1:J67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="162" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="H66" sqref="H66:I66"/>
+      <selection activeCell="H67" sqref="H67:I67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -3618,6 +3621,35 @@
         <v>45847</v>
       </c>
     </row>
+    <row r="67" ht="34" spans="1:9">
+      <c r="A67" s="1">
+        <v>252</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E67" s="1">
+        <v>5</v>
+      </c>
+      <c r="F67" s="1">
+        <v>0</v>
+      </c>
+      <c r="G67" s="1">
+        <v>5</v>
+      </c>
+      <c r="H67" s="4">
+        <v>45847</v>
+      </c>
+      <c r="I67" s="4">
+        <v>45847</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Add markdown file for LeetCode problem 253: Meeting Rooms II, including problem description, examples, and constraints. Update workspace configuration to include the new file and adjust references accordingly.
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="136">
   <si>
     <t>#</t>
   </si>
@@ -429,6 +429,12 @@
   </si>
   <si>
     <t>Meeting Rooms</t>
+  </si>
+  <si>
+    <t>Meeting Rooms II</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#greedy #sorting #heap #核心 </t>
   </si>
 </sst>
 </file>
@@ -1585,10 +1591,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J67"/>
+  <dimension ref="A1:J68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="162" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="H67" sqref="H67:I67"/>
+      <selection activeCell="H68" sqref="H68:I68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -3650,6 +3656,35 @@
         <v>45847</v>
       </c>
     </row>
+    <row r="68" ht="34" spans="1:9">
+      <c r="A68" s="1">
+        <v>253</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E68" s="1">
+        <v>4</v>
+      </c>
+      <c r="F68" s="1">
+        <v>1</v>
+      </c>
+      <c r="G68" s="1">
+        <v>18</v>
+      </c>
+      <c r="H68" s="4">
+        <v>45847</v>
+      </c>
+      <c r="I68" s="4">
+        <v>45847</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
更新工作区配置，替换旧文件 76. Minimum Window Substring 为新文件 3201. Find the Maximum Length of Valid Subsequence I，并新增 Markdown 文件 209. Minimum Size Subarray Sum，包含问题描述、示例及解决方案。
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="167">
   <si>
     <t>#</t>
   </si>
@@ -516,6 +516,18 @@
   </si>
   <si>
     <t xml:space="preserve">#hash-table #two-pointers #string #sliding-window #核心 </t>
+  </si>
+  <si>
+    <t>Find the Maximum Length of Valid Subsequence I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#array #dynamic-programming </t>
+  </si>
+  <si>
+    <t>Minimum Size Subarray Sum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#two-pointers #sliding-window #核心 </t>
   </si>
 </sst>
 </file>
@@ -1672,10 +1684,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J83"/>
+  <dimension ref="A1:J85"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="162" topLeftCell="B78" workbookViewId="0">
-      <selection activeCell="J82" sqref="J82"/>
+    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="162" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="G85" sqref="G85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -4197,6 +4209,67 @@
         <v>12</v>
       </c>
     </row>
+    <row r="84" ht="51" spans="1:10">
+      <c r="A84" s="1">
+        <v>3201</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E84" s="1">
+        <v>0</v>
+      </c>
+      <c r="F84" s="1">
+        <v>1</v>
+      </c>
+      <c r="G84" s="1">
+        <v>50</v>
+      </c>
+      <c r="H84" s="4">
+        <v>45854</v>
+      </c>
+      <c r="I84" s="4">
+        <v>45854</v>
+      </c>
+      <c r="J84" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="85" ht="51" spans="1:9">
+      <c r="A85" s="1">
+        <v>209</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E85" s="1">
+        <v>2</v>
+      </c>
+      <c r="F85" s="1">
+        <v>0</v>
+      </c>
+      <c r="G85" s="1">
+        <v>30</v>
+      </c>
+      <c r="H85" s="4">
+        <v>44366</v>
+      </c>
+      <c r="I85" s="4">
+        <v>45854</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Update workspace configuration and add new Markdown files for LeetCode problems 1967, 465, and 2163, including problem descriptions, examples, constraints, and solutions. Replace existing entries in the workspace with the new files.
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="174">
   <si>
     <t>#</t>
   </si>
@@ -540,6 +540,15 @@
   </si>
   <si>
     <t>???</t>
+  </si>
+  <si>
+    <t>Delete Characters to Make Fancy String</t>
+  </si>
+  <si>
+    <t>Optimal Account Balancing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#array #backtracking #dynamic-programming </t>
   </si>
 </sst>
 </file>
@@ -1696,10 +1705,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J87"/>
+  <dimension ref="A1:J89"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="162" topLeftCell="B84" workbookViewId="0">
-      <selection activeCell="I91" sqref="I91"/>
+    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="162" topLeftCell="B86" workbookViewId="0">
+      <selection activeCell="H90" sqref="H90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -4346,6 +4355,67 @@
         <v>170</v>
       </c>
     </row>
+    <row r="88" ht="34" spans="1:9">
+      <c r="A88" s="1">
+        <v>1967</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E88" s="1">
+        <v>1</v>
+      </c>
+      <c r="F88" s="1">
+        <v>0</v>
+      </c>
+      <c r="G88" s="1">
+        <v>12</v>
+      </c>
+      <c r="H88" s="4">
+        <v>45859</v>
+      </c>
+      <c r="I88" s="4">
+        <v>45859</v>
+      </c>
+    </row>
+    <row r="89" ht="68" spans="1:10">
+      <c r="A89" s="1">
+        <v>465</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E89" s="1">
+        <v>0</v>
+      </c>
+      <c r="F89" s="1">
+        <v>1</v>
+      </c>
+      <c r="G89" s="1">
+        <v>90</v>
+      </c>
+      <c r="H89" s="4">
+        <v>45859</v>
+      </c>
+      <c r="I89" s="4">
+        <v>45859</v>
+      </c>
+      <c r="J89" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Update workspace configuration and add Markdown files for LeetCode problems 1717 and 146, including problem descriptions and solutions.
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="29100" windowHeight="14540"/>
+    <workbookView windowWidth="26860" windowHeight="14540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="179">
   <si>
     <t>#</t>
   </si>
@@ -558,6 +558,12 @@
   </si>
   <si>
     <t>LRU Cache</t>
+  </si>
+  <si>
+    <t>Maximum Score From Removing Substrings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#string #stack #greedy </t>
   </si>
 </sst>
 </file>
@@ -1714,10 +1720,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J91"/>
+  <dimension ref="A1:J92"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="162" topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="H91" sqref="H91:I91"/>
+      <selection activeCell="H91" sqref="H91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -4473,11 +4479,38 @@
       <c r="G91" s="1">
         <v>10</v>
       </c>
-      <c r="H91" s="4">
-        <v>45860</v>
-      </c>
+      <c r="H91" s="4"/>
       <c r="I91" s="4">
         <v>45860</v>
+      </c>
+    </row>
+    <row r="92" ht="34" spans="1:9">
+      <c r="A92" s="1">
+        <v>1717</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E92" s="1">
+        <v>0</v>
+      </c>
+      <c r="F92" s="1">
+        <v>1</v>
+      </c>
+      <c r="G92" s="1">
+        <v>30</v>
+      </c>
+      <c r="H92" s="4">
+        <v>45861</v>
+      </c>
+      <c r="I92" s="4">
+        <v>45861</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update workspace configuration and add Markdown files for LeetCode problems 621 and 233, including problem descriptions and solutions.
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="26860" windowHeight="14540"/>
+    <workbookView windowWidth="29100" windowHeight="14540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="187">
   <si>
     <t>#</t>
   </si>
@@ -564,6 +564,30 @@
   </si>
   <si>
     <t xml:space="preserve">#string #stack #greedy </t>
+  </si>
+  <si>
+    <t>Maximum Subarray</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#array #divide-and-conquer #dynamic-programming </t>
+  </si>
+  <si>
+    <t>Minimum Score After Removals on a Tree</t>
+  </si>
+  <si>
+    <t>#array #bit-manipulation #tree #dfs</t>
+  </si>
+  <si>
+    <t>Task Scheduler</t>
+  </si>
+  <si>
+    <t>#array #greedy #queue</t>
+  </si>
+  <si>
+    <t>Number of Digit One</t>
+  </si>
+  <si>
+    <t>#math</t>
   </si>
 </sst>
 </file>
@@ -1720,10 +1744,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J92"/>
+  <dimension ref="A1:J96"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="162" topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="H91" sqref="H91"/>
+    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="162" topLeftCell="B89" workbookViewId="0">
+      <selection activeCell="J95" sqref="J95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -4513,6 +4537,128 @@
         <v>45861</v>
       </c>
     </row>
+    <row r="93" ht="68" spans="1:9">
+      <c r="A93" s="1">
+        <v>53</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E93" s="1">
+        <v>1</v>
+      </c>
+      <c r="F93" s="1">
+        <v>1</v>
+      </c>
+      <c r="G93" s="1">
+        <v>20</v>
+      </c>
+      <c r="I93" s="4">
+        <v>45861</v>
+      </c>
+    </row>
+    <row r="94" ht="51" spans="1:10">
+      <c r="A94" s="1">
+        <v>2322</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E94" s="1">
+        <v>0</v>
+      </c>
+      <c r="F94" s="1">
+        <v>1</v>
+      </c>
+      <c r="G94" s="1">
+        <v>65</v>
+      </c>
+      <c r="H94" s="4">
+        <v>45862</v>
+      </c>
+      <c r="I94" s="4">
+        <v>45862</v>
+      </c>
+      <c r="J94" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="95" ht="34" spans="1:10">
+      <c r="A95" s="1">
+        <v>621</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E95" s="1">
+        <v>1</v>
+      </c>
+      <c r="F95" s="1">
+        <v>1</v>
+      </c>
+      <c r="G95" s="1">
+        <v>50</v>
+      </c>
+      <c r="H95" s="4">
+        <v>45862</v>
+      </c>
+      <c r="I95" s="4">
+        <v>45862</v>
+      </c>
+      <c r="J95" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="96" ht="17" spans="1:10">
+      <c r="A96" s="1">
+        <v>233</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E96" s="1">
+        <v>0</v>
+      </c>
+      <c r="F96" s="1">
+        <v>1</v>
+      </c>
+      <c r="G96" s="1">
+        <v>40</v>
+      </c>
+      <c r="H96" s="4">
+        <v>45863</v>
+      </c>
+      <c r="I96" s="4">
+        <v>45863</v>
+      </c>
+      <c r="J96" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
feat: update Python interview cheatsheet title and add new markdown files for LeetCode problems 206 and 3487 with examples and complexity analysis
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="191">
   <si>
     <t>#</t>
   </si>
@@ -588,6 +588,18 @@
   </si>
   <si>
     <t>#math</t>
+  </si>
+  <si>
+    <t>Reverse Linked List</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#linked-list #recursive </t>
+  </si>
+  <si>
+    <t>Maximum Unique Subarray Sum After Deletion</t>
+  </si>
+  <si>
+    <t>#array #set</t>
   </si>
 </sst>
 </file>
@@ -1744,10 +1756,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J96"/>
+  <dimension ref="A1:J98"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="162" topLeftCell="B89" workbookViewId="0">
-      <selection activeCell="J95" sqref="J95"/>
+    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="162" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="H98" sqref="H98:I98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -4659,6 +4671,64 @@
         <v>12</v>
       </c>
     </row>
+    <row r="97" ht="34" spans="1:9">
+      <c r="A97" s="1">
+        <v>206</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E97" s="1">
+        <v>2</v>
+      </c>
+      <c r="F97" s="1">
+        <v>1</v>
+      </c>
+      <c r="G97" s="1">
+        <v>5</v>
+      </c>
+      <c r="H97" s="4">
+        <v>45864</v>
+      </c>
+      <c r="I97" s="4">
+        <v>45864</v>
+      </c>
+    </row>
+    <row r="98" ht="51" spans="1:9">
+      <c r="A98" s="1">
+        <v>3487</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E98" s="1">
+        <v>1</v>
+      </c>
+      <c r="F98" s="1">
+        <v>0</v>
+      </c>
+      <c r="G98" s="1">
+        <v>10</v>
+      </c>
+      <c r="H98" s="4">
+        <v>45864</v>
+      </c>
+      <c r="I98" s="4">
+        <v>45864</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Add new problem notes and update workspace
- Added notes for "713. Subarray Product Less Than K" and "239. Sliding Window Maximum" in the Obsidian Vault.
- Updated workspace configuration to include new notes and set "713. Subarray Product Less Than K" as the active note.
- Modified the outline title for "713. Subarray Product Less Than K".
- Updated the last open files list to reflect recent changes.
- Improved formatting and structure in the Python interview cheatsheet HTML file, including new sections for advanced topics and quick tips.
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="193">
   <si>
     <t>#</t>
   </si>
@@ -593,13 +593,19 @@
     <t>Reverse Linked List</t>
   </si>
   <si>
-    <t xml:space="preserve">#linked-list #recursive </t>
+    <t>#linked-list #recursive #必背</t>
   </si>
   <si>
     <t>Maximum Unique Subarray Sum After Deletion</t>
   </si>
   <si>
     <t>#array #set</t>
+  </si>
+  <si>
+    <t>Sliding Window Maximum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#sliding-window #monotonic-queue #array #queue #核心 </t>
   </si>
 </sst>
 </file>
@@ -1756,10 +1762,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J98"/>
+  <dimension ref="A1:J99"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="162" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="H98" sqref="H98:I98"/>
+    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="162" topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="H99" sqref="H99:I99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -4729,6 +4735,35 @@
         <v>45864</v>
       </c>
     </row>
+    <row r="99" ht="68" spans="1:9">
+      <c r="A99" s="1">
+        <v>239</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E99" s="1">
+        <v>0</v>
+      </c>
+      <c r="F99" s="1">
+        <v>2</v>
+      </c>
+      <c r="G99" s="1">
+        <v>40</v>
+      </c>
+      <c r="H99" s="4">
+        <v>45864</v>
+      </c>
+      <c r="I99" s="4">
+        <v>45864</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Add solutions for LeetCode problems 2044, 2210, and 3480; update markdown files for problem descriptions and examples; implement sliding window and recursive approaches for optimal solutions.
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="205">
   <si>
     <t>#</t>
   </si>
@@ -606,6 +606,42 @@
   </si>
   <si>
     <t xml:space="preserve">#sliding-window #monotonic-queue #array #queue #核心 </t>
+  </si>
+  <si>
+    <t>Subarray Product Less Than K</t>
+  </si>
+  <si>
+    <t>#array #two-pointers #sliding-window #核心 #count-subarrays</t>
+  </si>
+  <si>
+    <t>template: slide window</t>
+  </si>
+  <si>
+    <t>Longest Substring with At Least K Repeating Characters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#hash-table #string #sliding-window #divide-and-conquer  #重点 </t>
+  </si>
+  <si>
+    <t>Maximize Subarrays After Removing One Conflicting Pair</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#array #segment-tree #enumeration #prefix-sum </t>
+  </si>
+  <si>
+    <t>Count Hills and Valleys in an Array</t>
+  </si>
+  <si>
+    <t>#array</t>
+  </si>
+  <si>
+    <t>ezsy</t>
+  </si>
+  <si>
+    <t>Count Number of Maximum Bitwise-OR Subsets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#memoization #backtracking #recursive #dynamic-programming </t>
   </si>
 </sst>
 </file>
@@ -1762,10 +1798,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J99"/>
+  <dimension ref="A1:J104"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="162" topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="H99" sqref="H99:I99"/>
+    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="162" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="B107" sqref="B107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -4569,7 +4605,7 @@
         <v>15</v>
       </c>
       <c r="E93" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F93" s="1">
         <v>1</v>
@@ -4577,8 +4613,11 @@
       <c r="G93" s="1">
         <v>20</v>
       </c>
+      <c r="H93" s="4">
+        <v>44371</v>
+      </c>
       <c r="I93" s="4">
-        <v>45861</v>
+        <v>45863</v>
       </c>
     </row>
     <row r="94" ht="51" spans="1:10">
@@ -4762,6 +4801,157 @@
       </c>
       <c r="I99" s="4">
         <v>45864</v>
+      </c>
+    </row>
+    <row r="100" ht="68" spans="1:10">
+      <c r="A100" s="1">
+        <v>713</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E100" s="1">
+        <v>0</v>
+      </c>
+      <c r="F100" s="1">
+        <v>2</v>
+      </c>
+      <c r="G100" s="1">
+        <v>50</v>
+      </c>
+      <c r="H100" s="4">
+        <v>45864</v>
+      </c>
+      <c r="I100" s="4">
+        <v>45864</v>
+      </c>
+      <c r="J100" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="101" ht="84" spans="1:10">
+      <c r="A101" s="1">
+        <v>395</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E101" s="1">
+        <v>0</v>
+      </c>
+      <c r="F101" s="1">
+        <v>1</v>
+      </c>
+      <c r="G101" s="1">
+        <v>40</v>
+      </c>
+      <c r="H101" s="4">
+        <v>45864</v>
+      </c>
+      <c r="I101" s="4">
+        <v>45864</v>
+      </c>
+      <c r="J101" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="102" ht="51" spans="1:9">
+      <c r="A102" s="1">
+        <v>3480</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E102" s="1">
+        <v>0</v>
+      </c>
+      <c r="F102" s="1">
+        <v>1</v>
+      </c>
+      <c r="G102" s="1">
+        <v>50</v>
+      </c>
+      <c r="H102" s="4">
+        <v>45865</v>
+      </c>
+      <c r="I102" s="4">
+        <v>45865</v>
+      </c>
+    </row>
+    <row r="103" ht="34" spans="1:9">
+      <c r="A103" s="1">
+        <v>2210</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="E103" s="1">
+        <v>1</v>
+      </c>
+      <c r="F103" s="1">
+        <v>0</v>
+      </c>
+      <c r="G103" s="1">
+        <v>10</v>
+      </c>
+      <c r="H103" s="4">
+        <v>45865</v>
+      </c>
+      <c r="I103" s="4">
+        <v>45865</v>
+      </c>
+    </row>
+    <row r="104" ht="84" spans="1:9">
+      <c r="A104" s="1">
+        <v>2044</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E104" s="1">
+        <v>0</v>
+      </c>
+      <c r="F104" s="1">
+        <v>1</v>
+      </c>
+      <c r="G104" s="1">
+        <v>45</v>
+      </c>
+      <c r="H104" s="4">
+        <v>45866</v>
+      </c>
+      <c r="I104" s="4">
+        <v>45866</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add solution and markdown for LeetCode problem 2483: Minimum Penalty for a Shop
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="29100" windowHeight="14540"/>
+    <workbookView windowHeight="16760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="207">
   <si>
     <t>#</t>
   </si>
@@ -642,6 +642,12 @@
   </si>
   <si>
     <t xml:space="preserve">#memoization #backtracking #recursive #dynamic-programming </t>
+  </si>
+  <si>
+    <t>Minimum Penalty for a Shop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#string </t>
   </si>
 </sst>
 </file>
@@ -1798,10 +1804,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J104"/>
+  <dimension ref="A1:J105"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="162" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="B107" sqref="B107"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="H105" sqref="H105:I105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -4954,6 +4960,35 @@
         <v>45866</v>
       </c>
     </row>
+    <row r="105" ht="34" spans="1:9">
+      <c r="A105" s="1">
+        <v>2483</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E105" s="1">
+        <v>1</v>
+      </c>
+      <c r="F105" s="1">
+        <v>0</v>
+      </c>
+      <c r="G105" s="1">
+        <v>18</v>
+      </c>
+      <c r="H105" s="4">
+        <v>45866</v>
+      </c>
+      <c r="I105" s="4">
+        <v>45866</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
feat: update workspace and add markdown files for LeetCode problems 238, 2483, and 480; reorganize notes for better structure
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="16760"/>
+    <workbookView windowWidth="29100" windowHeight="14540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="209">
   <si>
     <t>#</t>
   </si>
@@ -648,6 +648,12 @@
   </si>
   <si>
     <t xml:space="preserve">#string </t>
+  </si>
+  <si>
+    <t>Product of Array Except Self</t>
+  </si>
+  <si>
+    <t>#array #prefix-sum</t>
   </si>
 </sst>
 </file>
@@ -1804,10 +1810,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J105"/>
+  <dimension ref="A1:J106"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="H105" sqref="H105:I105"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" topLeftCell="A101" workbookViewId="0">
+      <selection activeCell="K106" sqref="K106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -4989,6 +4995,35 @@
         <v>45866</v>
       </c>
     </row>
+    <row r="106" ht="34" spans="1:9">
+      <c r="A106" s="1">
+        <v>238</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E106" s="1">
+        <v>2</v>
+      </c>
+      <c r="F106" s="1">
+        <v>0</v>
+      </c>
+      <c r="G106" s="1">
+        <v>14</v>
+      </c>
+      <c r="H106" s="4">
+        <v>45867</v>
+      </c>
+      <c r="I106" s="4">
+        <v>45867</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
feat: update workspace and add markdown files for LeetCode problems 270, 272, and 2411; reorganize notes for better structure
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="29100" windowHeight="14540"/>
+    <workbookView windowHeight="16760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="215">
   <si>
     <t>#</t>
   </si>
@@ -654,6 +654,24 @@
   </si>
   <si>
     <t>#array #prefix-sum</t>
+  </si>
+  <si>
+    <t>Smallest Subarrays With Maximum Bitwise OR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#array #bit-minipulation #sliding-window </t>
+  </si>
+  <si>
+    <t>Closest Binary Search Tree Value II</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#two-pointers #stack #tree #dfs #bst #heap #binary-tree </t>
+  </si>
+  <si>
+    <t>deque</t>
+  </si>
+  <si>
+    <t>Closest Binary Search Tree Value</t>
   </si>
 </sst>
 </file>
@@ -1810,10 +1828,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J106"/>
+  <dimension ref="A1:J109"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="K106" sqref="K106"/>
+    <sheetView tabSelected="1" zoomScale="172" zoomScaleNormal="172" topLeftCell="A104" workbookViewId="0">
+      <selection activeCell="H109" sqref="H109:I109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -5024,6 +5042,96 @@
         <v>45867</v>
       </c>
     </row>
+    <row r="107" ht="51" spans="1:9">
+      <c r="A107" s="1">
+        <v>2411</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E107" s="1">
+        <v>0</v>
+      </c>
+      <c r="F107" s="1">
+        <v>1</v>
+      </c>
+      <c r="G107" s="1">
+        <v>50</v>
+      </c>
+      <c r="H107" s="4">
+        <v>45867</v>
+      </c>
+      <c r="I107" s="4">
+        <v>45867</v>
+      </c>
+    </row>
+    <row r="108" ht="68" spans="1:10">
+      <c r="A108" s="1">
+        <v>272</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E108" s="1">
+        <v>0</v>
+      </c>
+      <c r="F108" s="1">
+        <v>1</v>
+      </c>
+      <c r="G108" s="1">
+        <v>15</v>
+      </c>
+      <c r="H108" s="4">
+        <v>45867</v>
+      </c>
+      <c r="I108" s="4">
+        <v>45867</v>
+      </c>
+      <c r="J108" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="109" ht="34" spans="1:9">
+      <c r="A109" s="1">
+        <v>270</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E109" s="1">
+        <v>1</v>
+      </c>
+      <c r="F109" s="1">
+        <v>0</v>
+      </c>
+      <c r="G109" s="1">
+        <v>15</v>
+      </c>
+      <c r="H109" s="4">
+        <v>45867</v>
+      </c>
+      <c r="I109" s="4">
+        <v>45867</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
feat: update workspace configuration and add markdown file for LeetCode problem 2419: Longest Subarray With Maximum Bitwise AND
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="16760"/>
+    <workbookView windowWidth="29100" windowHeight="14540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="216">
   <si>
     <t>#</t>
   </si>
@@ -672,6 +672,9 @@
   </si>
   <si>
     <t>Closest Binary Search Tree Value</t>
+  </si>
+  <si>
+    <t>Longest Subarray With Maximum Bitwise AND</t>
   </si>
 </sst>
 </file>
@@ -1828,10 +1831,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J109"/>
+  <dimension ref="A1:J110"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="172" zoomScaleNormal="172" topLeftCell="A104" workbookViewId="0">
-      <selection activeCell="H109" sqref="H109:I109"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" topLeftCell="A104" workbookViewId="0">
+      <selection activeCell="J110" sqref="J110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -5132,6 +5135,35 @@
         <v>45867</v>
       </c>
     </row>
+    <row r="110" ht="34" spans="1:9">
+      <c r="A110" s="1">
+        <v>2419</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E110" s="1">
+        <v>1</v>
+      </c>
+      <c r="F110" s="1">
+        <v>0</v>
+      </c>
+      <c r="G110" s="1">
+        <v>10</v>
+      </c>
+      <c r="H110" s="4">
+        <v>45868</v>
+      </c>
+      <c r="I110" s="4">
+        <v>45868</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
feat: update workspace and add markdown file for LeetCode problem 898: Bitwise ORs of Subarrays
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="29100" windowHeight="14540"/>
+    <workbookView windowHeight="16760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="217">
   <si>
     <t>#</t>
   </si>
@@ -675,6 +675,9 @@
   </si>
   <si>
     <t>Longest Subarray With Maximum Bitwise AND</t>
+  </si>
+  <si>
+    <t>Bitwise ORs of Subarrays</t>
   </si>
 </sst>
 </file>
@@ -1831,10 +1834,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J110"/>
+  <dimension ref="A1:J111"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" topLeftCell="A104" workbookViewId="0">
-      <selection activeCell="J110" sqref="J110"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" topLeftCell="A108" workbookViewId="0">
+      <selection activeCell="C111" sqref="C111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -5164,6 +5167,14 @@
         <v>45868</v>
       </c>
     </row>
+    <row r="111" ht="17" spans="1:2">
+      <c r="A111" s="1">
+        <v>898</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
feat: update workspace and add solutions for LeetCode problems 480, 118, and 314
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="221">
   <si>
     <t>#</t>
   </si>
@@ -678,6 +678,18 @@
   </si>
   <si>
     <t>Bitwise ORs of Subarrays</t>
+  </si>
+  <si>
+    <t>#array #bit-minipulation #dynamic-programming</t>
+  </si>
+  <si>
+    <t>Pascal's Triangle</t>
+  </si>
+  <si>
+    <t>Binary Tree Vertical Order Traversal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#tree #binary-tree #hash-table #bfs </t>
   </si>
 </sst>
 </file>
@@ -1834,10 +1846,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J111"/>
+  <dimension ref="A1:J113"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" topLeftCell="A108" workbookViewId="0">
-      <selection activeCell="C111" sqref="C111"/>
+      <selection activeCell="D115" sqref="D115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -5167,12 +5179,91 @@
         <v>45868</v>
       </c>
     </row>
-    <row r="111" ht="17" spans="1:2">
+    <row r="111" ht="68" spans="1:9">
       <c r="A111" s="1">
         <v>898</v>
       </c>
       <c r="B111" s="2" t="s">
         <v>216</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E111" s="1">
+        <v>0</v>
+      </c>
+      <c r="F111" s="1">
+        <v>1</v>
+      </c>
+      <c r="G111" s="1">
+        <v>30</v>
+      </c>
+      <c r="H111" s="4">
+        <v>45869</v>
+      </c>
+      <c r="I111" s="4">
+        <v>45869</v>
+      </c>
+    </row>
+    <row r="112" ht="34" spans="1:9">
+      <c r="A112" s="1">
+        <v>118</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E112" s="1">
+        <v>1</v>
+      </c>
+      <c r="F112" s="1">
+        <v>0</v>
+      </c>
+      <c r="G112" s="1">
+        <v>6</v>
+      </c>
+      <c r="H112" s="4">
+        <v>45870</v>
+      </c>
+      <c r="I112" s="4">
+        <v>45870</v>
+      </c>
+    </row>
+    <row r="113" ht="34" spans="1:9">
+      <c r="A113" s="1">
+        <v>314</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E113" s="1">
+        <v>1</v>
+      </c>
+      <c r="F113" s="1">
+        <v>0</v>
+      </c>
+      <c r="G113" s="1">
+        <v>23</v>
+      </c>
+      <c r="H113" s="4">
+        <v>45870</v>
+      </c>
+      <c r="I113" s="4">
+        <v>45870</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: update workspace and add new implementations for LeetCode problems 3477, 2106, 2561, 904, and 161
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="16760"/>
+    <workbookView windowHeight="14540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="230">
   <si>
     <t>#</t>
   </si>
@@ -690,6 +690,33 @@
   </si>
   <si>
     <t xml:space="preserve">#tree #binary-tree #hash-table #bfs </t>
+  </si>
+  <si>
+    <t>Rearranging Fruits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#greedy #hash-table #sorting </t>
+  </si>
+  <si>
+    <t>One Edit Distance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#string #two-pointers #array </t>
+  </si>
+  <si>
+    <t>Fruit Into Baskets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#array #sliding-window </t>
+  </si>
+  <si>
+    <t>Fruits Into Baskets II</t>
+  </si>
+  <si>
+    <t>Maximum Fruits Harvested After at Most K Steps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#array #two-pointers #sliding-window </t>
   </si>
 </sst>
 </file>
@@ -1846,10 +1873,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J113"/>
+  <dimension ref="A1:J118"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" topLeftCell="A108" workbookViewId="0">
-      <selection activeCell="D115" sqref="D115"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="H118" sqref="H118:I118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -5266,6 +5293,151 @@
         <v>45870</v>
       </c>
     </row>
+    <row r="114" ht="34" spans="1:9">
+      <c r="A114" s="1">
+        <v>2561</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E114" s="1">
+        <v>0</v>
+      </c>
+      <c r="F114" s="1">
+        <v>1</v>
+      </c>
+      <c r="G114" s="1">
+        <v>20</v>
+      </c>
+      <c r="H114" s="4">
+        <v>45871</v>
+      </c>
+      <c r="I114" s="4">
+        <v>45871</v>
+      </c>
+    </row>
+    <row r="115" ht="34" spans="1:9">
+      <c r="A115" s="1">
+        <v>161</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E115" s="1">
+        <v>0</v>
+      </c>
+      <c r="F115" s="1">
+        <v>1</v>
+      </c>
+      <c r="G115" s="1">
+        <v>13</v>
+      </c>
+      <c r="H115" s="4">
+        <v>45872</v>
+      </c>
+      <c r="I115" s="4">
+        <v>45872</v>
+      </c>
+    </row>
+    <row r="116" ht="34" spans="1:9">
+      <c r="A116" s="1">
+        <v>904</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E116" s="1">
+        <v>0</v>
+      </c>
+      <c r="F116" s="1">
+        <v>1</v>
+      </c>
+      <c r="G116" s="1">
+        <v>20</v>
+      </c>
+      <c r="H116" s="4">
+        <v>45873</v>
+      </c>
+      <c r="I116" s="4">
+        <v>45873</v>
+      </c>
+    </row>
+    <row r="117" ht="17" spans="1:9">
+      <c r="A117" s="1">
+        <v>3477</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E117" s="1">
+        <v>1</v>
+      </c>
+      <c r="F117" s="1">
+        <v>0</v>
+      </c>
+      <c r="G117" s="1">
+        <v>5</v>
+      </c>
+      <c r="H117" s="4">
+        <v>45874</v>
+      </c>
+      <c r="I117" s="4">
+        <v>45874</v>
+      </c>
+    </row>
+    <row r="118" ht="51" spans="1:9">
+      <c r="A118" s="1">
+        <v>2106</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E118" s="1">
+        <v>0</v>
+      </c>
+      <c r="F118" s="1">
+        <v>1</v>
+      </c>
+      <c r="G118" s="1">
+        <v>36</v>
+      </c>
+      <c r="H118" s="4">
+        <v>45874</v>
+      </c>
+      <c r="I118" s="4">
+        <v>45874</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
feat: update workspace and add implementation for LeetCode problem 3479: Fruits Into Baskets III
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="14540"/>
+    <workbookView windowHeight="14500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="233">
   <si>
     <t>#</t>
   </si>
@@ -717,6 +717,15 @@
   </si>
   <si>
     <t xml:space="preserve">#array #two-pointers #sliding-window </t>
+  </si>
+  <si>
+    <t>Fruits Into Baskets III</t>
+  </si>
+  <si>
+    <t>#binary-tree #segment-tree #ordered-set</t>
+  </si>
+  <si>
+    <t>?segTree</t>
   </si>
 </sst>
 </file>
@@ -1873,10 +1882,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J118"/>
+  <dimension ref="A1:J119"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="H118" sqref="H118:I118"/>
+      <selection activeCell="I119" sqref="I119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -5438,6 +5447,38 @@
         <v>45874</v>
       </c>
     </row>
+    <row r="119" ht="51" spans="1:10">
+      <c r="A119" s="1">
+        <v>3479</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E119" s="1">
+        <v>0</v>
+      </c>
+      <c r="F119" s="1">
+        <v>1</v>
+      </c>
+      <c r="G119" s="1">
+        <v>50</v>
+      </c>
+      <c r="H119" s="4">
+        <v>45875</v>
+      </c>
+      <c r="I119" s="4">
+        <v>45875</v>
+      </c>
+      <c r="J119" s="2" t="s">
+        <v>232</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
feat: add implementations for LeetCode problems 808, 231, and 1198; update workspace configuration
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="14500"/>
+    <workbookView windowWidth="29100" windowHeight="14540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="241">
   <si>
     <t>#</t>
   </si>
@@ -726,6 +726,30 @@
   </si>
   <si>
     <t>?segTree</t>
+  </si>
+  <si>
+    <t>Find the Maximum Number of Fruits Collected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#dynamic-programming #rolling-array #matrix </t>
+  </si>
+  <si>
+    <t>Soup Servings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#dynamic-programming #math </t>
+  </si>
+  <si>
+    <t>Power of Two</t>
+  </si>
+  <si>
+    <t>return n &amp; (-n) == n</t>
+  </si>
+  <si>
+    <t>Find Smallest Common Element in All Rows</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#hash-table #binary-search #matrix #counting </t>
   </si>
 </sst>
 </file>
@@ -1882,10 +1906,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J119"/>
+  <dimension ref="A1:J123"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="I119" sqref="I119"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" topLeftCell="A119" workbookViewId="0">
+      <selection activeCell="E124" sqref="E124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -5479,6 +5503,128 @@
         <v>232</v>
       </c>
     </row>
+    <row r="120" ht="68" spans="1:9">
+      <c r="A120" s="1">
+        <v>3363</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E120" s="1">
+        <v>0</v>
+      </c>
+      <c r="F120" s="1">
+        <v>1</v>
+      </c>
+      <c r="G120" s="1">
+        <v>60</v>
+      </c>
+      <c r="H120" s="4">
+        <v>45876</v>
+      </c>
+      <c r="I120" s="4">
+        <v>45876</v>
+      </c>
+    </row>
+    <row r="121" ht="51" spans="1:10">
+      <c r="A121" s="1">
+        <v>808</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E121" s="1">
+        <v>0</v>
+      </c>
+      <c r="F121" s="1">
+        <v>1</v>
+      </c>
+      <c r="G121" s="1">
+        <v>20</v>
+      </c>
+      <c r="H121" s="4">
+        <v>45877</v>
+      </c>
+      <c r="I121" s="4">
+        <v>45877</v>
+      </c>
+      <c r="J121" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="122" ht="34" spans="1:10">
+      <c r="A122" s="1">
+        <v>231</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E122" s="1">
+        <v>1</v>
+      </c>
+      <c r="F122" s="1">
+        <v>0</v>
+      </c>
+      <c r="G122" s="1">
+        <v>5</v>
+      </c>
+      <c r="H122" s="4">
+        <v>45878</v>
+      </c>
+      <c r="I122" s="4">
+        <v>45878</v>
+      </c>
+      <c r="J122" s="2" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="123" ht="51" spans="1:9">
+      <c r="A123" s="1">
+        <v>1198</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E123" s="1">
+        <v>1</v>
+      </c>
+      <c r="F123" s="1">
+        <v>0</v>
+      </c>
+      <c r="G123" s="1">
+        <v>10</v>
+      </c>
+      <c r="H123" s="4">
+        <v>45878</v>
+      </c>
+      <c r="I123" s="4">
+        <v>45878</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
feat: update workspace configuration and add implementation for LeetCode problem 869: Reordered Power of 2
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="243">
   <si>
     <t>#</t>
   </si>
@@ -750,6 +750,12 @@
   </si>
   <si>
     <t xml:space="preserve">#hash-table #binary-search #matrix #counting </t>
+  </si>
+  <si>
+    <t>Reordered Power of 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#enumeration </t>
   </si>
 </sst>
 </file>
@@ -1906,10 +1912,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J123"/>
+  <dimension ref="A1:J124"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" topLeftCell="A119" workbookViewId="0">
-      <selection activeCell="E124" sqref="E124"/>
+      <selection activeCell="I129" sqref="I129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -5625,6 +5631,35 @@
         <v>45878</v>
       </c>
     </row>
+    <row r="124" ht="17" spans="1:9">
+      <c r="A124" s="1">
+        <v>869</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E124" s="1">
+        <v>1</v>
+      </c>
+      <c r="F124" s="1">
+        <v>0</v>
+      </c>
+      <c r="G124" s="1">
+        <v>20</v>
+      </c>
+      <c r="H124" s="4">
+        <v>45879</v>
+      </c>
+      <c r="I124" s="4">
+        <v>45879</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
feat: add implementation for LeetCode problem 2438: Range Product Queries of Powers and update workspace configuration
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="29100" windowHeight="14540"/>
+    <workbookView windowHeight="16760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="244">
   <si>
     <t>#</t>
   </si>
@@ -756,6 +756,9 @@
   </si>
   <si>
     <t xml:space="preserve">#enumeration </t>
+  </si>
+  <si>
+    <t>Range Product Queries of Powers</t>
   </si>
 </sst>
 </file>
@@ -1912,10 +1915,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J124"/>
+  <dimension ref="A1:J125"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" topLeftCell="A119" workbookViewId="0">
-      <selection activeCell="I129" sqref="I129"/>
+      <selection activeCell="K125" sqref="K125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -5660,6 +5663,32 @@
         <v>45879</v>
       </c>
     </row>
+    <row r="125" ht="34" spans="1:9">
+      <c r="A125" s="1">
+        <v>2438</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E125" s="1">
+        <v>0</v>
+      </c>
+      <c r="F125" s="1">
+        <v>1</v>
+      </c>
+      <c r="G125" s="1">
+        <v>20</v>
+      </c>
+      <c r="H125" s="4">
+        <v>45880</v>
+      </c>
+      <c r="I125" s="4">
+        <v>45880</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Add notes for 326
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="16760"/>
+    <workbookView windowWidth="29100" windowHeight="14540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="247">
   <si>
     <t>#</t>
   </si>
@@ -759,6 +759,15 @@
   </si>
   <si>
     <t>Range Product Queries of Powers</t>
+  </si>
+  <si>
+    <t>Ways to Express an Integer as Sum of Powers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#dynamic-programming </t>
+  </si>
+  <si>
+    <t>Power of Three</t>
   </si>
 </sst>
 </file>
@@ -1915,10 +1924,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J125"/>
+  <dimension ref="A1:J129"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" topLeftCell="A119" workbookViewId="0">
-      <selection activeCell="K125" sqref="K125"/>
+      <selection activeCell="H129" sqref="H129:I129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -5689,6 +5698,83 @@
         <v>45880</v>
       </c>
     </row>
+    <row r="126" ht="34" spans="1:10">
+      <c r="A126" s="1">
+        <v>2787</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E126" s="1">
+        <v>0</v>
+      </c>
+      <c r="F126" s="1">
+        <v>1</v>
+      </c>
+      <c r="G126" s="1">
+        <v>30</v>
+      </c>
+      <c r="H126" s="4">
+        <v>45881</v>
+      </c>
+      <c r="I126" s="4">
+        <v>45881</v>
+      </c>
+      <c r="J126" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="127" ht="17" spans="1:9">
+      <c r="A127" s="1">
+        <v>326</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E127" s="1">
+        <v>1</v>
+      </c>
+      <c r="F127" s="1">
+        <v>0</v>
+      </c>
+      <c r="G127" s="1">
+        <v>5</v>
+      </c>
+      <c r="H127" s="4">
+        <v>45882</v>
+      </c>
+      <c r="I127" s="4">
+        <v>45882</v>
+      </c>
+    </row>
+    <row r="128" spans="8:9">
+      <c r="H128" s="4">
+        <v>45883</v>
+      </c>
+      <c r="I128" s="4">
+        <v>45883</v>
+      </c>
+    </row>
+    <row r="129" spans="8:9">
+      <c r="H129" s="4">
+        <v>45883</v>
+      </c>
+      <c r="I129" s="4">
+        <v>45883</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
add notes for 2264
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="248">
   <si>
     <t>#</t>
   </si>
@@ -768,6 +768,9 @@
   </si>
   <si>
     <t>Power of Three</t>
+  </si>
+  <si>
+    <t>Largest 3-Same-Digit Number in String</t>
   </si>
 </sst>
 </file>
@@ -1927,7 +1930,7 @@
   <dimension ref="A1:J129"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" topLeftCell="A119" workbookViewId="0">
-      <selection activeCell="H129" sqref="H129:I129"/>
+      <selection activeCell="G128" sqref="G128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -5759,7 +5762,28 @@
         <v>45882</v>
       </c>
     </row>
-    <row r="128" spans="8:9">
+    <row r="128" ht="34" spans="1:9">
+      <c r="A128" s="1">
+        <v>2264</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D128" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E128" s="1">
+        <v>1</v>
+      </c>
+      <c r="F128" s="1">
+        <v>0</v>
+      </c>
+      <c r="G128" s="1">
+        <v>5</v>
+      </c>
       <c r="H128" s="4">
         <v>45883</v>
       </c>

</xml_diff>

<commit_message>
add notes for 303
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="250">
   <si>
     <t>#</t>
   </si>
@@ -771,6 +771,12 @@
   </si>
   <si>
     <t>Largest 3-Same-Digit Number in String</t>
+  </si>
+  <si>
+    <t>Range Sum Query - Immutable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#array #prefix-sum </t>
   </si>
 </sst>
 </file>
@@ -1929,8 +1935,8 @@
   <sheetPr/>
   <dimension ref="A1:J129"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" topLeftCell="A119" workbookViewId="0">
-      <selection activeCell="G128" sqref="G128"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" topLeftCell="A120" workbookViewId="0">
+      <selection activeCell="G129" sqref="G129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -5791,7 +5797,28 @@
         <v>45883</v>
       </c>
     </row>
-    <row r="129" spans="8:9">
+    <row r="129" ht="34" spans="1:9">
+      <c r="A129" s="1">
+        <v>303</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E129" s="1">
+        <v>1</v>
+      </c>
+      <c r="F129" s="1">
+        <v>0</v>
+      </c>
+      <c r="G129" s="1">
+        <v>5</v>
+      </c>
       <c r="H129" s="4">
         <v>45883</v>
       </c>

</xml_diff>

<commit_message>
Add notes for 342
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="29100" windowHeight="14540"/>
+    <workbookView windowWidth="26860" windowHeight="14540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="252">
   <si>
     <t>#</t>
   </si>
@@ -777,6 +777,12 @@
   </si>
   <si>
     <t xml:space="preserve">#array #prefix-sum </t>
+  </si>
+  <si>
+    <t>Power of Four</t>
+  </si>
+  <si>
+    <t>#binary-search</t>
   </si>
 </sst>
 </file>
@@ -1933,10 +1939,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J129"/>
+  <dimension ref="A1:J130"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" topLeftCell="A120" workbookViewId="0">
-      <selection activeCell="G129" sqref="G129"/>
+      <selection activeCell="D125" sqref="D125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -5826,6 +5832,35 @@
         <v>45883</v>
       </c>
     </row>
+    <row r="130" ht="17" spans="1:9">
+      <c r="A130" s="1">
+        <v>342</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E130" s="1">
+        <v>1</v>
+      </c>
+      <c r="F130" s="1">
+        <v>0</v>
+      </c>
+      <c r="G130" s="1">
+        <v>5</v>
+      </c>
+      <c r="H130" s="4">
+        <v>45884</v>
+      </c>
+      <c r="I130" s="4">
+        <v>45884</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Update workspace and add solution for LeetCode problem 3195: Find the Minimum Area to Cover All Ones I
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="261">
   <si>
     <t>#</t>
   </si>
@@ -804,6 +804,12 @@
   </si>
   <si>
     <t xml:space="preserve">#matrix #monotonic-stack #dynamic-programming </t>
+  </si>
+  <si>
+    <t>Find the Minimum Area to Cover All Ones I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#array #matrix </t>
   </si>
 </sst>
 </file>
@@ -1960,10 +1966,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J137"/>
+  <dimension ref="A1:J138"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" topLeftCell="A125" workbookViewId="0">
-      <selection activeCell="J137" sqref="J137"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" topLeftCell="A135" workbookViewId="0">
+      <selection activeCell="I141" sqref="I141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -5998,6 +6004,35 @@
         <v>45890</v>
       </c>
     </row>
+    <row r="138" ht="34" spans="1:9">
+      <c r="A138" s="1">
+        <v>3195</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="C138" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="D138" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E138" s="1">
+        <v>0</v>
+      </c>
+      <c r="F138" s="1">
+        <v>1</v>
+      </c>
+      <c r="G138" s="1">
+        <v>15</v>
+      </c>
+      <c r="H138" s="4">
+        <v>45891</v>
+      </c>
+      <c r="I138" s="4">
+        <v>45891</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Add solutions for various LeetCode problems and their corresponding markdown documentation
- Implemented solution for problem 1181: Before and After Puzzle.
- Added solution for problem 3000: Maximum Area of Longest Diagonal Rectangle.
- Created solution for problem 3021: Alice and Bob Playing Flower Game.
- Developed solution for problem 3446: Sort Matrix by Diagonals.
- Added solution for problem 3459: Length of Longest V-Shaped Diagonal Segment.
- Created markdown documentation for each problem including examples and constraints.
- Updated binary files in the Obsidian Vault.
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="272">
   <si>
     <t>#</t>
   </si>
@@ -810,6 +810,39 @@
   </si>
   <si>
     <t xml:space="preserve">#array #matrix </t>
+  </si>
+  <si>
+    <t>Diagonal Traverse</t>
+  </si>
+  <si>
+    <t>Maximum Area of Longest Diagonal Rectangle</t>
+  </si>
+  <si>
+    <t>Before and After Puzzle</t>
+  </si>
+  <si>
+    <t>#array #hash-table #string #sorting</t>
+  </si>
+  <si>
+    <t>Length of Longest V-Shaped Diagonal Segment</t>
+  </si>
+  <si>
+    <t>#matrix #dfs #cache</t>
+  </si>
+  <si>
+    <t>@cache?</t>
+  </si>
+  <si>
+    <t>Sort Matrix by Diagonals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#matrix #sorting </t>
+  </si>
+  <si>
+    <t>Alice and Bob Playing Flower Game</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#math </t>
   </si>
 </sst>
 </file>
@@ -1966,10 +1999,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J138"/>
+  <dimension ref="A1:J147"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" topLeftCell="A135" workbookViewId="0">
-      <selection activeCell="I141" sqref="I141"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="J147" sqref="J147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -6033,6 +6066,192 @@
         <v>45891</v>
       </c>
     </row>
+    <row r="139" spans="8:9">
+      <c r="H139" s="4"/>
+      <c r="I139" s="4"/>
+    </row>
+    <row r="140" spans="8:9">
+      <c r="H140" s="4"/>
+      <c r="I140" s="4"/>
+    </row>
+    <row r="141" spans="8:9">
+      <c r="H141" s="4"/>
+      <c r="I141" s="4"/>
+    </row>
+    <row r="142" ht="17" spans="1:9">
+      <c r="A142" s="1">
+        <v>498</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="C142" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="D142" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E142" s="1">
+        <v>1</v>
+      </c>
+      <c r="F142" s="1">
+        <v>0</v>
+      </c>
+      <c r="G142" s="1">
+        <v>25</v>
+      </c>
+      <c r="H142" s="4">
+        <v>45894</v>
+      </c>
+      <c r="I142" s="4">
+        <v>45894</v>
+      </c>
+    </row>
+    <row r="143" ht="51" spans="1:9">
+      <c r="A143" s="1">
+        <v>3000</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="D143" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E143" s="1">
+        <v>1</v>
+      </c>
+      <c r="F143" s="1">
+        <v>0</v>
+      </c>
+      <c r="G143" s="1">
+        <v>5</v>
+      </c>
+      <c r="H143" s="4">
+        <v>45895</v>
+      </c>
+      <c r="I143" s="4">
+        <v>45895</v>
+      </c>
+    </row>
+    <row r="144" ht="34" spans="1:9">
+      <c r="A144" s="1">
+        <v>1181</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C144" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="D144" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E144" s="1">
+        <v>0</v>
+      </c>
+      <c r="F144" s="1">
+        <v>1</v>
+      </c>
+      <c r="G144" s="1">
+        <v>25</v>
+      </c>
+      <c r="H144" s="4">
+        <v>45895</v>
+      </c>
+      <c r="I144" s="4">
+        <v>45895</v>
+      </c>
+    </row>
+    <row r="145" ht="51" spans="1:10">
+      <c r="A145" s="1">
+        <v>3459</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="C145" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="D145" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E145" s="1">
+        <v>0</v>
+      </c>
+      <c r="F145" s="1">
+        <v>1</v>
+      </c>
+      <c r="G145" s="1">
+        <v>30</v>
+      </c>
+      <c r="H145" s="4">
+        <v>45896</v>
+      </c>
+      <c r="I145" s="4">
+        <v>45896</v>
+      </c>
+      <c r="J145" s="2" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="146" ht="17" spans="1:9">
+      <c r="A146" s="1">
+        <v>3446</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="C146" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="D146" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E146" s="1">
+        <v>1</v>
+      </c>
+      <c r="F146" s="1">
+        <v>0</v>
+      </c>
+      <c r="G146" s="1">
+        <v>22</v>
+      </c>
+      <c r="H146" s="4">
+        <v>45897</v>
+      </c>
+      <c r="I146" s="4">
+        <v>45897</v>
+      </c>
+    </row>
+    <row r="147" ht="34" spans="1:9">
+      <c r="A147" s="1">
+        <v>3021</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="C147" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="D147" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E147" s="1">
+        <v>1</v>
+      </c>
+      <c r="F147" s="1">
+        <v>0</v>
+      </c>
+      <c r="G147" s="1">
+        <v>10</v>
+      </c>
+      <c r="H147" s="4">
+        <v>45898</v>
+      </c>
+      <c r="I147" s="4">
+        <v>45898</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Add solution for LeetCode problem 1792: Maximum Average Pass Ratio and update workspace
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="274">
   <si>
     <t>#</t>
   </si>
@@ -843,6 +843,12 @@
   </si>
   <si>
     <t xml:space="preserve">#math </t>
+  </si>
+  <si>
+    <t>Maximum Average Pass Ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#array #heap #math #greedy </t>
   </si>
 </sst>
 </file>
@@ -1999,10 +2005,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J147"/>
+  <dimension ref="A1:J148"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="J147" sqref="J147"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" topLeftCell="A143" workbookViewId="0">
+      <selection activeCell="I148" sqref="I148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -6252,6 +6258,35 @@
         <v>45898</v>
       </c>
     </row>
+    <row r="148" ht="34" spans="1:9">
+      <c r="A148" s="1">
+        <v>1972</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C148" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="D148" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E148" s="1">
+        <v>1</v>
+      </c>
+      <c r="F148" s="1">
+        <v>0</v>
+      </c>
+      <c r="G148" s="1">
+        <v>21</v>
+      </c>
+      <c r="H148" s="4">
+        <v>45901</v>
+      </c>
+      <c r="I148" s="4">
+        <v>45901</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Add solution for LeetCode problem 37: Sudoku Solver and update related markdown documentation
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="276">
   <si>
     <t>#</t>
   </si>
@@ -843,6 +843,12 @@
   </si>
   <si>
     <t xml:space="preserve">#math </t>
+  </si>
+  <si>
+    <t>Sudoku Solver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#matrix #bit-minipulation #hash-table #backtracking </t>
   </si>
   <si>
     <t>Maximum Average Pass Ratio</t>
@@ -2005,10 +2011,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J148"/>
+  <dimension ref="A1:J151"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" topLeftCell="A143" workbookViewId="0">
-      <selection activeCell="I148" sqref="I148"/>
+      <selection activeCell="H155" sqref="H155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -6258,32 +6264,74 @@
         <v>45898</v>
       </c>
     </row>
-    <row r="148" ht="34" spans="1:9">
-      <c r="A148" s="1">
+    <row r="148" spans="8:9">
+      <c r="H148" s="4">
+        <v>45899</v>
+      </c>
+      <c r="I148" s="4">
+        <v>45899</v>
+      </c>
+    </row>
+    <row r="149" spans="8:9">
+      <c r="H149" s="4">
+        <v>45900</v>
+      </c>
+      <c r="I149" s="4">
+        <v>45900</v>
+      </c>
+    </row>
+    <row r="150" ht="68" spans="1:9">
+      <c r="A150" s="1">
+        <v>37</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C150" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="D150" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E150" s="1">
+        <v>0</v>
+      </c>
+      <c r="F150" s="1">
+        <v>1</v>
+      </c>
+      <c r="H150" s="4">
+        <v>45900</v>
+      </c>
+      <c r="I150" s="4">
+        <v>45900</v>
+      </c>
+    </row>
+    <row r="151" ht="34" spans="1:9">
+      <c r="A151" s="1">
         <v>1972</v>
       </c>
-      <c r="B148" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="C148" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="D148" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E148" s="1">
-        <v>1</v>
-      </c>
-      <c r="F148" s="1">
-        <v>0</v>
-      </c>
-      <c r="G148" s="1">
+      <c r="B151" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="C151" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="D151" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E151" s="1">
+        <v>1</v>
+      </c>
+      <c r="F151" s="1">
+        <v>0</v>
+      </c>
+      <c r="G151" s="1">
         <v>21</v>
       </c>
-      <c r="H148" s="4">
+      <c r="H151" s="4">
         <v>45901</v>
       </c>
-      <c r="I148" s="4">
+      <c r="I151" s="4">
         <v>45901</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add solutions for LeetCode problems 36: Valid Sudoku and 1182: Shortest Distance to Target Color, and update related markdown documentation
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="279">
   <si>
     <t>#</t>
   </si>
@@ -843,6 +843,15 @@
   </si>
   <si>
     <t xml:space="preserve">#math </t>
+  </si>
+  <si>
+    <t>Shortest Distance to Target Color</t>
+  </si>
+  <si>
+    <t>Valid Sudoku</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#set #matrix </t>
   </si>
   <si>
     <t>Sudoku Solver</t>
@@ -2014,7 +2023,7 @@
   <dimension ref="A1:J151"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" topLeftCell="A143" workbookViewId="0">
-      <selection activeCell="H155" sqref="H155"/>
+      <selection activeCell="G153" sqref="G153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -6264,7 +6273,28 @@
         <v>45898</v>
       </c>
     </row>
-    <row r="148" spans="8:9">
+    <row r="148" ht="34" spans="1:9">
+      <c r="A148" s="1">
+        <v>1182</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C148" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="D148" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E148" s="1">
+        <v>0</v>
+      </c>
+      <c r="F148" s="1">
+        <v>1</v>
+      </c>
+      <c r="G148" s="1">
+        <v>30</v>
+      </c>
       <c r="H148" s="4">
         <v>45899</v>
       </c>
@@ -6272,7 +6302,28 @@
         <v>45899</v>
       </c>
     </row>
-    <row r="149" spans="8:9">
+    <row r="149" ht="17" spans="1:9">
+      <c r="A149" s="1">
+        <v>36</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="C149" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="D149" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E149" s="1">
+        <v>1</v>
+      </c>
+      <c r="F149" s="1">
+        <v>0</v>
+      </c>
+      <c r="G149" s="1">
+        <v>11</v>
+      </c>
       <c r="H149" s="4">
         <v>45900</v>
       </c>
@@ -6285,10 +6336,10 @@
         <v>37</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="D150" s="1" t="s">
         <v>23</v>
@@ -6311,10 +6362,10 @@
         <v>1972</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="D151" s="1" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Add solution for LeetCode problem 3025: Find the Number of Ways to Place People I and update related markdown documentation
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="281">
   <si>
     <t>#</t>
   </si>
@@ -864,6 +864,12 @@
   </si>
   <si>
     <t xml:space="preserve">#array #heap #math #greedy </t>
+  </si>
+  <si>
+    <t>Find the Number of Ways to Place People I</t>
+  </si>
+  <si>
+    <t>#greedy #sorting</t>
   </si>
 </sst>
 </file>
@@ -2020,10 +2026,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J151"/>
+  <dimension ref="A1:J152"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" topLeftCell="A143" workbookViewId="0">
-      <selection activeCell="G153" sqref="G153"/>
+      <selection activeCell="F145" sqref="F145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -6386,6 +6392,35 @@
         <v>45901</v>
       </c>
     </row>
+    <row r="152" ht="34" spans="1:9">
+      <c r="A152" s="1">
+        <v>3025</v>
+      </c>
+      <c r="B152" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="C152" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="D152" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E152" s="1">
+        <v>1</v>
+      </c>
+      <c r="F152" s="1">
+        <v>0</v>
+      </c>
+      <c r="G152" s="1">
+        <v>21</v>
+      </c>
+      <c r="H152" s="4">
+        <v>45902</v>
+      </c>
+      <c r="I152" s="4">
+        <v>45902</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Add solution for LeetCode problem 3027: Find the Number of Ways to Place People II and update related markdown documentation
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="283">
   <si>
     <t>#</t>
   </si>
@@ -870,6 +870,12 @@
   </si>
   <si>
     <t>#greedy #sorting</t>
+  </si>
+  <si>
+    <t>Find the Number of Ways to Place People II</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#array #math #geometry #sorting #enumeration </t>
   </si>
 </sst>
 </file>
@@ -2026,10 +2032,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J152"/>
+  <dimension ref="A1:J153"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" topLeftCell="A143" workbookViewId="0">
-      <selection activeCell="F145" sqref="F145"/>
+      <selection activeCell="H148" sqref="H148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -6421,6 +6427,35 @@
         <v>45902</v>
       </c>
     </row>
+    <row r="153" ht="51" spans="1:9">
+      <c r="A153" s="1">
+        <v>3027</v>
+      </c>
+      <c r="B153" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="C153" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="D153" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E153" s="1">
+        <v>0</v>
+      </c>
+      <c r="F153" s="1">
+        <v>1</v>
+      </c>
+      <c r="G153" s="1">
+        <v>20</v>
+      </c>
+      <c r="H153" s="4">
+        <v>45903</v>
+      </c>
+      <c r="I153" s="4">
+        <v>45903</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Add solutions for LeetCode problems 2749: Minimum Operations to Make the Integer Zero and 3516: Find Closest Person, and update related markdown documentation
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="286">
   <si>
     <t>#</t>
   </si>
@@ -876,6 +876,15 @@
   </si>
   <si>
     <t xml:space="preserve">#array #math #geometry #sorting #enumeration </t>
+  </si>
+  <si>
+    <t>Find Closest Person</t>
+  </si>
+  <si>
+    <t>Minimum Operations to Make the Integer Zero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#bit-minipulation </t>
   </si>
 </sst>
 </file>
@@ -2032,10 +2041,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J153"/>
+  <dimension ref="A1:J155"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" topLeftCell="A143" workbookViewId="0">
-      <selection activeCell="H148" sqref="H148"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" topLeftCell="A150" workbookViewId="0">
+      <selection activeCell="F155" sqref="F155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -6456,6 +6465,64 @@
         <v>45903</v>
       </c>
     </row>
+    <row r="154" ht="17" spans="1:9">
+      <c r="A154" s="1">
+        <v>3516</v>
+      </c>
+      <c r="B154" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="C154" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D154" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E154" s="1">
+        <v>1</v>
+      </c>
+      <c r="F154" s="1">
+        <v>0</v>
+      </c>
+      <c r="G154" s="1">
+        <v>5</v>
+      </c>
+      <c r="H154" s="4">
+        <v>45904</v>
+      </c>
+      <c r="I154" s="4">
+        <v>45904</v>
+      </c>
+    </row>
+    <row r="155" ht="34" spans="1:9">
+      <c r="A155" s="1">
+        <v>2749</v>
+      </c>
+      <c r="B155" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="C155" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="D155" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E155" s="1">
+        <v>0</v>
+      </c>
+      <c r="F155" s="1">
+        <v>1</v>
+      </c>
+      <c r="G155" s="1">
+        <v>13</v>
+      </c>
+      <c r="H155" s="4">
+        <v>45905</v>
+      </c>
+      <c r="I155" s="4">
+        <v>45905</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Add solution for LeetCode problem 567: Permutation in String and update related markdown documentation
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="288">
   <si>
     <t>#</t>
   </si>
@@ -885,6 +885,12 @@
   </si>
   <si>
     <t xml:space="preserve">#bit-minipulation </t>
+  </si>
+  <si>
+    <t>Permutation in String</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#two-pointers #sliding-window </t>
   </si>
 </sst>
 </file>
@@ -2041,10 +2047,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J155"/>
+  <dimension ref="A1:J156"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" topLeftCell="A150" workbookViewId="0">
-      <selection activeCell="F155" sqref="F155"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" topLeftCell="A152" workbookViewId="0">
+      <selection activeCell="H156" sqref="H156:I156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -6523,6 +6529,35 @@
         <v>45905</v>
       </c>
     </row>
+    <row r="156" ht="34" spans="1:9">
+      <c r="A156" s="1">
+        <v>567</v>
+      </c>
+      <c r="B156" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="C156" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="D156" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E156" s="1">
+        <v>0</v>
+      </c>
+      <c r="F156" s="1">
+        <v>1</v>
+      </c>
+      <c r="G156" s="1">
+        <v>19</v>
+      </c>
+      <c r="H156" s="4">
+        <v>45905</v>
+      </c>
+      <c r="I156" s="4">
+        <v>45905</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Add solutions for LeetCode problems 1304: Find N Unique Integers Sum up to Zero and 1317: Convert Integer to the Sum of Two No-Zero Integers, and update related markdown documentation
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="29100" windowHeight="14540"/>
+    <workbookView windowWidth="26860" windowHeight="14480"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="290">
   <si>
     <t>#</t>
   </si>
@@ -635,9 +635,6 @@
     <t>#array</t>
   </si>
   <si>
-    <t>ezsy</t>
-  </si>
-  <si>
     <t>Count Number of Maximum Bitwise-OR Subsets</t>
   </si>
   <si>
@@ -891,6 +888,15 @@
   </si>
   <si>
     <t xml:space="preserve">#two-pointers #sliding-window </t>
+  </si>
+  <si>
+    <t>Find N Unique Integers Sum up to Zero</t>
+  </si>
+  <si>
+    <t>#math #array</t>
+  </si>
+  <si>
+    <t>Convert Integer to the Sum of Two No-Zero Integers</t>
   </si>
 </sst>
 </file>
@@ -2047,10 +2053,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J156"/>
+  <dimension ref="A1:J158"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" topLeftCell="A152" workbookViewId="0">
-      <selection activeCell="H156" sqref="H156:I156"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" topLeftCell="A155" workbookViewId="0">
+      <selection activeCell="G158" sqref="G158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -5156,7 +5162,7 @@
         <v>201</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>202</v>
+        <v>11</v>
       </c>
       <c r="E103" s="1">
         <v>1</v>
@@ -5179,10 +5185,10 @@
         <v>2044</v>
       </c>
       <c r="B104" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C104" s="2" t="s">
         <v>203</v>
-      </c>
-      <c r="C104" s="2" t="s">
-        <v>204</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>15</v>
@@ -5208,10 +5214,10 @@
         <v>2483</v>
       </c>
       <c r="B105" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="C105" s="2" t="s">
         <v>205</v>
-      </c>
-      <c r="C105" s="2" t="s">
-        <v>206</v>
       </c>
       <c r="D105" s="1" t="s">
         <v>15</v>
@@ -5237,10 +5243,10 @@
         <v>238</v>
       </c>
       <c r="B106" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C106" s="2" t="s">
         <v>207</v>
-      </c>
-      <c r="C106" s="2" t="s">
-        <v>208</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>15</v>
@@ -5266,10 +5272,10 @@
         <v>2411</v>
       </c>
       <c r="B107" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C107" s="2" t="s">
         <v>209</v>
-      </c>
-      <c r="C107" s="2" t="s">
-        <v>210</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>15</v>
@@ -5295,10 +5301,10 @@
         <v>272</v>
       </c>
       <c r="B108" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="C108" s="2" t="s">
         <v>211</v>
-      </c>
-      <c r="C108" s="2" t="s">
-        <v>212</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>23</v>
@@ -5319,7 +5325,7 @@
         <v>45867</v>
       </c>
       <c r="J108" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="109" ht="34" spans="1:9">
@@ -5327,7 +5333,7 @@
         <v>270</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C109" s="2" t="s">
         <v>139</v>
@@ -5356,7 +5362,7 @@
         <v>2419</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C110" s="2" t="s">
         <v>201</v>
@@ -5385,10 +5391,10 @@
         <v>898</v>
       </c>
       <c r="B111" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C111" s="2" t="s">
         <v>216</v>
-      </c>
-      <c r="C111" s="2" t="s">
-        <v>217</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>15</v>
@@ -5414,7 +5420,7 @@
         <v>118</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C112" s="2" t="s">
         <v>164</v>
@@ -5443,10 +5449,10 @@
         <v>314</v>
       </c>
       <c r="B113" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C113" s="2" t="s">
         <v>219</v>
-      </c>
-      <c r="C113" s="2" t="s">
-        <v>220</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>15</v>
@@ -5472,10 +5478,10 @@
         <v>2561</v>
       </c>
       <c r="B114" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C114" s="2" t="s">
         <v>221</v>
-      </c>
-      <c r="C114" s="2" t="s">
-        <v>222</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>23</v>
@@ -5501,10 +5507,10 @@
         <v>161</v>
       </c>
       <c r="B115" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="C115" s="2" t="s">
         <v>223</v>
-      </c>
-      <c r="C115" s="2" t="s">
-        <v>224</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>15</v>
@@ -5530,10 +5536,10 @@
         <v>904</v>
       </c>
       <c r="B116" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="C116" s="2" t="s">
         <v>225</v>
-      </c>
-      <c r="C116" s="2" t="s">
-        <v>226</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>15</v>
@@ -5559,7 +5565,7 @@
         <v>3477</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C117" s="2" t="s">
         <v>201</v>
@@ -5588,10 +5594,10 @@
         <v>2106</v>
       </c>
       <c r="B118" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C118" s="2" t="s">
         <v>228</v>
-      </c>
-      <c r="C118" s="2" t="s">
-        <v>229</v>
       </c>
       <c r="D118" s="1" t="s">
         <v>23</v>
@@ -5617,10 +5623,10 @@
         <v>3479</v>
       </c>
       <c r="B119" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C119" s="2" t="s">
         <v>230</v>
-      </c>
-      <c r="C119" s="2" t="s">
-        <v>231</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>15</v>
@@ -5641,7 +5647,7 @@
         <v>45875</v>
       </c>
       <c r="J119" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="120" ht="68" spans="1:9">
@@ -5649,10 +5655,10 @@
         <v>3363</v>
       </c>
       <c r="B120" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C120" s="2" t="s">
         <v>233</v>
-      </c>
-      <c r="C120" s="2" t="s">
-        <v>234</v>
       </c>
       <c r="D120" s="1" t="s">
         <v>23</v>
@@ -5678,10 +5684,10 @@
         <v>808</v>
       </c>
       <c r="B121" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="C121" s="2" t="s">
         <v>235</v>
-      </c>
-      <c r="C121" s="2" t="s">
-        <v>236</v>
       </c>
       <c r="D121" s="1" t="s">
         <v>15</v>
@@ -5710,7 +5716,7 @@
         <v>231</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C122" s="2" t="s">
         <v>105</v>
@@ -5734,7 +5740,7 @@
         <v>45878</v>
       </c>
       <c r="J122" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="123" ht="51" spans="1:9">
@@ -5742,10 +5748,10 @@
         <v>1198</v>
       </c>
       <c r="B123" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="C123" s="2" t="s">
         <v>239</v>
-      </c>
-      <c r="C123" s="2" t="s">
-        <v>240</v>
       </c>
       <c r="D123" s="1" t="s">
         <v>15</v>
@@ -5771,10 +5777,10 @@
         <v>869</v>
       </c>
       <c r="B124" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C124" s="2" t="s">
         <v>241</v>
-      </c>
-      <c r="C124" s="2" t="s">
-        <v>242</v>
       </c>
       <c r="D124" s="1" t="s">
         <v>15</v>
@@ -5800,7 +5806,7 @@
         <v>2438</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D125" s="1" t="s">
         <v>15</v>
@@ -5826,10 +5832,10 @@
         <v>2787</v>
       </c>
       <c r="B126" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C126" s="2" t="s">
         <v>244</v>
-      </c>
-      <c r="C126" s="2" t="s">
-        <v>245</v>
       </c>
       <c r="D126" s="1" t="s">
         <v>15</v>
@@ -5858,7 +5864,7 @@
         <v>326</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C127" s="2" t="s">
         <v>186</v>
@@ -5887,7 +5893,7 @@
         <v>2264</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C128" s="2" t="s">
         <v>71</v>
@@ -5916,10 +5922,10 @@
         <v>303</v>
       </c>
       <c r="B129" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="C129" s="2" t="s">
         <v>248</v>
-      </c>
-      <c r="C129" s="2" t="s">
-        <v>249</v>
       </c>
       <c r="D129" s="1" t="s">
         <v>11</v>
@@ -5945,10 +5951,10 @@
         <v>342</v>
       </c>
       <c r="B130" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C130" s="2" t="s">
         <v>250</v>
-      </c>
-      <c r="C130" s="2" t="s">
-        <v>251</v>
       </c>
       <c r="D130" s="1" t="s">
         <v>11</v>
@@ -5996,7 +6002,7 @@
         <v>679</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H133" s="4">
         <v>45887</v>
@@ -6007,7 +6013,7 @@
         <v>2348</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H134" s="4">
         <v>45888</v>
@@ -6018,10 +6024,10 @@
         <v>1277</v>
       </c>
       <c r="B135" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="C135" s="2" t="s">
         <v>254</v>
-      </c>
-      <c r="C135" s="2" t="s">
-        <v>255</v>
       </c>
       <c r="D135" s="1" t="s">
         <v>15</v>
@@ -6047,7 +6053,7 @@
         <v>1166</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H136" s="4">
         <v>45889</v>
@@ -6061,10 +6067,10 @@
         <v>1504</v>
       </c>
       <c r="B137" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="C137" s="2" t="s">
         <v>257</v>
-      </c>
-      <c r="C137" s="2" t="s">
-        <v>258</v>
       </c>
       <c r="D137" s="1" t="s">
         <v>15</v>
@@ -6090,10 +6096,10 @@
         <v>3195</v>
       </c>
       <c r="B138" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="C138" s="2" t="s">
         <v>259</v>
-      </c>
-      <c r="C138" s="2" t="s">
-        <v>260</v>
       </c>
       <c r="D138" s="1" t="s">
         <v>15</v>
@@ -6131,10 +6137,10 @@
         <v>498</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D142" s="1" t="s">
         <v>15</v>
@@ -6160,7 +6166,7 @@
         <v>3000</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D143" s="1" t="s">
         <v>11</v>
@@ -6186,10 +6192,10 @@
         <v>1181</v>
       </c>
       <c r="B144" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C144" s="2" t="s">
         <v>263</v>
-      </c>
-      <c r="C144" s="2" t="s">
-        <v>264</v>
       </c>
       <c r="D144" s="1" t="s">
         <v>15</v>
@@ -6215,10 +6221,10 @@
         <v>3459</v>
       </c>
       <c r="B145" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="C145" s="2" t="s">
         <v>265</v>
-      </c>
-      <c r="C145" s="2" t="s">
-        <v>266</v>
       </c>
       <c r="D145" s="1" t="s">
         <v>23</v>
@@ -6239,7 +6245,7 @@
         <v>45896</v>
       </c>
       <c r="J145" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="146" ht="17" spans="1:9">
@@ -6247,10 +6253,10 @@
         <v>3446</v>
       </c>
       <c r="B146" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="C146" s="2" t="s">
         <v>268</v>
-      </c>
-      <c r="C146" s="2" t="s">
-        <v>269</v>
       </c>
       <c r="D146" s="1" t="s">
         <v>15</v>
@@ -6276,10 +6282,10 @@
         <v>3021</v>
       </c>
       <c r="B147" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="C147" s="2" t="s">
         <v>270</v>
-      </c>
-      <c r="C147" s="2" t="s">
-        <v>271</v>
       </c>
       <c r="D147" s="1" t="s">
         <v>15</v>
@@ -6305,7 +6311,7 @@
         <v>1182</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C148" s="2" t="s">
         <v>201</v>
@@ -6334,10 +6340,10 @@
         <v>36</v>
       </c>
       <c r="B149" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C149" s="2" t="s">
         <v>273</v>
-      </c>
-      <c r="C149" s="2" t="s">
-        <v>274</v>
       </c>
       <c r="D149" s="1" t="s">
         <v>15</v>
@@ -6363,10 +6369,10 @@
         <v>37</v>
       </c>
       <c r="B150" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="C150" s="2" t="s">
         <v>275</v>
-      </c>
-      <c r="C150" s="2" t="s">
-        <v>276</v>
       </c>
       <c r="D150" s="1" t="s">
         <v>23</v>
@@ -6389,10 +6395,10 @@
         <v>1972</v>
       </c>
       <c r="B151" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="C151" s="2" t="s">
         <v>277</v>
-      </c>
-      <c r="C151" s="2" t="s">
-        <v>278</v>
       </c>
       <c r="D151" s="1" t="s">
         <v>15</v>
@@ -6418,10 +6424,10 @@
         <v>3025</v>
       </c>
       <c r="B152" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="C152" s="2" t="s">
         <v>279</v>
-      </c>
-      <c r="C152" s="2" t="s">
-        <v>280</v>
       </c>
       <c r="D152" s="1" t="s">
         <v>15</v>
@@ -6447,10 +6453,10 @@
         <v>3027</v>
       </c>
       <c r="B153" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="C153" s="2" t="s">
         <v>281</v>
-      </c>
-      <c r="C153" s="2" t="s">
-        <v>282</v>
       </c>
       <c r="D153" s="1" t="s">
         <v>23</v>
@@ -6476,7 +6482,7 @@
         <v>3516</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C154" s="2" t="s">
         <v>186</v>
@@ -6505,10 +6511,10 @@
         <v>2749</v>
       </c>
       <c r="B155" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="C155" s="2" t="s">
         <v>284</v>
-      </c>
-      <c r="C155" s="2" t="s">
-        <v>285</v>
       </c>
       <c r="D155" s="1" t="s">
         <v>15</v>
@@ -6534,10 +6540,10 @@
         <v>567</v>
       </c>
       <c r="B156" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="C156" s="2" t="s">
         <v>286</v>
-      </c>
-      <c r="C156" s="2" t="s">
-        <v>287</v>
       </c>
       <c r="D156" s="1" t="s">
         <v>15</v>
@@ -6556,6 +6562,64 @@
       </c>
       <c r="I156" s="4">
         <v>45905</v>
+      </c>
+    </row>
+    <row r="157" ht="34" spans="1:9">
+      <c r="A157" s="1">
+        <v>1304</v>
+      </c>
+      <c r="B157" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="C157" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="D157" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E157" s="1">
+        <v>1</v>
+      </c>
+      <c r="F157" s="1">
+        <v>0</v>
+      </c>
+      <c r="G157" s="1">
+        <v>3</v>
+      </c>
+      <c r="H157" s="4">
+        <v>45908</v>
+      </c>
+      <c r="I157" s="4">
+        <v>45908</v>
+      </c>
+    </row>
+    <row r="158" ht="51" spans="1:9">
+      <c r="A158" s="1">
+        <v>1317</v>
+      </c>
+      <c r="B158" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="C158" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D158" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E158" s="1">
+        <v>1</v>
+      </c>
+      <c r="F158" s="1">
+        <v>0</v>
+      </c>
+      <c r="G158" s="1">
+        <v>10</v>
+      </c>
+      <c r="H158" s="4">
+        <v>45908</v>
+      </c>
+      <c r="I158" s="4">
+        <v>45908</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add solution for LeetCode problem 3227: Vowels Game in a String and update related markdown documentation
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="26860" windowHeight="14480"/>
+    <workbookView windowWidth="29100" windowHeight="14540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="293">
   <si>
     <t>#</t>
   </si>
@@ -897,6 +897,15 @@
   </si>
   <si>
     <t>Convert Integer to the Sum of Two No-Zero Integers</t>
+  </si>
+  <si>
+    <t>Sort Vowels in a String</t>
+  </si>
+  <si>
+    <t>Vowels Game in a String</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#math #string #greedy </t>
   </si>
 </sst>
 </file>
@@ -2053,10 +2062,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J158"/>
+  <dimension ref="A1:J160"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" topLeftCell="A155" workbookViewId="0">
-      <selection activeCell="G158" sqref="G158"/>
+      <selection activeCell="G156" sqref="G156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -6622,6 +6631,64 @@
         <v>45908</v>
       </c>
     </row>
+    <row r="159" ht="17" spans="1:9">
+      <c r="A159" s="1">
+        <v>2785</v>
+      </c>
+      <c r="B159" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="C159" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D159" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E159" s="1">
+        <v>1</v>
+      </c>
+      <c r="F159" s="1">
+        <v>0</v>
+      </c>
+      <c r="G159" s="1">
+        <v>10</v>
+      </c>
+      <c r="H159" s="4">
+        <v>45912</v>
+      </c>
+      <c r="I159" s="4">
+        <v>45912</v>
+      </c>
+    </row>
+    <row r="160" ht="34" spans="1:9">
+      <c r="A160" s="1">
+        <v>3227</v>
+      </c>
+      <c r="B160" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="C160" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="D160" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E160" s="1">
+        <v>1</v>
+      </c>
+      <c r="F160" s="1">
+        <v>0</v>
+      </c>
+      <c r="G160" s="1">
+        <v>21</v>
+      </c>
+      <c r="H160" s="4">
+        <v>45913</v>
+      </c>
+      <c r="I160" s="4">
+        <v>45913</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Add solution for LeetCode problem 1935: Maximum Number of Words You Can Type and update related markdown documentation
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="29100" windowHeight="14540"/>
+    <workbookView windowHeight="16760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="294">
   <si>
     <t>#</t>
   </si>
@@ -906,6 +906,9 @@
   </si>
   <si>
     <t xml:space="preserve">#math #string #greedy </t>
+  </si>
+  <si>
+    <t>Maximum Number of Words You Can Type</t>
   </si>
 </sst>
 </file>
@@ -2062,10 +2065,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J160"/>
+  <dimension ref="A1:J161"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" topLeftCell="A155" workbookViewId="0">
-      <selection activeCell="G156" sqref="G156"/>
+    <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" topLeftCell="A158" workbookViewId="0">
+      <selection activeCell="I163" sqref="I163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -6689,6 +6692,35 @@
         <v>45913</v>
       </c>
     </row>
+    <row r="161" ht="34" spans="1:9">
+      <c r="A161" s="1">
+        <v>1935</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="C161" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D161" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E161" s="1">
+        <v>1</v>
+      </c>
+      <c r="F161" s="1">
+        <v>0</v>
+      </c>
+      <c r="G161" s="1">
+        <v>3</v>
+      </c>
+      <c r="H161" s="4">
+        <v>45915</v>
+      </c>
+      <c r="I161" s="4">
+        <v>45915</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Add solutions for LeetCode problems 1133: Largest Unique Number, 1150: Check If a Number Is Majority Element in a Sorted Array, and 2197: Replace Non-Coprime Numbers in Array, along with related markdown documentation updates
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="16760"/>
+    <workbookView windowWidth="29100" windowHeight="14540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="299">
   <si>
     <t>#</t>
   </si>
@@ -909,6 +909,21 @@
   </si>
   <si>
     <t>Maximum Number of Words You Can Type</t>
+  </si>
+  <si>
+    <t>Largest Unique Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#array  #hash-table </t>
+  </si>
+  <si>
+    <t>Check If a Number Is Majority Element in a Sorted Array</t>
+  </si>
+  <si>
+    <t>Replace Non-Coprime Numbers in Array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#array #greedy #stack </t>
   </si>
 </sst>
 </file>
@@ -2065,10 +2080,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J161"/>
+  <dimension ref="A1:J164"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" topLeftCell="A158" workbookViewId="0">
-      <selection activeCell="I163" sqref="I163"/>
+    <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" topLeftCell="A161" workbookViewId="0">
+      <selection activeCell="H167" sqref="H167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -6721,6 +6736,93 @@
         <v>45915</v>
       </c>
     </row>
+    <row r="162" ht="34" spans="1:9">
+      <c r="A162" s="1">
+        <v>1133</v>
+      </c>
+      <c r="B162" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="C162" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="D162" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E162" s="1">
+        <v>1</v>
+      </c>
+      <c r="F162" s="1">
+        <v>0</v>
+      </c>
+      <c r="G162" s="1">
+        <v>2</v>
+      </c>
+      <c r="H162" s="4">
+        <v>45915</v>
+      </c>
+      <c r="I162" s="4">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="163" ht="51" spans="1:9">
+      <c r="A163" s="1">
+        <v>1150</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="C163" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D163" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E163" s="1">
+        <v>1</v>
+      </c>
+      <c r="F163" s="1">
+        <v>0</v>
+      </c>
+      <c r="G163" s="1">
+        <v>1</v>
+      </c>
+      <c r="H163" s="4">
+        <v>45915</v>
+      </c>
+      <c r="I163" s="4">
+        <v>45915</v>
+      </c>
+    </row>
+    <row r="164" ht="34" spans="1:9">
+      <c r="A164" s="1">
+        <v>2197</v>
+      </c>
+      <c r="B164" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="C164" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D164" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E164" s="1">
+        <v>0</v>
+      </c>
+      <c r="F164" s="1">
+        <v>1</v>
+      </c>
+      <c r="G164" s="1">
+        <v>45</v>
+      </c>
+      <c r="H164" s="4">
+        <v>45916</v>
+      </c>
+      <c r="I164" s="4">
+        <v>45916</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Add solutions for LeetCode problems 1152: Analyze User Website Visit Pattern and 3005: Count Elements With Maximum Frequency, along with related markdown documentation updates
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="29100" windowHeight="14540"/>
+    <workbookView windowHeight="16740"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="305">
   <si>
     <t>#</t>
   </si>
@@ -924,6 +924,24 @@
   </si>
   <si>
     <t xml:space="preserve">#array #greedy #stack </t>
+  </si>
+  <si>
+    <t>Design a Food Rating System</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#array #string #hash-table #set </t>
+  </si>
+  <si>
+    <t>Count Elements With Maximum Frequency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#array #hash-table #counting </t>
+  </si>
+  <si>
+    <t>Analyze User Website Visit Pattern</t>
+  </si>
+  <si>
+    <t>#array #hash-table #string #permutation #combination</t>
   </si>
 </sst>
 </file>
@@ -2080,10 +2098,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J164"/>
+  <dimension ref="A1:J167"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" topLeftCell="A161" workbookViewId="0">
-      <selection activeCell="H167" sqref="H167"/>
+      <selection activeCell="G171" sqref="G171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -6823,6 +6841,93 @@
         <v>45916</v>
       </c>
     </row>
+    <row r="165" ht="34" spans="1:9">
+      <c r="A165" s="1">
+        <v>2353</v>
+      </c>
+      <c r="B165" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="C165" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="D165" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E165" s="1">
+        <v>0</v>
+      </c>
+      <c r="F165" s="1">
+        <v>1</v>
+      </c>
+      <c r="G165" s="1">
+        <v>23</v>
+      </c>
+      <c r="H165" s="4">
+        <v>45917</v>
+      </c>
+      <c r="I165" s="4">
+        <v>45917</v>
+      </c>
+    </row>
+    <row r="166" ht="34" spans="1:9">
+      <c r="A166" s="1">
+        <v>3005</v>
+      </c>
+      <c r="B166" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="C166" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="D166" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E166" s="1">
+        <v>1</v>
+      </c>
+      <c r="F166" s="1">
+        <v>0</v>
+      </c>
+      <c r="G166" s="1">
+        <v>5</v>
+      </c>
+      <c r="H166" s="4">
+        <v>45922</v>
+      </c>
+      <c r="I166" s="4">
+        <v>45922</v>
+      </c>
+    </row>
+    <row r="167" ht="68" spans="1:9">
+      <c r="A167" s="1">
+        <v>1152</v>
+      </c>
+      <c r="B167" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="C167" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="D167" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E167" s="1">
+        <v>0</v>
+      </c>
+      <c r="F167" s="1">
+        <v>1</v>
+      </c>
+      <c r="G167" s="1">
+        <v>10</v>
+      </c>
+      <c r="H167" s="4">
+        <v>45922</v>
+      </c>
+      <c r="I167" s="4">
+        <v>45922</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Add solution for LeetCode problem 165: Compare Version Numbers and update related markdown documentation
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="307">
   <si>
     <t>#</t>
   </si>
@@ -942,6 +942,12 @@
   </si>
   <si>
     <t>#array #hash-table #string #permutation #combination</t>
+  </si>
+  <si>
+    <t>Compare Version Numbers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#string #two-pointers </t>
   </si>
 </sst>
 </file>
@@ -2098,10 +2104,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J167"/>
+  <dimension ref="A1:J168"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" topLeftCell="A161" workbookViewId="0">
-      <selection activeCell="G171" sqref="G171"/>
+      <selection activeCell="G167" sqref="G167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -6928,6 +6934,35 @@
         <v>45922</v>
       </c>
     </row>
+    <row r="168" ht="34" spans="1:9">
+      <c r="A168" s="1">
+        <v>165</v>
+      </c>
+      <c r="B168" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="C168" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="D168" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E168" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F168" s="1">
+        <v>1</v>
+      </c>
+      <c r="G168" s="1">
+        <v>11</v>
+      </c>
+      <c r="H168" s="4">
+        <v>45923</v>
+      </c>
+      <c r="I168" s="4">
+        <v>45923</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Add solution for LeetCode problem 120: Triangle and update related markdown documentation
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="16740"/>
+    <workbookView windowWidth="29100" windowHeight="14540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="308">
   <si>
     <t>#</t>
   </si>
@@ -948,6 +948,9 @@
   </si>
   <si>
     <t xml:space="preserve">#string #two-pointers </t>
+  </si>
+  <si>
+    <t>Triangle</t>
   </si>
 </sst>
 </file>
@@ -2104,10 +2107,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J168"/>
+  <dimension ref="A1:J169"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" topLeftCell="A161" workbookViewId="0">
-      <selection activeCell="G167" sqref="G167"/>
+    <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" topLeftCell="A164" workbookViewId="0">
+      <selection activeCell="C167" sqref="C167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -6963,6 +6966,35 @@
         <v>45923</v>
       </c>
     </row>
+    <row r="169" ht="34" spans="1:9">
+      <c r="A169" s="1">
+        <v>120</v>
+      </c>
+      <c r="B169" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="C169" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D169" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E169" s="1">
+        <v>0</v>
+      </c>
+      <c r="F169" s="1">
+        <v>1</v>
+      </c>
+      <c r="G169" s="1">
+        <v>20</v>
+      </c>
+      <c r="H169" s="4">
+        <v>45925</v>
+      </c>
+      <c r="I169" s="4">
+        <v>45925</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Add solution for LeetCode problem 611: Valid Triangle Number and update related markdown documentation
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="309">
   <si>
     <t>#</t>
   </si>
@@ -951,6 +951,9 @@
   </si>
   <si>
     <t>Triangle</t>
+  </si>
+  <si>
+    <t>Valid Triangle Number</t>
   </si>
 </sst>
 </file>
@@ -2107,10 +2110,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J169"/>
+  <dimension ref="A1:J171"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" topLeftCell="A164" workbookViewId="0">
-      <selection activeCell="C167" sqref="C167"/>
+      <selection activeCell="J170" sqref="J170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -6995,6 +6998,40 @@
         <v>45925</v>
       </c>
     </row>
+    <row r="170" ht="17" spans="1:9">
+      <c r="A170" s="1">
+        <v>611</v>
+      </c>
+      <c r="B170" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="C170" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="D170" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E170" s="1">
+        <v>1</v>
+      </c>
+      <c r="F170" s="1">
+        <v>0</v>
+      </c>
+      <c r="G170" s="1">
+        <v>5</v>
+      </c>
+      <c r="H170" s="4">
+        <v>45926</v>
+      </c>
+      <c r="I170" s="4">
+        <v>45926</v>
+      </c>
+    </row>
+    <row r="171" ht="17" spans="3:3">
+      <c r="C171" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Add solution for LeetCode problem 1039: Minimum Score Triangulation of Polygon and update related markdown documentation
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="311">
   <si>
     <t>#</t>
   </si>
@@ -954,6 +954,12 @@
   </si>
   <si>
     <t>Valid Triangle Number</t>
+  </si>
+  <si>
+    <t>Minimum Score Triangulation of Polygon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#dynamic-programming #array </t>
   </si>
 </sst>
 </file>
@@ -2112,8 +2118,8 @@
   <sheetPr/>
   <dimension ref="A1:J171"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" topLeftCell="A164" workbookViewId="0">
-      <selection activeCell="J170" sqref="J170"/>
+    <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" topLeftCell="A165" workbookViewId="0">
+      <selection activeCell="D170" sqref="D170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -7027,9 +7033,33 @@
         <v>45926</v>
       </c>
     </row>
-    <row r="171" ht="17" spans="3:3">
+    <row r="171" ht="51" spans="1:9">
+      <c r="A171" s="1">
+        <v>1039</v>
+      </c>
+      <c r="B171" s="2" t="s">
+        <v>309</v>
+      </c>
       <c r="C171" s="2" t="s">
-        <v>201</v>
+        <v>310</v>
+      </c>
+      <c r="D171" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E171" s="1">
+        <v>0</v>
+      </c>
+      <c r="F171" s="1">
+        <v>1</v>
+      </c>
+      <c r="G171" s="1">
+        <v>20</v>
+      </c>
+      <c r="H171" s="4">
+        <v>45929</v>
+      </c>
+      <c r="I171" s="4">
+        <v>45929</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add solutions for LeetCode problems 1121: Divide Array Into Increasing Sequences and 2221: Find Triangular Sum of an Array, along with related markdown documentation updates
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="315">
   <si>
     <t>#</t>
   </si>
@@ -960,6 +960,18 @@
   </si>
   <si>
     <t xml:space="preserve">#dynamic-programming #array </t>
+  </si>
+  <si>
+    <t>Find Triangular Sum of an Array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#array #math #simulation #combination </t>
+  </si>
+  <si>
+    <t>Divide Array Into Increasing Sequences</t>
+  </si>
+  <si>
+    <t>#array #counting</t>
   </si>
 </sst>
 </file>
@@ -2116,10 +2128,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J171"/>
+  <dimension ref="A1:J173"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" topLeftCell="A165" workbookViewId="0">
-      <selection activeCell="D170" sqref="D170"/>
+    <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" topLeftCell="A168" workbookViewId="0">
+      <selection activeCell="C174" sqref="C174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -7062,6 +7074,64 @@
         <v>45929</v>
       </c>
     </row>
+    <row r="172" ht="51" spans="1:9">
+      <c r="A172" s="1">
+        <v>2221</v>
+      </c>
+      <c r="B172" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="C172" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="D172" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E172" s="1">
+        <v>1</v>
+      </c>
+      <c r="F172" s="1">
+        <v>0</v>
+      </c>
+      <c r="G172" s="1">
+        <v>30</v>
+      </c>
+      <c r="H172" s="4">
+        <v>45930</v>
+      </c>
+      <c r="I172" s="4">
+        <v>45930</v>
+      </c>
+    </row>
+    <row r="173" ht="34" spans="1:9">
+      <c r="A173" s="1">
+        <v>1121</v>
+      </c>
+      <c r="B173" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="C173" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="D173" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E173" s="1">
+        <v>0</v>
+      </c>
+      <c r="F173" s="1">
+        <v>1</v>
+      </c>
+      <c r="G173" s="1">
+        <v>20</v>
+      </c>
+      <c r="H173" s="4">
+        <v>45930</v>
+      </c>
+      <c r="I173" s="4">
+        <v>45930</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Add solution for LeetCode problem 1518: Water Bottles and related markdown documentation
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="29100" windowHeight="14540"/>
+    <workbookView windowWidth="28700" windowHeight="14140"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="317">
   <si>
     <t>#</t>
   </si>
@@ -972,6 +972,12 @@
   </si>
   <si>
     <t>#array #counting</t>
+  </si>
+  <si>
+    <t>Water Bottles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#math #simulation </t>
   </si>
 </sst>
 </file>
@@ -2128,10 +2134,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J173"/>
+  <dimension ref="A1:J174"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" topLeftCell="A168" workbookViewId="0">
-      <selection activeCell="C174" sqref="C174"/>
+      <selection activeCell="C176" sqref="C176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -7132,6 +7138,35 @@
         <v>45930</v>
       </c>
     </row>
+    <row r="174" ht="17" spans="1:9">
+      <c r="A174" s="1">
+        <v>1518</v>
+      </c>
+      <c r="B174" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="C174" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="D174" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E174" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F174" s="1">
+        <v>0</v>
+      </c>
+      <c r="G174" s="1">
+        <v>9</v>
+      </c>
+      <c r="H174" s="4">
+        <v>45931</v>
+      </c>
+      <c r="I174" s="4">
+        <v>45931</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Add solution for LeetCode problem 778: Swim in Rising Water and related markdown documentation
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28700" windowHeight="14140"/>
+    <workbookView windowWidth="29100" windowHeight="14540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="319">
   <si>
     <t>#</t>
   </si>
@@ -978,6 +978,12 @@
   </si>
   <si>
     <t xml:space="preserve">#math #simulation </t>
+  </si>
+  <si>
+    <t>Swim in Rising Water</t>
+  </si>
+  <si>
+    <t>#dfs</t>
   </si>
 </sst>
 </file>
@@ -2134,10 +2140,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J174"/>
+  <dimension ref="A1:J175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" topLeftCell="A168" workbookViewId="0">
-      <selection activeCell="C176" sqref="C176"/>
+      <selection activeCell="I175" sqref="I175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -7167,6 +7173,35 @@
         <v>45931</v>
       </c>
     </row>
+    <row r="175" ht="17" spans="1:9">
+      <c r="A175" s="1">
+        <v>778</v>
+      </c>
+      <c r="B175" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="C175" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="D175" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E175" s="1">
+        <v>0</v>
+      </c>
+      <c r="F175" s="1">
+        <v>1</v>
+      </c>
+      <c r="G175" s="1">
+        <v>20</v>
+      </c>
+      <c r="H175" s="4">
+        <v>45936</v>
+      </c>
+      <c r="I175" s="4">
+        <v>45936</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Add solution for LeetCode problem 1135: Connecting Cities With Minimum Cost and related markdown documentation
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="321">
   <si>
     <t>#</t>
   </si>
@@ -984,6 +984,12 @@
   </si>
   <si>
     <t>#dfs</t>
+  </si>
+  <si>
+    <t>Connecting Cities With Minimum Cost</t>
+  </si>
+  <si>
+    <t>#union-find #graph #minimum-spanning-tree</t>
   </si>
 </sst>
 </file>
@@ -2140,10 +2146,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J175"/>
+  <dimension ref="A1:J176"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" topLeftCell="A168" workbookViewId="0">
-      <selection activeCell="I175" sqref="I175"/>
+    <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" topLeftCell="A172" workbookViewId="0">
+      <selection activeCell="H176" sqref="H176:I176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -7202,6 +7208,35 @@
         <v>45936</v>
       </c>
     </row>
+    <row r="176" ht="68" spans="1:9">
+      <c r="A176" s="1">
+        <v>1135</v>
+      </c>
+      <c r="B176" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="C176" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="D176" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E176" s="1">
+        <v>0</v>
+      </c>
+      <c r="F176" s="1">
+        <v>1</v>
+      </c>
+      <c r="G176" s="1">
+        <v>20</v>
+      </c>
+      <c r="H176" s="4">
+        <v>45936</v>
+      </c>
+      <c r="I176" s="4">
+        <v>45936</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Add solutions for LeetCode problems 1488: Avoid Flood in The City, 2300: Successful Pairs of Spells and Potions, and 774: Minimize Max Distance to Gas Station, along with related markdown documentation
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="326">
   <si>
     <t>#</t>
   </si>
@@ -990,6 +990,21 @@
   </si>
   <si>
     <t>#union-find #graph #minimum-spanning-tree</t>
+  </si>
+  <si>
+    <t>Avoid Flood in The City</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#greedy #binary-search </t>
+  </si>
+  <si>
+    <t>Successful Pairs of Spells and Potions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#binary-search #sorting </t>
+  </si>
+  <si>
+    <t>Minimize Max Distance to Gas Station</t>
   </si>
 </sst>
 </file>
@@ -2146,10 +2161,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J176"/>
+  <dimension ref="A1:J179"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" topLeftCell="A172" workbookViewId="0">
-      <selection activeCell="H176" sqref="H176:I176"/>
+      <selection activeCell="H179" sqref="H179:I179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -7237,6 +7252,93 @@
         <v>45936</v>
       </c>
     </row>
+    <row r="177" ht="34" spans="1:9">
+      <c r="A177" s="1">
+        <v>1488</v>
+      </c>
+      <c r="B177" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="C177" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="D177" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E177" s="1">
+        <v>0</v>
+      </c>
+      <c r="F177" s="1">
+        <v>1</v>
+      </c>
+      <c r="G177" s="1">
+        <v>20</v>
+      </c>
+      <c r="H177" s="4">
+        <v>45937</v>
+      </c>
+      <c r="I177" s="4">
+        <v>45937</v>
+      </c>
+    </row>
+    <row r="178" ht="34" spans="1:9">
+      <c r="A178" s="1">
+        <v>2300</v>
+      </c>
+      <c r="B178" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="C178" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="D178" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E178" s="1">
+        <v>1</v>
+      </c>
+      <c r="F178" s="1">
+        <v>0</v>
+      </c>
+      <c r="G178" s="1">
+        <v>21</v>
+      </c>
+      <c r="H178" s="4">
+        <v>45938</v>
+      </c>
+      <c r="I178" s="4">
+        <v>45938</v>
+      </c>
+    </row>
+    <row r="179" ht="34" spans="1:9">
+      <c r="A179" s="1">
+        <v>774</v>
+      </c>
+      <c r="B179" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="C179" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="D179" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E179" s="1">
+        <v>1</v>
+      </c>
+      <c r="F179" s="1">
+        <v>0</v>
+      </c>
+      <c r="G179" s="1">
+        <v>20</v>
+      </c>
+      <c r="H179" s="4">
+        <v>45938</v>
+      </c>
+      <c r="I179" s="4">
+        <v>45938</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Add solutions for LeetCode problems 3349: Adjacent Increasing Subarrays Detection I, 3494: Find the Minimum Amount of Time to Brew Potions, and 8: String to Integer (atoi), along with related markdown documentation
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="331">
   <si>
     <t>#</t>
   </si>
@@ -1005,6 +1005,21 @@
   </si>
   <si>
     <t>Minimize Max Distance to Gas Station</t>
+  </si>
+  <si>
+    <t>Find the Minimum Amount of Time to Brew Potions</t>
+  </si>
+  <si>
+    <t>String to Integer (atoi)</t>
+  </si>
+  <si>
+    <t>#math #string</t>
+  </si>
+  <si>
+    <t>Adjacent Increasing Subarrays Detection I</t>
+  </si>
+  <si>
+    <t>Adjacent Increasing Subarrays Detection II</t>
   </si>
 </sst>
 </file>
@@ -2161,10 +2176,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J179"/>
+  <dimension ref="A1:J183"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" topLeftCell="A172" workbookViewId="0">
-      <selection activeCell="H179" sqref="H179:I179"/>
+    <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" topLeftCell="A178" workbookViewId="0">
+      <selection activeCell="C182" sqref="C182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -7339,6 +7354,119 @@
         <v>45938</v>
       </c>
     </row>
+    <row r="180" ht="51" spans="1:9">
+      <c r="A180" s="1">
+        <v>3494</v>
+      </c>
+      <c r="B180" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="C180" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="D180" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E180" s="1">
+        <v>0</v>
+      </c>
+      <c r="F180" s="1">
+        <v>1</v>
+      </c>
+      <c r="G180" s="1">
+        <v>35</v>
+      </c>
+      <c r="H180" s="4">
+        <v>45939</v>
+      </c>
+      <c r="I180" s="4">
+        <v>45939</v>
+      </c>
+    </row>
+    <row r="181" ht="17" spans="1:9">
+      <c r="A181" s="1">
+        <v>8</v>
+      </c>
+      <c r="B181" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C181" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="D181" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E181" s="1">
+        <v>0</v>
+      </c>
+      <c r="F181" s="1">
+        <v>1</v>
+      </c>
+      <c r="G181" s="1">
+        <v>20</v>
+      </c>
+      <c r="H181" s="4">
+        <v>45943</v>
+      </c>
+      <c r="I181" s="4">
+        <v>45943</v>
+      </c>
+    </row>
+    <row r="182" ht="34" spans="1:9">
+      <c r="A182" s="1">
+        <v>3349</v>
+      </c>
+      <c r="B182" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="C182" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="D182" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E182" s="1">
+        <v>0</v>
+      </c>
+      <c r="F182" s="1">
+        <v>1</v>
+      </c>
+      <c r="H182" s="4">
+        <v>45944</v>
+      </c>
+      <c r="I182" s="4">
+        <v>45944</v>
+      </c>
+    </row>
+    <row r="183" ht="34" spans="1:9">
+      <c r="A183" s="1">
+        <v>3350</v>
+      </c>
+      <c r="B183" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C183" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="D183" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E183" s="1">
+        <v>1</v>
+      </c>
+      <c r="F183" s="1">
+        <v>0</v>
+      </c>
+      <c r="G183" s="1">
+        <v>5</v>
+      </c>
+      <c r="H183" s="4">
+        <v>45945</v>
+      </c>
+      <c r="I183" s="4">
+        <v>45945</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Add solutions for LeetCode problems 24: Swap Nodes in Pairs and 29: Divide Two Integers, along with related markdown documentation
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="29100" windowHeight="14540"/>
+    <workbookView windowWidth="29100" windowHeight="14520"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="334">
   <si>
     <t>#</t>
   </si>
@@ -1020,6 +1020,15 @@
   </si>
   <si>
     <t>Adjacent Increasing Subarrays Detection II</t>
+  </si>
+  <si>
+    <t>Swap Nodes in Pairs</t>
+  </si>
+  <si>
+    <t>Divide Two Integers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#math #binary-search #bit-minipulation </t>
   </si>
 </sst>
 </file>
@@ -2176,10 +2185,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J183"/>
+  <dimension ref="A1:J185"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" topLeftCell="A178" workbookViewId="0">
-      <selection activeCell="C182" sqref="C182"/>
+      <selection activeCell="I185" sqref="I185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -7467,6 +7476,64 @@
         <v>45945</v>
       </c>
     </row>
+    <row r="184" ht="17" spans="1:9">
+      <c r="A184" s="1">
+        <v>24</v>
+      </c>
+      <c r="B184" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="C184" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D184" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E184" s="1">
+        <v>0</v>
+      </c>
+      <c r="F184" s="1">
+        <v>1</v>
+      </c>
+      <c r="G184" s="1">
+        <v>10</v>
+      </c>
+      <c r="H184" s="4">
+        <v>45950</v>
+      </c>
+      <c r="I184" s="4">
+        <v>45950</v>
+      </c>
+    </row>
+    <row r="185" ht="51" spans="1:9">
+      <c r="A185" s="1">
+        <v>29</v>
+      </c>
+      <c r="B185" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="C185" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="D185" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E185" s="1">
+        <v>0</v>
+      </c>
+      <c r="F185" s="1">
+        <v>1</v>
+      </c>
+      <c r="G185" s="1">
+        <v>20</v>
+      </c>
+      <c r="H185" s="4">
+        <v>45950</v>
+      </c>
+      <c r="I185" s="4">
+        <v>45950</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Add solutions for LeetCode problems 1570: Dot Product of Two Sparse Vectors and 3347: Maximum Frequency of an Element After Performing Operations II, along with related markdown documentation
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="29100" windowHeight="14520"/>
+    <workbookView windowWidth="29100" windowHeight="14540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="340">
   <si>
     <t>#</t>
   </si>
@@ -1029,6 +1029,24 @@
   </si>
   <si>
     <t xml:space="preserve">#math #binary-search #bit-minipulation </t>
+  </si>
+  <si>
+    <t>Maximum Frequency of an Element After Performing Operations I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#binary-search  #array #sorting </t>
+  </si>
+  <si>
+    <t>Dot Product of Two Sparse Vectors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#set #hash-table #design </t>
+  </si>
+  <si>
+    <t>Maximum Frequency of an Element After Performing Operations II</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#binary-search #sliding-window #sorting #prefix-sum #array </t>
   </si>
 </sst>
 </file>
@@ -2185,10 +2203,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J185"/>
+  <dimension ref="A1:J188"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" topLeftCell="A178" workbookViewId="0">
-      <selection activeCell="I185" sqref="I185"/>
+    <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" topLeftCell="A185" workbookViewId="0">
+      <selection activeCell="E188" sqref="E188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -7534,6 +7552,93 @@
         <v>45950</v>
       </c>
     </row>
+    <row r="186" ht="51" spans="1:9">
+      <c r="A186" s="1">
+        <v>3346</v>
+      </c>
+      <c r="B186" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="C186" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="D186" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E186" s="1">
+        <v>0</v>
+      </c>
+      <c r="F186" s="1">
+        <v>1</v>
+      </c>
+      <c r="G186" s="1">
+        <v>20</v>
+      </c>
+      <c r="H186" s="4">
+        <v>45951</v>
+      </c>
+      <c r="I186" s="4">
+        <v>45951</v>
+      </c>
+    </row>
+    <row r="187" ht="34" spans="1:9">
+      <c r="A187" s="1">
+        <v>1570</v>
+      </c>
+      <c r="B187" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="C187" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="D187" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E187" s="1">
+        <v>1</v>
+      </c>
+      <c r="F187" s="1">
+        <v>0</v>
+      </c>
+      <c r="G187" s="1">
+        <v>17</v>
+      </c>
+      <c r="H187" s="4">
+        <v>45952</v>
+      </c>
+      <c r="I187" s="4">
+        <v>45952</v>
+      </c>
+    </row>
+    <row r="188" ht="68" spans="1:9">
+      <c r="A188" s="1">
+        <v>3347</v>
+      </c>
+      <c r="B188" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="C188" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="D188" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E188" s="1">
+        <v>0</v>
+      </c>
+      <c r="F188" s="1">
+        <v>1</v>
+      </c>
+      <c r="G188" s="1">
+        <v>55</v>
+      </c>
+      <c r="H188" s="4">
+        <v>45952</v>
+      </c>
+      <c r="I188" s="4">
+        <v>45952</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Add solution for LeetCode problem 3461: Check If Digits Are Equal in String After Operations I, along with related markdown documentation
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="342">
   <si>
     <t>#</t>
   </si>
@@ -1047,6 +1047,12 @@
   </si>
   <si>
     <t xml:space="preserve">#binary-search #sliding-window #sorting #prefix-sum #array </t>
+  </si>
+  <si>
+    <t>Check If Digits Are Equal in String After Operations I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#math #simulation #string </t>
   </si>
 </sst>
 </file>
@@ -2203,10 +2209,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J188"/>
+  <dimension ref="A1:J189"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" topLeftCell="A185" workbookViewId="0">
-      <selection activeCell="E188" sqref="E188"/>
+      <selection activeCell="G189" sqref="G189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -7639,6 +7645,35 @@
         <v>45952</v>
       </c>
     </row>
+    <row r="189" ht="51" spans="1:9">
+      <c r="A189" s="1">
+        <v>3461</v>
+      </c>
+      <c r="B189" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="C189" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="D189" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E189" s="1">
+        <v>1</v>
+      </c>
+      <c r="F189" s="1">
+        <v>0</v>
+      </c>
+      <c r="G189" s="1">
+        <v>5</v>
+      </c>
+      <c r="H189" s="4">
+        <v>45953</v>
+      </c>
+      <c r="I189" s="4">
+        <v>45953</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Add solutions for LeetCode problems 1716: Calculate Money in Leetcode Bank, 2048: Next Greater Numerically Balanced Number, 2125: Number of Laser Beams in a Bank, and 3347: Maximum Frequency of an Element After Performing Operations II, along with related markdown documentation
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="347">
   <si>
     <t>#</t>
   </si>
@@ -1053,6 +1053,21 @@
   </si>
   <si>
     <t xml:space="preserve">#math #simulation #string </t>
+  </si>
+  <si>
+    <t>Next Greater Numerically Balanced Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#math #emueration </t>
+  </si>
+  <si>
+    <t>Calculate Money in Leetcode Bank</t>
+  </si>
+  <si>
+    <t>Number of Laser Beams in a Bank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#string  #greedy </t>
   </si>
 </sst>
 </file>
@@ -2209,10 +2224,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J189"/>
+  <dimension ref="A1:J192"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" topLeftCell="A185" workbookViewId="0">
-      <selection activeCell="G189" sqref="G189"/>
+    <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" topLeftCell="A187" workbookViewId="0">
+      <selection activeCell="E191" sqref="E191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -7674,6 +7689,93 @@
         <v>45953</v>
       </c>
     </row>
+    <row r="190" ht="51" spans="1:9">
+      <c r="A190" s="1">
+        <v>2048</v>
+      </c>
+      <c r="B190" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="C190" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="D190" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E190" s="1">
+        <v>0</v>
+      </c>
+      <c r="F190" s="1">
+        <v>1</v>
+      </c>
+      <c r="G190" s="1">
+        <v>25</v>
+      </c>
+      <c r="H190" s="4">
+        <v>45954</v>
+      </c>
+      <c r="I190" s="4">
+        <v>45954</v>
+      </c>
+    </row>
+    <row r="191" ht="34" spans="1:9">
+      <c r="A191" s="1">
+        <v>1716</v>
+      </c>
+      <c r="B191" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="C191" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D191" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E191" s="1">
+        <v>1</v>
+      </c>
+      <c r="F191" s="1">
+        <v>0</v>
+      </c>
+      <c r="G191" s="1">
+        <v>9</v>
+      </c>
+      <c r="H191" s="4">
+        <v>45955</v>
+      </c>
+      <c r="I191" s="4">
+        <v>45955</v>
+      </c>
+    </row>
+    <row r="192" ht="34" spans="1:9">
+      <c r="A192" s="1">
+        <v>2125</v>
+      </c>
+      <c r="B192" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="C192" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="D192" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E192" s="1">
+        <v>1</v>
+      </c>
+      <c r="F192" s="1">
+        <v>0</v>
+      </c>
+      <c r="G192" s="1">
+        <v>8</v>
+      </c>
+      <c r="H192" s="4">
+        <v>45957</v>
+      </c>
+      <c r="I192" s="4">
+        <v>45957</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Add solutions for LeetCode problems 2464: Minimum Subarrays in a Valid Split, 3354: Make Array Elements Equal to Zero, and 3370: Smallest Number With All Set Bits, along with related markdown documentation
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="29100" windowHeight="14540"/>
+    <workbookView windowWidth="29100" windowHeight="14520"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="351">
   <si>
     <t>#</t>
   </si>
@@ -1068,6 +1068,18 @@
   </si>
   <si>
     <t xml:space="preserve">#string  #greedy </t>
+  </si>
+  <si>
+    <t>Make Array Elements Equal to Zero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#array #prefix-sum #simulation </t>
+  </si>
+  <si>
+    <t>Smallest Number With All Set Bits</t>
+  </si>
+  <si>
+    <t>Minimum Subarrays in a Valid Split</t>
   </si>
 </sst>
 </file>
@@ -2224,10 +2236,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J192"/>
+  <dimension ref="A1:J195"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" topLeftCell="A187" workbookViewId="0">
-      <selection activeCell="E191" sqref="E191"/>
+    <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" topLeftCell="A191" workbookViewId="0">
+      <selection activeCell="G195" sqref="G195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -7776,6 +7788,93 @@
         <v>45957</v>
       </c>
     </row>
+    <row r="193" ht="34" spans="1:9">
+      <c r="A193" s="1">
+        <v>3354</v>
+      </c>
+      <c r="B193" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="C193" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D193" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E193" s="1">
+        <v>1</v>
+      </c>
+      <c r="F193" s="1">
+        <v>0</v>
+      </c>
+      <c r="G193" s="1">
+        <v>7</v>
+      </c>
+      <c r="H193" s="4">
+        <v>45958</v>
+      </c>
+      <c r="I193" s="4">
+        <v>45958</v>
+      </c>
+    </row>
+    <row r="194" ht="34" spans="1:9">
+      <c r="A194" s="1">
+        <v>3370</v>
+      </c>
+      <c r="B194" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="C194" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="D194" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E194" s="1">
+        <v>1</v>
+      </c>
+      <c r="F194" s="1">
+        <v>0</v>
+      </c>
+      <c r="G194" s="1">
+        <v>4</v>
+      </c>
+      <c r="H194" s="4">
+        <v>45959</v>
+      </c>
+      <c r="I194" s="4">
+        <v>45959</v>
+      </c>
+    </row>
+    <row r="195" ht="51" spans="1:9">
+      <c r="A195" s="1">
+        <v>2464</v>
+      </c>
+      <c r="B195" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="C195" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="D195" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E195" s="1">
+        <v>0</v>
+      </c>
+      <c r="F195" s="1">
+        <v>1</v>
+      </c>
+      <c r="G195" s="1">
+        <v>20</v>
+      </c>
+      <c r="H195" s="4">
+        <v>45959</v>
+      </c>
+      <c r="I195" s="4">
+        <v>45959</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Refactor workspace and update notes for LeetCode problems
- Updated workspace.json to reflect changes in opened files and current tab.
- Added new Python solutions for the following problems:
  - 1526. Minimum Number of Increments on Subarrays to Form a Target Array
  - 1578. Minimum Time to Make Rope Colorful
  - 2257. Count Unguarded Cells in the Grid
  - 3217. Delete Nodes From Linked List Present in Array
  - 3289. The Two Sneaky Numbers of Digitville
  - 45. Jump Game II
- Updated corresponding markdown files with problem descriptions, examples, and solutions.
- Removed duplicate entries and cleaned up workspace structure.
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="29100" windowHeight="14520"/>
+    <workbookView windowWidth="29100" windowHeight="14540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="363">
   <si>
     <t>#</t>
   </si>
@@ -1080,6 +1080,42 @@
   </si>
   <si>
     <t>Minimum Subarrays in a Valid Split</t>
+  </si>
+  <si>
+    <t>Count and Say</t>
+  </si>
+  <si>
+    <t>Minimum Number of Increments on Subarrays to Form a Target Array</t>
+  </si>
+  <si>
+    <t>The Two Sneaky Numbers of Digitville</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#array #bit-minipulation #set </t>
+  </si>
+  <si>
+    <t>Jump Game II</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#array #greedy </t>
+  </si>
+  <si>
+    <t>Minimum Time to Make Rope Colorful</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#string #array #greedy </t>
+  </si>
+  <si>
+    <t>Count Unguarded Cells in the Grid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#matrix #simulation </t>
+  </si>
+  <si>
+    <t>Delete Nodes From Linked List Present in Array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#set #linked-list </t>
   </si>
 </sst>
 </file>
@@ -2236,10 +2272,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J195"/>
+  <dimension ref="A1:J202"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" topLeftCell="A191" workbookViewId="0">
-      <selection activeCell="G195" sqref="G195"/>
+    <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" topLeftCell="A194" workbookViewId="0">
+      <selection activeCell="D199" sqref="D199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -7875,6 +7911,209 @@
         <v>45959</v>
       </c>
     </row>
+    <row r="196" ht="17" spans="1:9">
+      <c r="A196" s="1">
+        <v>38</v>
+      </c>
+      <c r="B196" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="C196" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D196" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E196" s="1">
+        <v>0</v>
+      </c>
+      <c r="F196" s="1">
+        <v>1</v>
+      </c>
+      <c r="G196" s="1">
+        <v>20</v>
+      </c>
+      <c r="H196" s="4">
+        <v>45960</v>
+      </c>
+      <c r="I196" s="4">
+        <v>45960</v>
+      </c>
+    </row>
+    <row r="197" ht="51" spans="1:9">
+      <c r="A197" s="1">
+        <v>1526</v>
+      </c>
+      <c r="B197" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="C197" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D197" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E197" s="1">
+        <v>1</v>
+      </c>
+      <c r="F197" s="1">
+        <v>0</v>
+      </c>
+      <c r="G197" s="1">
+        <v>50</v>
+      </c>
+      <c r="H197" s="4">
+        <v>45960</v>
+      </c>
+      <c r="I197" s="4">
+        <v>45960</v>
+      </c>
+    </row>
+    <row r="198" ht="34" spans="1:9">
+      <c r="A198" s="1">
+        <v>3289</v>
+      </c>
+      <c r="B198" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="C198" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="D198" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E198" s="1">
+        <v>1</v>
+      </c>
+      <c r="F198" s="1">
+        <v>0</v>
+      </c>
+      <c r="G198" s="1">
+        <v>5</v>
+      </c>
+      <c r="H198" s="4">
+        <v>45961</v>
+      </c>
+      <c r="I198" s="4">
+        <v>45961</v>
+      </c>
+    </row>
+    <row r="199" ht="17" spans="1:9">
+      <c r="A199" s="1">
+        <v>45</v>
+      </c>
+      <c r="B199" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="C199" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="D199" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E199" s="1">
+        <v>0</v>
+      </c>
+      <c r="F199" s="1">
+        <v>1</v>
+      </c>
+      <c r="G199" s="1">
+        <v>20</v>
+      </c>
+      <c r="H199" s="4">
+        <v>45961</v>
+      </c>
+      <c r="I199" s="4">
+        <v>45961</v>
+      </c>
+    </row>
+    <row r="200" ht="34" spans="1:9">
+      <c r="A200" s="1">
+        <v>1578</v>
+      </c>
+      <c r="B200" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="C200" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="D200" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E200" s="1">
+        <v>1</v>
+      </c>
+      <c r="F200" s="1">
+        <v>1</v>
+      </c>
+      <c r="G200" s="1">
+        <v>20</v>
+      </c>
+      <c r="H200" s="4">
+        <v>44837</v>
+      </c>
+      <c r="I200" s="4">
+        <v>45964</v>
+      </c>
+    </row>
+    <row r="201" ht="34" spans="1:9">
+      <c r="A201" s="1">
+        <v>2257</v>
+      </c>
+      <c r="B201" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="C201" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="D201" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E201" s="1">
+        <v>0</v>
+      </c>
+      <c r="F201" s="1">
+        <v>1</v>
+      </c>
+      <c r="G201" s="1">
+        <v>20</v>
+      </c>
+      <c r="H201" s="4">
+        <v>44837</v>
+      </c>
+      <c r="I201" s="4">
+        <v>45964</v>
+      </c>
+    </row>
+    <row r="202" ht="51" spans="1:9">
+      <c r="A202" s="1">
+        <v>3217</v>
+      </c>
+      <c r="B202" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="C202" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D202" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E202" s="1">
+        <v>1</v>
+      </c>
+      <c r="F202" s="1">
+        <v>0</v>
+      </c>
+      <c r="G202" s="1">
+        <v>8</v>
+      </c>
+      <c r="H202" s="4">
+        <v>44837</v>
+      </c>
+      <c r="I202" s="4">
+        <v>45964</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Add solutions for LeetCode problems 1183: Maximum Number of Ones and 3318: Find X-Sum of All K-Long Subarrays I, along with related markdown documentation and workspace updates.
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="367">
   <si>
     <t>#</t>
   </si>
@@ -1116,6 +1116,18 @@
   </si>
   <si>
     <t xml:space="preserve">#set #linked-list </t>
+  </si>
+  <si>
+    <t>Find X-Sum of All K-Long Subarrays I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#hash-table #sorting #array </t>
+  </si>
+  <si>
+    <t>Maximum Number of Ones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#matrix #greedy #sorting </t>
   </si>
 </sst>
 </file>
@@ -2272,10 +2284,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J202"/>
+  <dimension ref="A1:J204"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" topLeftCell="A194" workbookViewId="0">
-      <selection activeCell="D199" sqref="D199"/>
+    <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" topLeftCell="A199" workbookViewId="0">
+      <selection activeCell="H204" sqref="H204:I204"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -8114,6 +8126,64 @@
         <v>45964</v>
       </c>
     </row>
+    <row r="203" ht="34" spans="1:9">
+      <c r="A203" s="1">
+        <v>3318</v>
+      </c>
+      <c r="B203" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="C203" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="D203" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E203" s="1">
+        <v>0</v>
+      </c>
+      <c r="F203" s="1">
+        <v>1</v>
+      </c>
+      <c r="G203" s="1">
+        <v>18</v>
+      </c>
+      <c r="H203" s="4">
+        <v>44838</v>
+      </c>
+      <c r="I203" s="4">
+        <v>45965</v>
+      </c>
+    </row>
+    <row r="204" ht="34" spans="1:9">
+      <c r="A204" s="1">
+        <v>1183</v>
+      </c>
+      <c r="B204" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="C204" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="D204" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E204" s="1">
+        <v>0</v>
+      </c>
+      <c r="F204" s="1">
+        <v>1</v>
+      </c>
+      <c r="G204" s="1">
+        <v>35</v>
+      </c>
+      <c r="H204" s="4">
+        <v>44838</v>
+      </c>
+      <c r="I204" s="4">
+        <v>45965</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Add solution and documentation for LeetCode problem 170: Two Sum III - Data structure design, including workspace updates.
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="378">
   <si>
     <t>#</t>
   </si>
@@ -1155,6 +1155,12 @@
   </si>
   <si>
     <t>Count Operations to Obtain Zero</t>
+  </si>
+  <si>
+    <t>Two Sum III - Data structure design</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#hash-table #design </t>
   </si>
 </sst>
 </file>
@@ -2311,10 +2317,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J209"/>
+  <dimension ref="A1:J210"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" topLeftCell="A202" workbookViewId="0">
-      <selection activeCell="H209" sqref="H209:I209"/>
+    <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" topLeftCell="A208" workbookViewId="0">
+      <selection activeCell="I210" sqref="I210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -8356,6 +8362,35 @@
         <v>45971</v>
       </c>
     </row>
+    <row r="210" ht="34" spans="1:9">
+      <c r="A210" s="1">
+        <v>170</v>
+      </c>
+      <c r="B210" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="C210" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="D210" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E210" s="1">
+        <v>1</v>
+      </c>
+      <c r="F210" s="1">
+        <v>0</v>
+      </c>
+      <c r="G210" s="1">
+        <v>15</v>
+      </c>
+      <c r="H210" s="4">
+        <v>45972</v>
+      </c>
+      <c r="I210" s="4">
+        <v>45972</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Add solutions and documentation for LeetCode problems 1437: Check If All 1's Are at Least Length K Places Away, 1513: Number of Substrings With Only 1s, and 259: 3Sum Smaller, along with workspace updates.
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="26860" windowHeight="14520"/>
+    <workbookView windowWidth="30860" windowHeight="14520"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="393">
   <si>
     <t>#</t>
   </si>
@@ -1182,6 +1182,30 @@
   </si>
   <si>
     <t>Missing Number</t>
+  </si>
+  <si>
+    <t>Graph Valid Tree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#union-find #bfs #graph #tree </t>
+  </si>
+  <si>
+    <t>Check If All 1's Are at Least Length K Places Away</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#array #counting </t>
+  </si>
+  <si>
+    <t>Number of Substrings With Only 1s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#string #counting </t>
+  </si>
+  <si>
+    <t>3Sum Smaller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#two-pointers #sorting #binary-search </t>
   </si>
 </sst>
 </file>
@@ -2338,10 +2362,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J214"/>
+  <dimension ref="A1:J218"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" topLeftCell="A209" workbookViewId="0">
-      <selection activeCell="A214" sqref="A214"/>
+    <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" topLeftCell="A213" workbookViewId="0">
+      <selection activeCell="I219" sqref="I219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -8528,6 +8552,122 @@
         <v>45974</v>
       </c>
     </row>
+    <row r="215" ht="34" spans="1:9">
+      <c r="A215" s="1">
+        <v>261</v>
+      </c>
+      <c r="B215" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="C215" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="D215" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E215" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F215" s="1">
+        <v>0</v>
+      </c>
+      <c r="G215" s="1">
+        <v>25</v>
+      </c>
+      <c r="H215" s="4">
+        <v>45974</v>
+      </c>
+      <c r="I215" s="4">
+        <v>45974</v>
+      </c>
+    </row>
+    <row r="216" ht="51" spans="1:9">
+      <c r="A216" s="1">
+        <v>1437</v>
+      </c>
+      <c r="B216" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="C216" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="D216" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E216" s="1">
+        <v>1</v>
+      </c>
+      <c r="F216" s="1">
+        <v>0</v>
+      </c>
+      <c r="G216" s="1">
+        <v>20</v>
+      </c>
+      <c r="H216" s="4">
+        <v>45978</v>
+      </c>
+      <c r="I216" s="4">
+        <v>45978</v>
+      </c>
+    </row>
+    <row r="217" ht="34" spans="1:9">
+      <c r="A217" s="1">
+        <v>1513</v>
+      </c>
+      <c r="B217" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="C217" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="D217" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E217" s="1">
+        <v>1</v>
+      </c>
+      <c r="F217" s="1">
+        <v>0</v>
+      </c>
+      <c r="G217" s="1">
+        <v>5</v>
+      </c>
+      <c r="H217" s="4">
+        <v>45978</v>
+      </c>
+      <c r="I217" s="4">
+        <v>45978</v>
+      </c>
+    </row>
+    <row r="218" ht="51" spans="1:9">
+      <c r="A218" s="1">
+        <v>259</v>
+      </c>
+      <c r="B218" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="C218" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="D218" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E218" s="1">
+        <v>0</v>
+      </c>
+      <c r="F218" s="1">
+        <v>1</v>
+      </c>
+      <c r="G218" s="1">
+        <v>25</v>
+      </c>
+      <c r="H218" s="4">
+        <v>45979</v>
+      </c>
+      <c r="I218" s="4">
+        <v>45979</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Add solutions and documentation for LeetCode problems 2154: Keep Multiplying Found Values by Two, 717: 1-bit and 2-bit Characters, and 757: Set Intersection Size At Least Two; update workspace and notes
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="30860" windowHeight="14520"/>
+    <workbookView windowHeight="16640"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="398">
   <si>
     <t>#</t>
   </si>
@@ -1206,6 +1206,21 @@
   </si>
   <si>
     <t xml:space="preserve">#two-pointers #sorting #binary-search </t>
+  </si>
+  <si>
+    <t>1-bit and 2-bit Characters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#array #math </t>
+  </si>
+  <si>
+    <t>Keep Multiplying Found Values by Two</t>
+  </si>
+  <si>
+    <t>Set Intersection Size At Least Two</t>
+  </si>
+  <si>
+    <t>#array #intervals</t>
   </si>
 </sst>
 </file>
@@ -2362,10 +2377,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J218"/>
+  <dimension ref="A1:J221"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" topLeftCell="A213" workbookViewId="0">
-      <selection activeCell="I219" sqref="I219"/>
+      <selection activeCell="F215" sqref="F215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -8668,6 +8683,93 @@
         <v>45979</v>
       </c>
     </row>
+    <row r="219" ht="34" spans="1:9">
+      <c r="A219" s="1">
+        <v>717</v>
+      </c>
+      <c r="B219" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="C219" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="D219" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E219" s="1">
+        <v>0</v>
+      </c>
+      <c r="F219" s="1">
+        <v>1</v>
+      </c>
+      <c r="G219" s="1">
+        <v>25</v>
+      </c>
+      <c r="H219" s="4">
+        <v>45980</v>
+      </c>
+      <c r="I219" s="4">
+        <v>45980</v>
+      </c>
+    </row>
+    <row r="220" ht="34" spans="1:9">
+      <c r="A220" s="1">
+        <v>2154</v>
+      </c>
+      <c r="B220" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="C220" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="D220" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E220" s="1">
+        <v>0</v>
+      </c>
+      <c r="F220" s="1">
+        <v>1</v>
+      </c>
+      <c r="G220" s="1">
+        <v>5</v>
+      </c>
+      <c r="H220" s="4">
+        <v>45980</v>
+      </c>
+      <c r="I220" s="4">
+        <v>45980</v>
+      </c>
+    </row>
+    <row r="221" ht="34" spans="1:9">
+      <c r="A221" s="1">
+        <v>757</v>
+      </c>
+      <c r="B221" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="C221" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="D221" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E221" s="1">
+        <v>0</v>
+      </c>
+      <c r="F221" s="1">
+        <v>1</v>
+      </c>
+      <c r="G221" s="1">
+        <v>55</v>
+      </c>
+      <c r="H221" s="4">
+        <v>45981</v>
+      </c>
+      <c r="I221" s="4">
+        <v>45981</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Add solution and documentation for LeetCode problem 1930: Unique Length-3 Palindromic Subsequences; update workspace and notes
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="16640"/>
+    <workbookView windowWidth="29100" windowHeight="14620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="400">
   <si>
     <t>#</t>
   </si>
@@ -1221,6 +1221,12 @@
   </si>
   <si>
     <t>#array #intervals</t>
+  </si>
+  <si>
+    <t>Unique Length-3 Palindromic Subsequences</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#palindrom #string #set </t>
   </si>
 </sst>
 </file>
@@ -2377,10 +2383,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J221"/>
+  <dimension ref="A1:J222"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" topLeftCell="A213" workbookViewId="0">
-      <selection activeCell="F215" sqref="F215"/>
+    <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" topLeftCell="A216" workbookViewId="0">
+      <selection activeCell="J222" sqref="J222"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -8770,6 +8776,35 @@
         <v>45981</v>
       </c>
     </row>
+    <row r="222" ht="51" spans="1:9">
+      <c r="A222" s="1">
+        <v>1930</v>
+      </c>
+      <c r="B222" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="C222" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="D222" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E222" s="1">
+        <v>0</v>
+      </c>
+      <c r="F222" s="1">
+        <v>1</v>
+      </c>
+      <c r="G222" s="1">
+        <v>25</v>
+      </c>
+      <c r="H222" s="4">
+        <v>45982</v>
+      </c>
+      <c r="I222" s="4">
+        <v>45982</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Add solutions and documentation for LeetCode problems 1018: Binary Prefix Divisible By 5, 1262: Greatest Sum Divisible by Three, 3190: Find Minimum Operations to Make All Elements Divisible by Three, and 364: Nested List Weight Sum II; update workspace and notes
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="406">
   <si>
     <t>#</t>
   </si>
@@ -1227,6 +1227,24 @@
   </si>
   <si>
     <t xml:space="preserve">#palindrom #string #set </t>
+  </si>
+  <si>
+    <t>Find Minimum Operations to Make All Elements Divisible by Three</t>
+  </si>
+  <si>
+    <t>Greatest Sum Divisible by Three</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#array #greedy #dynamic-programming #sorting </t>
+  </si>
+  <si>
+    <t>Binary Prefix Divisible By 5</t>
+  </si>
+  <si>
+    <t>Nested List Weight Sum II</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#bfs #dfs #deque #queue </t>
   </si>
 </sst>
 </file>
@@ -2383,10 +2401,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J222"/>
+  <dimension ref="A1:J226"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" topLeftCell="A216" workbookViewId="0">
-      <selection activeCell="J222" sqref="J222"/>
+    <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" topLeftCell="A222" workbookViewId="0">
+      <selection activeCell="J226" sqref="J226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -8805,6 +8823,122 @@
         <v>45982</v>
       </c>
     </row>
+    <row r="223" ht="68" spans="1:9">
+      <c r="A223" s="1">
+        <v>3190</v>
+      </c>
+      <c r="B223" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="C223" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="D223" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E223" s="1">
+        <v>1</v>
+      </c>
+      <c r="F223" s="1">
+        <v>0</v>
+      </c>
+      <c r="G223" s="1">
+        <v>2</v>
+      </c>
+      <c r="H223" s="4">
+        <v>45983</v>
+      </c>
+      <c r="I223" s="4">
+        <v>45983</v>
+      </c>
+    </row>
+    <row r="224" ht="68" spans="1:9">
+      <c r="A224" s="1">
+        <v>1262</v>
+      </c>
+      <c r="B224" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="C224" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="D224" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E224" s="1">
+        <v>0</v>
+      </c>
+      <c r="F224" s="1">
+        <v>1</v>
+      </c>
+      <c r="G224" s="1">
+        <v>55</v>
+      </c>
+      <c r="H224" s="4">
+        <v>45984</v>
+      </c>
+      <c r="I224" s="4">
+        <v>45984</v>
+      </c>
+    </row>
+    <row r="225" ht="34" spans="1:9">
+      <c r="A225" s="1">
+        <v>1018</v>
+      </c>
+      <c r="B225" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="C225" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="D225" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E225" s="1">
+        <v>1</v>
+      </c>
+      <c r="F225" s="1">
+        <v>0</v>
+      </c>
+      <c r="G225" s="1">
+        <v>5</v>
+      </c>
+      <c r="H225" s="4">
+        <v>45985</v>
+      </c>
+      <c r="I225" s="4">
+        <v>45985</v>
+      </c>
+    </row>
+    <row r="226" ht="34" spans="1:9">
+      <c r="A226" s="1">
+        <v>364</v>
+      </c>
+      <c r="B226" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="C226" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="D226" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E226" s="1">
+        <v>1</v>
+      </c>
+      <c r="F226" s="1">
+        <v>0</v>
+      </c>
+      <c r="G226" s="1">
+        <v>24</v>
+      </c>
+      <c r="H226" s="4">
+        <v>45986</v>
+      </c>
+      <c r="I226" s="4">
+        <v>45986</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Add solution and documentation for LeetCode problem 1015: Smallest Integer Divisible by K; update workspace and notes
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="407">
   <si>
     <t>#</t>
   </si>
@@ -1245,6 +1245,9 @@
   </si>
   <si>
     <t xml:space="preserve">#bfs #dfs #deque #queue </t>
+  </si>
+  <si>
+    <t>Smallest Integer Divisible by K</t>
   </si>
 </sst>
 </file>
@@ -2401,10 +2404,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J226"/>
+  <dimension ref="A1:J227"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" topLeftCell="A222" workbookViewId="0">
-      <selection activeCell="J226" sqref="J226"/>
+      <selection activeCell="D224" sqref="D224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -8939,6 +8942,35 @@
         <v>45986</v>
       </c>
     </row>
+    <row r="227" ht="34" spans="1:9">
+      <c r="A227" s="1">
+        <v>1015</v>
+      </c>
+      <c r="B227" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="C227" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D227" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E227" s="1">
+        <v>0</v>
+      </c>
+      <c r="F227" s="1">
+        <v>2</v>
+      </c>
+      <c r="G227" s="1">
+        <v>25</v>
+      </c>
+      <c r="H227" s="4">
+        <v>44559</v>
+      </c>
+      <c r="I227" s="4">
+        <v>45986</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Add solution and documentation for LeetCode problem 2435: Paths in Matrix Whose Sum Is Divisible by K; update workspace and notes
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="29100" windowHeight="14620"/>
+    <workbookView windowHeight="16640"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="409">
   <si>
     <t>#</t>
   </si>
@@ -1248,6 +1248,12 @@
   </si>
   <si>
     <t>Smallest Integer Divisible by K</t>
+  </si>
+  <si>
+    <t>Paths in Matrix Whose Sum Is Divisible by K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#greedy #matrix #dynamic-programming  </t>
   </si>
 </sst>
 </file>
@@ -2404,10 +2410,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J227"/>
+  <dimension ref="A1:J228"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" topLeftCell="A222" workbookViewId="0">
-      <selection activeCell="D224" sqref="D224"/>
+      <selection activeCell="J226" sqref="J226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -8971,6 +8977,35 @@
         <v>45986</v>
       </c>
     </row>
+    <row r="228" ht="51" spans="1:9">
+      <c r="A228" s="1">
+        <v>2435</v>
+      </c>
+      <c r="B228" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="C228" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="D228" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E228" s="1">
+        <v>0</v>
+      </c>
+      <c r="F228" s="1">
+        <v>1</v>
+      </c>
+      <c r="G228" s="1">
+        <v>55</v>
+      </c>
+      <c r="H228" s="4">
+        <v>45987</v>
+      </c>
+      <c r="I228" s="4">
+        <v>45987</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Add solution and documentation for LeetCode problem 3381: Maximum Subarray Sum With Length Divisible by K; update workspace and notes
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="411">
   <si>
     <t>#</t>
   </si>
@@ -1254,6 +1254,12 @@
   </si>
   <si>
     <t xml:space="preserve">#greedy #matrix #dynamic-programming  </t>
+  </si>
+  <si>
+    <t>Maximum Subarray Sum With Length Divisible by K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#prefix-sum #array #divide </t>
   </si>
 </sst>
 </file>
@@ -2410,10 +2416,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J228"/>
+  <dimension ref="A1:J229"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" topLeftCell="A222" workbookViewId="0">
-      <selection activeCell="J226" sqref="J226"/>
+      <selection activeCell="A229" sqref="A229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -9006,6 +9012,35 @@
         <v>45987</v>
       </c>
     </row>
+    <row r="229" ht="51" spans="1:9">
+      <c r="A229" s="1">
+        <v>3381</v>
+      </c>
+      <c r="B229" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="C229" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="D229" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E229" s="1">
+        <v>0</v>
+      </c>
+      <c r="F229" s="1">
+        <v>1</v>
+      </c>
+      <c r="G229" s="1">
+        <v>35</v>
+      </c>
+      <c r="H229" s="4">
+        <v>45988</v>
+      </c>
+      <c r="I229" s="4">
+        <v>45988</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Add solution and documentation for LeetCode problem 2872: Maximum Number of K-Divisible Components; update workspace and notes
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="413">
   <si>
     <t>#</t>
   </si>
@@ -1260,6 +1260,12 @@
   </si>
   <si>
     <t xml:space="preserve">#prefix-sum #array #divide </t>
+  </si>
+  <si>
+    <t>Maximum Number of K-Divisible Components</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#tree #graph #dfs #bfs #set </t>
   </si>
 </sst>
 </file>
@@ -2416,10 +2422,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J229"/>
+  <dimension ref="A1:J230"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" topLeftCell="A222" workbookViewId="0">
-      <selection activeCell="A229" sqref="A229"/>
+    <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" topLeftCell="A225" workbookViewId="0">
+      <selection activeCell="C231" sqref="C231"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -9041,6 +9047,35 @@
         <v>45988</v>
       </c>
     </row>
+    <row r="230" ht="34" spans="1:9">
+      <c r="A230" s="1">
+        <v>2872</v>
+      </c>
+      <c r="B230" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="C230" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D230" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E230" s="1">
+        <v>0</v>
+      </c>
+      <c r="F230" s="1">
+        <v>1</v>
+      </c>
+      <c r="G230" s="1">
+        <v>30</v>
+      </c>
+      <c r="H230" s="4">
+        <v>45989</v>
+      </c>
+      <c r="I230" s="4">
+        <v>45989</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Add solutions and documentation for LeetCode problems 1214: Two Sum BSTs, 1590: Make Sum Divisible by P, 2141: Maximum Running Time of N Computers, 370: Range Addition, and 3623: Count Number of Trapezoids I; update workspace and notes
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="421">
   <si>
     <t>#</t>
   </si>
@@ -1266,6 +1266,30 @@
   </si>
   <si>
     <t xml:space="preserve">#tree #graph #dfs #bfs #set </t>
+  </si>
+  <si>
+    <t>Range Addition</t>
+  </si>
+  <si>
+    <t>Make Sum Divisible by P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#array #prefix-sum #divide </t>
+  </si>
+  <si>
+    <t>Maximum Running Time of N Computers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#array #binary-search #greedy </t>
+  </si>
+  <si>
+    <t>Count Number of Trapezoids I</t>
+  </si>
+  <si>
+    <t>Two Sum BSTs</t>
+  </si>
+  <si>
+    <t>#binary-tree #bst #bfs #dfs #morris</t>
   </si>
 </sst>
 </file>
@@ -2422,10 +2446,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J230"/>
+  <dimension ref="A1:J235"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" topLeftCell="A225" workbookViewId="0">
-      <selection activeCell="C231" sqref="C231"/>
+      <selection activeCell="H235" sqref="H235:I235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -9076,6 +9100,148 @@
         <v>45989</v>
       </c>
     </row>
+    <row r="231" ht="17" spans="1:9">
+      <c r="A231" s="1">
+        <v>370</v>
+      </c>
+      <c r="B231" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="C231" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="D231" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E231" s="1">
+        <v>0</v>
+      </c>
+      <c r="F231" s="1">
+        <v>1</v>
+      </c>
+      <c r="G231" s="1">
+        <v>30</v>
+      </c>
+      <c r="H231" s="4">
+        <v>45990</v>
+      </c>
+      <c r="I231" s="4">
+        <v>45990</v>
+      </c>
+    </row>
+    <row r="232" ht="34" spans="1:9">
+      <c r="A232" s="1">
+        <v>1590</v>
+      </c>
+      <c r="B232" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="C232" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="D232" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E232" s="1">
+        <v>0</v>
+      </c>
+      <c r="F232" s="1">
+        <v>1</v>
+      </c>
+      <c r="G232" s="1">
+        <v>25</v>
+      </c>
+      <c r="H232" s="4">
+        <v>45991</v>
+      </c>
+      <c r="I232" s="4">
+        <v>45991</v>
+      </c>
+    </row>
+    <row r="233" ht="34" spans="1:9">
+      <c r="A233" s="1">
+        <v>2141</v>
+      </c>
+      <c r="B233" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="C233" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="D233" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E233" s="1">
+        <v>0</v>
+      </c>
+      <c r="F233" s="1">
+        <v>1</v>
+      </c>
+      <c r="G233" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="H233" s="4">
+        <v>45992</v>
+      </c>
+      <c r="I233" s="4">
+        <v>45992</v>
+      </c>
+    </row>
+    <row r="234" ht="34" spans="1:9">
+      <c r="A234" s="1">
+        <v>3623</v>
+      </c>
+      <c r="B234" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="D234" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E234" s="1">
+        <v>0</v>
+      </c>
+      <c r="F234" s="1">
+        <v>1</v>
+      </c>
+      <c r="G234" s="1">
+        <v>45</v>
+      </c>
+      <c r="H234" s="4">
+        <v>45993</v>
+      </c>
+      <c r="I234" s="4">
+        <v>45993</v>
+      </c>
+    </row>
+    <row r="235" ht="34" spans="1:9">
+      <c r="A235" s="1">
+        <v>1214</v>
+      </c>
+      <c r="B235" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="C235" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="D235" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E235" s="1">
+        <v>1</v>
+      </c>
+      <c r="F235" s="1">
+        <v>0</v>
+      </c>
+      <c r="G235" s="1">
+        <v>16</v>
+      </c>
+      <c r="H235" s="4">
+        <v>45993</v>
+      </c>
+      <c r="I235" s="4">
+        <v>45993</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Add solutions and documentation for LeetCode problems 2211: Count Collisions on a Road, 242: Valid Anagram, 424: Longest Repeating Character Replacement, and 3625: Count Number of Trapezoids II; update workspace and notes
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="429">
   <si>
     <t>#</t>
   </si>
@@ -1290,6 +1290,30 @@
   </si>
   <si>
     <t>#binary-tree #bst #bfs #dfs #morris</t>
+  </si>
+  <si>
+    <t>Count Number of Trapezoids II</t>
+  </si>
+  <si>
+    <t>55??</t>
+  </si>
+  <si>
+    <t>Valid Anagram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#hash-table </t>
+  </si>
+  <si>
+    <t>Count Collisions on a Road</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#string #array #simulation </t>
+  </si>
+  <si>
+    <t>Longest Repeating Character Replacement</t>
+  </si>
+  <si>
+    <t>75??</t>
   </si>
 </sst>
 </file>
@@ -2446,10 +2470,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J235"/>
+  <dimension ref="A1:J239"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" topLeftCell="A225" workbookViewId="0">
-      <selection activeCell="H235" sqref="H235:I235"/>
+    <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" topLeftCell="A232" workbookViewId="0">
+      <selection activeCell="H239" sqref="H239:I239"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -9242,6 +9266,119 @@
         <v>45993</v>
       </c>
     </row>
+    <row r="236" ht="34" spans="1:9">
+      <c r="A236" s="1">
+        <v>3625</v>
+      </c>
+      <c r="B236" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D236" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E236" s="1">
+        <v>0</v>
+      </c>
+      <c r="F236" s="1">
+        <v>1</v>
+      </c>
+      <c r="G236" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="H236" s="4">
+        <v>45994</v>
+      </c>
+      <c r="I236" s="4">
+        <v>45994</v>
+      </c>
+    </row>
+    <row r="237" ht="17" spans="1:9">
+      <c r="A237" s="1">
+        <v>242</v>
+      </c>
+      <c r="B237" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="C237" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="D237" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E237" s="1">
+        <v>1</v>
+      </c>
+      <c r="F237" s="1">
+        <v>0</v>
+      </c>
+      <c r="G237" s="1">
+        <v>5</v>
+      </c>
+      <c r="H237" s="4">
+        <v>45994</v>
+      </c>
+      <c r="I237" s="4">
+        <v>45994</v>
+      </c>
+    </row>
+    <row r="238" ht="34" spans="1:9">
+      <c r="A238" s="1">
+        <v>2211</v>
+      </c>
+      <c r="B238" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="C238" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="D238" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E238" s="1">
+        <v>0</v>
+      </c>
+      <c r="F238" s="1">
+        <v>1</v>
+      </c>
+      <c r="G238" s="1">
+        <v>45</v>
+      </c>
+      <c r="H238" s="4">
+        <v>45995</v>
+      </c>
+      <c r="I238" s="4">
+        <v>45995</v>
+      </c>
+    </row>
+    <row r="239" ht="34" spans="1:9">
+      <c r="A239" s="1">
+        <v>424</v>
+      </c>
+      <c r="B239" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="C239" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="D239" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E239" s="1">
+        <v>0</v>
+      </c>
+      <c r="F239" s="1">
+        <v>1</v>
+      </c>
+      <c r="G239" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="H239" s="4">
+        <v>45995</v>
+      </c>
+      <c r="I239" s="4">
+        <v>45995</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Refactor workspace and update notes for various LeetCode problems
- Updated workspace.json to reflect changes in opened files and current tabs.
- Replaced the file for problem 2211 with 3578 in workspace.
- Added new Python solution files for problems 152, 1925, 198, 3432, and 3578.
- Created markdown notes for problems 152, 1925, 198, 3432, and 3578 with problem descriptions, examples, and solutions.
- Updated tags and companies in markdown files for better categorization.
- Modified existing markdown files to improve clarity and consistency.
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="437">
   <si>
     <t>#</t>
   </si>
@@ -1314,6 +1314,30 @@
   </si>
   <si>
     <t>75??</t>
+  </si>
+  <si>
+    <t>Count Partitions with Even Sum Difference</t>
+  </si>
+  <si>
+    <t>House Robber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#array #dynamic-programming  </t>
+  </si>
+  <si>
+    <t>Maximum Product Subarray</t>
+  </si>
+  <si>
+    <t>Count Partitions With Max-Min Difference at Most K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#sliding-window #dynamic-programming </t>
+  </si>
+  <si>
+    <t>Count Odd Numbers in an Interval Range</t>
+  </si>
+  <si>
+    <t>Count Square Sum Triples</t>
   </si>
 </sst>
 </file>
@@ -2470,10 +2494,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J239"/>
+  <dimension ref="A1:J245"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" topLeftCell="A232" workbookViewId="0">
-      <selection activeCell="H239" sqref="H239:I239"/>
+    <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" topLeftCell="A241" workbookViewId="0">
+      <selection activeCell="A248" sqref="A248"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -9379,6 +9403,180 @@
         <v>45995</v>
       </c>
     </row>
+    <row r="240" ht="34" spans="1:9">
+      <c r="A240" s="1">
+        <v>3432</v>
+      </c>
+      <c r="B240" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="C240" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="D240" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E240" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F240" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="G240" s="1">
+        <v>5</v>
+      </c>
+      <c r="H240" s="4">
+        <v>45996</v>
+      </c>
+      <c r="I240" s="4">
+        <v>45996</v>
+      </c>
+    </row>
+    <row r="241" ht="34" spans="1:9">
+      <c r="A241" s="1">
+        <v>198</v>
+      </c>
+      <c r="B241" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="C241" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="D241" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E241" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F241" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="G241" s="1">
+        <v>8</v>
+      </c>
+      <c r="H241" s="4">
+        <v>45996</v>
+      </c>
+      <c r="I241" s="4">
+        <v>45996</v>
+      </c>
+    </row>
+    <row r="242" ht="34" spans="1:9">
+      <c r="A242" s="1">
+        <v>152</v>
+      </c>
+      <c r="B242" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="C242" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D242" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E242" s="1">
+        <v>0</v>
+      </c>
+      <c r="F242" s="1">
+        <v>1</v>
+      </c>
+      <c r="G242" s="1">
+        <v>50</v>
+      </c>
+      <c r="H242" s="4">
+        <v>45996</v>
+      </c>
+      <c r="I242" s="4">
+        <v>45996</v>
+      </c>
+    </row>
+    <row r="243" ht="51" spans="1:9">
+      <c r="A243" s="1">
+        <v>3578</v>
+      </c>
+      <c r="B243" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="C243" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="D243" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E243" s="1">
+        <v>0</v>
+      </c>
+      <c r="F243" s="1">
+        <v>0</v>
+      </c>
+      <c r="G243" s="1">
+        <v>40</v>
+      </c>
+      <c r="H243" s="4">
+        <v>45997</v>
+      </c>
+      <c r="I243" s="4">
+        <v>45997</v>
+      </c>
+    </row>
+    <row r="244" ht="34" spans="1:9">
+      <c r="A244" s="1">
+        <v>1523</v>
+      </c>
+      <c r="B244" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="C244" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D244" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E244" s="1">
+        <v>1</v>
+      </c>
+      <c r="F244" s="1">
+        <v>0</v>
+      </c>
+      <c r="G244" s="1">
+        <v>3</v>
+      </c>
+      <c r="H244" s="4">
+        <v>45998</v>
+      </c>
+      <c r="I244" s="4">
+        <v>45998</v>
+      </c>
+    </row>
+    <row r="245" ht="34" spans="1:9">
+      <c r="A245" s="1">
+        <v>1925</v>
+      </c>
+      <c r="B245" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="C245" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D245" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E245" s="1">
+        <v>1</v>
+      </c>
+      <c r="F245" s="1">
+        <v>0</v>
+      </c>
+      <c r="G245" s="1">
+        <v>3</v>
+      </c>
+      <c r="H245" s="4">
+        <v>45999</v>
+      </c>
+      <c r="I245" s="4">
+        <v>45999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Add solutions and documentation for LeetCode problems 1874: Minimize Product Sum of Two Arrays, 3577: Count the Number of Computer Unlocking Permutations, and 3583: Count Special Triplets; update workspace and notes
</commit_message>
<xml_diff>
--- a/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
+++ b/Obsidian Vault/刷题笔记 - 记录/刷题记录表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="442">
   <si>
     <t>#</t>
   </si>
@@ -1338,6 +1338,21 @@
   </si>
   <si>
     <t>Count Square Sum Triples</t>
+  </si>
+  <si>
+    <t>Count Special Triplets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#array #hash-table </t>
+  </si>
+  <si>
+    <t>Count the Number of Computer Unlocking Permutations</t>
+  </si>
+  <si>
+    <t>Minimize Product Sum of Two Arrays</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#math #array </t>
   </si>
 </sst>
 </file>
@@ -2494,10 +2509,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J245"/>
+  <dimension ref="A1:J249"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" topLeftCell="A241" workbookViewId="0">
-      <selection activeCell="A248" sqref="A248"/>
+      <selection activeCell="H249" sqref="H249:I249"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -9577,6 +9592,101 @@
         <v>45999</v>
       </c>
     </row>
+    <row r="246" ht="17" spans="1:9">
+      <c r="A246" s="1">
+        <v>3583</v>
+      </c>
+      <c r="B246" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="C246" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="D246" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E246" s="1">
+        <v>0</v>
+      </c>
+      <c r="F246" s="1">
+        <v>1</v>
+      </c>
+      <c r="G246" s="1">
+        <v>30</v>
+      </c>
+      <c r="H246" s="4">
+        <v>46000</v>
+      </c>
+      <c r="I246" s="4">
+        <v>46000</v>
+      </c>
+    </row>
+    <row r="247" ht="51" spans="1:9">
+      <c r="A247" s="1">
+        <v>3577</v>
+      </c>
+      <c r="B247" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="C247" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="D247" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E247" s="1">
+        <v>1</v>
+      </c>
+      <c r="F247" s="1">
+        <v>0</v>
+      </c>
+      <c r="G247" s="1">
+        <v>10</v>
+      </c>
+      <c r="H247" s="4">
+        <v>46001</v>
+      </c>
+      <c r="I247" s="4">
+        <v>46001</v>
+      </c>
+    </row>
+    <row r="248" ht="34" spans="1:9">
+      <c r="A248" s="1">
+        <v>1874</v>
+      </c>
+      <c r="B248" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="C248" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="D248" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E248" s="1">
+        <v>1</v>
+      </c>
+      <c r="F248" s="1">
+        <v>0</v>
+      </c>
+      <c r="G248" s="1">
+        <v>4</v>
+      </c>
+      <c r="H248" s="4">
+        <v>46001</v>
+      </c>
+      <c r="I248" s="4">
+        <v>46001</v>
+      </c>
+    </row>
+    <row r="249" spans="8:9">
+      <c r="H249" s="4">
+        <v>46001</v>
+      </c>
+      <c r="I249" s="4">
+        <v>46001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>